<commit_message>
Miscellaneous standardization and fixes throughout the app
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9968C46-848E-4649-AB00-A7BBF9EB6BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AB902F-576A-4147-A16F-FE9BF72BBAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="48440" windowHeight="28280" activeTab="1" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="1080" yWindow="22100" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="945">
   <si>
     <t>Finding_Category_ID</t>
   </si>
@@ -2734,9 +2734,6 @@
   </si>
   <si>
     <t>ID.AM-5</t>
-  </si>
-  <si>
-    <t>Mediun</t>
   </si>
   <si>
     <t>Inconsistent Interpretation of HTTP Requests</t>
@@ -4256,7 +4253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43849457-AD8B-FC4F-883C-916F9AD054DA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4493,7 +4490,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4528,7 +4525,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4563,7 +4560,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4599,7 +4596,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4637,7 +4634,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4709,7 +4706,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4893,7 +4890,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -4929,7 +4926,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5478,9 +5475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE6EBA3-B14F-E947-A615-39B9D02994B2}">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5690,7 +5687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>37</v>
       </c>
@@ -5941,7 +5938,7 @@
         <v>294</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>295</v>
@@ -6055,7 +6052,7 @@
         <v>317</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6128,7 +6125,7 @@
         <v>329</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>330</v>
@@ -8208,7 +8205,7 @@
         <v>676</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="K73" s="10" t="s">
         <v>677</v>
@@ -8244,7 +8241,7 @@
         <v>682</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="K74" s="10" t="s">
         <v>330</v>
@@ -8953,7 +8950,7 @@
         <v>3</v>
       </c>
       <c r="L93" s="15" t="s">
-        <v>800</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="356" x14ac:dyDescent="0.2">
@@ -8967,26 +8964,26 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="E94" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="10" t="s">
         <v>802</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="G94" s="10" t="s">
         <v>803</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>804</v>
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="J94" s="4" t="s">
+      <c r="K94" s="4" t="s">
         <v>806</v>
-      </c>
-      <c r="K94" s="4" t="s">
-        <v>807</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>43</v>
@@ -9003,28 +9000,28 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>808</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="F95" s="10" t="s">
         <v>809</v>
       </c>
-      <c r="F95" s="10" t="s">
+      <c r="G95" s="10" t="s">
         <v>810</v>
       </c>
-      <c r="G95" s="10" t="s">
+      <c r="H95" s="10" t="s">
         <v>811</v>
       </c>
-      <c r="H95" s="10" t="s">
+      <c r="I95" s="4" t="s">
         <v>812</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="J95" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="J95" s="4" t="s">
+      <c r="K95" s="4" t="s">
         <v>814</v>
-      </c>
-      <c r="K95" s="4" t="s">
-        <v>815</v>
       </c>
       <c r="L95" s="15" t="s">
         <v>386</v>
@@ -9041,28 +9038,28 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>816</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="F96" s="11" t="s">
         <v>817</v>
       </c>
-      <c r="F96" s="11" t="s">
+      <c r="G96" s="29" t="s">
         <v>818</v>
       </c>
-      <c r="G96" s="29" t="s">
+      <c r="H96" s="12" t="s">
         <v>819</v>
       </c>
-      <c r="H96" s="12" t="s">
+      <c r="I96" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="I96" s="4" t="s">
+      <c r="J96" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="K96" s="4" t="s">
         <v>822</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>823</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>386</v>
@@ -9079,25 +9076,25 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="E97" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="E97" s="11" t="s">
+      <c r="F97" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="F97" s="11" t="s">
+      <c r="G97" s="43" t="s">
         <v>826</v>
       </c>
-      <c r="G97" s="43" t="s">
+      <c r="H97" s="43" t="s">
+        <v>826</v>
+      </c>
+      <c r="I97" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="H97" s="43" t="s">
-        <v>827</v>
-      </c>
-      <c r="I97" s="4" t="s">
+      <c r="J97" s="4" t="s">
         <v>828</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>829</v>
       </c>
       <c r="K97" s="4">
         <v>3</v>
@@ -9117,19 +9114,19 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="E98" s="10" t="s">
         <v>830</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="F98" s="10" t="s">
         <v>831</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="I98" s="48" t="s">
         <v>832</v>
       </c>
-      <c r="I98" s="48" t="s">
+      <c r="J98" s="48" t="s">
         <v>833</v>
-      </c>
-      <c r="J98" s="48" t="s">
-        <v>834</v>
       </c>
       <c r="K98" s="48" t="s">
         <v>100</v>
@@ -9149,28 +9146,28 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="E99" s="11" t="s">
+      <c r="F99" s="11" t="s">
         <v>836</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="G99" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="G99" s="10" t="s">
+      <c r="H99" s="10" t="s">
         <v>838</v>
       </c>
-      <c r="H99" s="10" t="s">
+      <c r="I99" s="11" t="s">
         <v>839</v>
       </c>
-      <c r="I99" s="11" t="s">
+      <c r="J99" s="11" t="s">
+        <v>944</v>
+      </c>
+      <c r="K99" s="11" t="s">
         <v>840</v>
-      </c>
-      <c r="J99" s="11" t="s">
-        <v>945</v>
-      </c>
-      <c r="K99" s="11" t="s">
-        <v>841</v>
       </c>
       <c r="L99" s="15" t="s">
         <v>386</v>
@@ -9187,28 +9184,28 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="E100" s="11" t="s">
         <v>842</v>
       </c>
-      <c r="E100" s="11" t="s">
+      <c r="F100" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="F100" s="11" t="s">
+      <c r="G100" s="10" t="s">
         <v>844</v>
       </c>
-      <c r="G100" s="10" t="s">
+      <c r="H100" s="11" t="s">
         <v>845</v>
       </c>
-      <c r="H100" s="11" t="s">
+      <c r="I100" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="I100" s="11" t="s">
+      <c r="J100" s="11" t="s">
         <v>847</v>
       </c>
-      <c r="J100" s="11" t="s">
+      <c r="K100" s="11" t="s">
         <v>848</v>
-      </c>
-      <c r="K100" s="11" t="s">
-        <v>849</v>
       </c>
       <c r="L100" s="15" t="s">
         <v>386</v>
@@ -9225,25 +9222,25 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>850</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="F101" s="11" t="s">
         <v>851</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="10" t="s">
         <v>852</v>
       </c>
-      <c r="G101" s="10" t="s">
+      <c r="H101" s="10" t="s">
         <v>853</v>
       </c>
-      <c r="H101" s="10" t="s">
+      <c r="I101" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="I101" s="11" t="s">
+      <c r="J101" s="11" t="s">
         <v>855</v>
-      </c>
-      <c r="J101" s="11" t="s">
-        <v>856</v>
       </c>
       <c r="K101" s="11" t="s">
         <v>515</v>
@@ -9263,25 +9260,25 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="E102" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="E102" s="11" t="s">
+      <c r="F102" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="G102" s="11" t="s">
         <v>859</v>
       </c>
-      <c r="G102" s="11" t="s">
+      <c r="H102" s="11" t="s">
         <v>860</v>
       </c>
-      <c r="H102" s="11" t="s">
+      <c r="I102" s="11" t="s">
         <v>861</v>
       </c>
-      <c r="I102" s="11" t="s">
+      <c r="J102" s="11" t="s">
         <v>862</v>
-      </c>
-      <c r="J102" s="11" t="s">
-        <v>863</v>
       </c>
       <c r="K102" s="11" t="s">
         <v>182</v>
@@ -9301,25 +9298,25 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
+        <v>863</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>864</v>
       </c>
-      <c r="E103" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>865</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="G103" s="10" t="s">
         <v>866</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="H103" s="14" t="s">
         <v>867</v>
       </c>
-      <c r="H103" s="14" t="s">
+      <c r="I103" s="11" t="s">
         <v>868</v>
       </c>
-      <c r="I103" s="11" t="s">
+      <c r="J103" s="11" t="s">
         <v>869</v>
-      </c>
-      <c r="J103" s="11" t="s">
-        <v>870</v>
       </c>
       <c r="K103" s="11" t="s">
         <v>211</v>
@@ -9339,25 +9336,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
+        <v>870</v>
+      </c>
+      <c r="E104" s="11" t="s">
         <v>871</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="F104" s="11" t="s">
         <v>872</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="G104" s="10" t="s">
         <v>873</v>
       </c>
-      <c r="G104" s="10" t="s">
+      <c r="H104" s="11" t="s">
         <v>874</v>
       </c>
-      <c r="H104" s="11" t="s">
+      <c r="I104" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="I104" s="11" t="s">
+      <c r="J104" s="11" t="s">
         <v>876</v>
-      </c>
-      <c r="J104" s="11" t="s">
-        <v>877</v>
       </c>
       <c r="K104" s="11"/>
       <c r="L104" s="15" t="s">
@@ -9375,25 +9372,25 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
+        <v>877</v>
+      </c>
+      <c r="E105" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="F105" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="G105" s="10" t="s">
         <v>880</v>
       </c>
-      <c r="G105" s="10" t="s">
+      <c r="H105" s="10" t="s">
         <v>881</v>
       </c>
-      <c r="H105" s="10" t="s">
+      <c r="I105" s="11" t="s">
         <v>882</v>
       </c>
-      <c r="I105" s="11" t="s">
+      <c r="J105" s="11" t="s">
         <v>883</v>
-      </c>
-      <c r="J105" s="11" t="s">
-        <v>884</v>
       </c>
       <c r="K105" s="11" t="s">
         <v>167</v>
@@ -9413,25 +9410,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
+        <v>884</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>885</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="F106" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="G106" s="10" t="s">
         <v>887</v>
       </c>
-      <c r="G106" s="10" t="s">
+      <c r="H106" s="14" t="s">
         <v>888</v>
       </c>
-      <c r="H106" s="14" t="s">
+      <c r="I106" s="11" t="s">
         <v>889</v>
       </c>
-      <c r="I106" s="11" t="s">
+      <c r="J106" s="11" t="s">
         <v>890</v>
-      </c>
-      <c r="J106" s="11" t="s">
-        <v>891</v>
       </c>
       <c r="K106" s="11" t="s">
         <v>182</v>
@@ -9451,22 +9448,22 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
+        <v>891</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="F107" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="G107" s="10" t="s">
         <v>894</v>
       </c>
-      <c r="G107" s="10" t="s">
+      <c r="H107" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="H107" s="11" t="s">
+      <c r="I107" s="11" t="s">
         <v>896</v>
-      </c>
-      <c r="I107" s="11" t="s">
-        <v>897</v>
       </c>
       <c r="J107" s="11" t="s">
         <v>210</v>
@@ -9489,28 +9486,28 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="F108" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="G108" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="G108" s="10" t="s">
+      <c r="H108" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="H108" s="10" t="s">
+      <c r="I108" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="I108" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="J108" s="11" t="s">
+      <c r="K108" s="11" t="s">
         <v>904</v>
-      </c>
-      <c r="K108" s="11" t="s">
-        <v>905</v>
       </c>
       <c r="L108" s="15" t="s">
         <v>43</v>
@@ -9527,28 +9524,28 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
+        <v>905</v>
+      </c>
+      <c r="E109" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="F109" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="G109" s="12" t="s">
         <v>908</v>
       </c>
-      <c r="G109" s="12" t="s">
+      <c r="H109" s="14" t="s">
+        <v>867</v>
+      </c>
+      <c r="I109" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="H109" s="14" t="s">
-        <v>868</v>
-      </c>
-      <c r="I109" s="11" t="s">
+      <c r="J109" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="J109" s="11" t="s">
+      <c r="K109" s="11" t="s">
         <v>911</v>
-      </c>
-      <c r="K109" s="11" t="s">
-        <v>912</v>
       </c>
       <c r="L109" s="15" t="s">
         <v>386</v>
@@ -9565,25 +9562,25 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
+        <v>912</v>
+      </c>
+      <c r="E110" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="F110" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="G110" s="10" t="s">
         <v>915</v>
       </c>
-      <c r="G110" s="10" t="s">
+      <c r="H110" s="14" t="s">
         <v>916</v>
       </c>
-      <c r="H110" s="14" t="s">
+      <c r="I110" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="I110" s="11" t="s">
+      <c r="J110" s="11" t="s">
         <v>918</v>
-      </c>
-      <c r="J110" s="11" t="s">
-        <v>919</v>
       </c>
       <c r="K110" s="11" t="s">
         <v>218</v>
@@ -9603,22 +9600,22 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>919</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>920</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="F111" s="11" t="s">
         <v>921</v>
       </c>
-      <c r="F111" s="11" t="s">
+      <c r="G111" s="13" t="s">
         <v>922</v>
       </c>
-      <c r="G111" s="13" t="s">
+      <c r="H111" s="11" t="s">
         <v>923</v>
       </c>
-      <c r="H111" s="11" t="s">
+      <c r="I111" s="11" t="s">
         <v>924</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>925</v>
       </c>
       <c r="J111" s="11" t="s">
         <v>210</v>
@@ -9641,25 +9638,25 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>925</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="F112" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="G112" s="11" t="s">
         <v>928</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="H112" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="H112" s="11" t="s">
+      <c r="I112" s="11" t="s">
         <v>930</v>
       </c>
-      <c r="I112" s="11" t="s">
+      <c r="J112" s="11" t="s">
         <v>931</v>
-      </c>
-      <c r="J112" s="11" t="s">
-        <v>932</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>67</v>
@@ -9779,21 +9776,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -9925,24 +9907,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9958,4 +9938,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Miscellaneous bug fixes and addition of widescreen out-brief generation
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AB902F-576A-4147-A16F-FE9BF72BBAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ED047B-AF1A-BB4C-BDA9-862528ACE9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="22100" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="21360" yWindow="2620" windowWidth="34820" windowHeight="19640" activeTab="3" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="959">
   <si>
     <t>Finding_Category_ID</t>
   </si>
@@ -1825,9 +1825,6 @@
     <t>AU-13, AC-1, AC-2, AC-3, AC-4, AC-5, AC-6, AC-14, AC-16, AC-24, MP-2, MP-3, MP-4, MP-5, MP-6, MP-7, MP-8, PE-19, PS-6, SC-7, SI-4, SC-28</t>
   </si>
   <si>
-    <t>PR.DS- 1,  PR.DS-5, PR.AC-4</t>
-  </si>
-  <si>
     <t>Unauthenticated File Share or Server Access</t>
   </si>
   <si>
@@ -3186,6 +3183,51 @@
   </si>
   <si>
     <t>PR.PT-3, PR.AC-3, PR.AC-7</t>
+  </si>
+  <si>
+    <t>Insecure Storage of Sensitive Data</t>
+  </si>
+  <si>
+    <t>https://cwe.mitre.org/data/definitions/312.html</t>
+  </si>
+  <si>
+    <t>https://cwe.mitre.org/data/definitions/256.html</t>
+  </si>
+  <si>
+    <t>Storing personally identifiable information (PII), protected health information (PHI), classified information, and/or other sensitive data in cleartext, especially in a location that can be accessed by unauthorized users, is a serious security risk. This poses a risk to the privacy and security of the affected entities.</t>
+  </si>
+  <si>
+    <t>AC-1, AC-2, AC-3, AC-4, AC-6, AC-21, AC-22, AT-1, AT-2, AT-3, AT-6, AU-1, AU-3, AU-6, AU-7, AU-9, AU-13, CA-7, CA-8, IA-1, IA-2, IA-5, MA-2, MA-3, MA-6, MP-1, MP-2, MP-4, MP-6, PM-5, PM-14, PM-31, RA-5, SC-4, SC-7, SC-28</t>
+  </si>
+  <si>
+    <t>AC-1, AC-2, AC-3, AC-4, AC-5, AC-6, AC-17, AC-20, AC-21, AC-22, AT-1, AT-2, AT-3, AT-6, AU-1, AU-3, AU-6, AU-7, AU-9, AU-13, CA-3, CA-7, CA-8, CA-9, IA-1, IA-2, IA-5, IR-9, MA-2, MA-3, MA-6, MP-1, MP-2, MP-4, MP-6, PL-8, PM-5, PM-14, PM-31, PT-1, PT-2, PT-3, PT-4, PT-5, PT-6, PT-7, PT-8, RA-5, SC-4, SC-7, SC-28</t>
+  </si>
+  <si>
+    <t>PR.DS-1,  PR.DS-5, PR.AC-4</t>
+  </si>
+  <si>
+    <t>ID.AM-1, ID.AM-2, ID.AM-5, ID.AM-6, ID.GV-3, PR.AC-1, PR.AC-2, PR.AC-3, PR.AC-4, PR.AC-5, PR.AC-6, PR.AC-7, PR.AT-1, PR.AT-2, PR.AT-3, PR.AT-4, PR.AT-5, PR.DS-1, PR.DS-3, PR.DS-5, PR.IP-6, PR.IP-7, PR.IP-11, PR.MA-2, PR.PT-1, DE.AE-1, DE.AE-2, DE.AE-3, DE.DP-5</t>
+  </si>
+  <si>
+    <t>ID.AM-1, ID.AM-2, ID.AM-5, PR.AC-1, PR.AC-2, PR.AC-3, PR.AC-4, PR.AC-5, PR.AC-6, PR.AC-7, PR.AT-1, PR.AT-2, PR.AT-3, PR.AT-4, PR.AT-5, PR.DS-1, PR.DS-3, PR.DS-5, PR.IP-7, PR.IP-11, PR.PT-1, DE.AE-1, DE.AE-2, DE.AE-3, DE.DP-5</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 6, 7, 8, 9, 14</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 14, 16</t>
+  </si>
+  <si>
+    <t>Insecure Storage of Credentials</t>
+  </si>
+  <si>
+    <t>Storing credentials in cleartext, especially in a location that can be accessed by unauthorized users, is a serious security risk. An adversary with access to files containing cleartext credentials could authenticate to corresponding applications or systems under the guise of a legitimate user. Accountability is lost because logging would show valid user accounts accessing the applications or systems.</t>
+  </si>
+  <si>
+    <t>Implement a review process for files and systems to look for cleartext account credentials. When credentials are found, remove or encrypt the data and change potentially compromised credentials to maintain security. Conduct periodic scans of systems using automated tools to determine whether passwords are present on the system in cleartext. User awareness training outlining best practices for credential storage can be effective, but does not guarantee secure storage.</t>
+  </si>
+  <si>
+    <t>Implement a review process for files and systems to identify insecure handling of PII, PHI, and other sensitive information. Properly secure or remove the information. Conduct periodic scans of systems using automated tools to determine whether sensitive data is present on the system in cleartext. User awareness training outlining best practices for sensitive information storage can be effective, but does not guarantee secure storage.</t>
   </si>
 </sst>
 </file>
@@ -4405,8 +4447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228C06AC-317E-5044-B7A5-92100984FDF0}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -4490,7 +4532,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4525,7 +4567,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4560,7 +4602,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4596,7 +4638,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4634,7 +4676,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4706,7 +4748,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4890,7 +4932,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -4926,7 +4968,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5473,11 +5515,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE6EBA3-B14F-E947-A615-39B9D02994B2}">
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L94" sqref="L94"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5490,7 +5532,7 @@
     <col min="6" max="6" width="40" style="10" customWidth="1"/>
     <col min="7" max="8" width="19.1640625" style="10" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" style="10" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.1640625" style="15" customWidth="1"/>
     <col min="13" max="16383" width="11" style="15"/>
@@ -5687,7 +5729,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>37</v>
       </c>
@@ -5938,7 +5980,7 @@
         <v>294</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>295</v>
@@ -6023,7 +6065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>50</v>
       </c>
@@ -6052,7 +6094,7 @@
         <v>317</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6125,7 +6167,7 @@
         <v>329</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>330</v>
@@ -7246,7 +7288,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>120</v>
       </c>
@@ -7257,32 +7299,32 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>525</v>
+        <v>955</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>956</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>957</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>526</v>
+        <v>946</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
-        <v>527</v>
+        <v>948</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>528</v>
+        <v>952</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>487</v>
+        <v>953</v>
       </c>
       <c r="L48" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>120</v>
       </c>
@@ -7293,32 +7335,32 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>530</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>531</v>
+        <v>944</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>947</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>958</v>
       </c>
       <c r="G49" s="29" t="s">
-        <v>532</v>
+        <v>945</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
-        <v>172</v>
+        <v>949</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>533</v>
+        <v>951</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>534</v>
+        <v>954</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>120</v>
       </c>
@@ -7329,108 +7371,104 @@
         <v>49</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="4" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>540</v>
+        <v>950</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>541</v>
+        <v>487</v>
       </c>
       <c r="L50" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B51" s="10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51" s="5">
         <v>50</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="G51" s="43" t="s">
-        <v>545</v>
-      </c>
-      <c r="H51" s="43" t="s">
-        <v>545</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>530</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>531</v>
+      </c>
+      <c r="H51" s="29"/>
       <c r="I51" s="4" t="s">
-        <v>546</v>
+        <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="238" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B52" s="10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52" s="5">
         <v>51</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>550</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>551</v>
-      </c>
-      <c r="G52" s="43" t="s">
-        <v>545</v>
-      </c>
-      <c r="H52" s="43" t="s">
-        <v>545</v>
-      </c>
+        <v>534</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>537</v>
+      </c>
+      <c r="H52" s="29"/>
       <c r="I52" s="4" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="L52" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="238" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
         <v>126</v>
       </c>
@@ -7441,34 +7479,34 @@
         <v>52</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="G53" s="43" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="H53" s="43" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="I53" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="J53" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>548</v>
       </c>
       <c r="L53" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>126</v>
       </c>
@@ -7479,34 +7517,34 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>557</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>560</v>
+        <v>549</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="G54" s="43" t="s">
+        <v>544</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>544</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>561</v>
+        <v>545</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>364</v>
+        <v>547</v>
       </c>
       <c r="L54" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>126</v>
       </c>
@@ -7517,106 +7555,106 @@
         <v>54</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>564</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
+        <v>552</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="G55" s="43" t="s">
+        <v>554</v>
+      </c>
+      <c r="H55" s="43" t="s">
+        <v>554</v>
+      </c>
       <c r="I55" s="4" t="s">
-        <v>561</v>
+        <v>545</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>364</v>
+        <v>547</v>
       </c>
       <c r="L55" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B56" s="10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56" s="5">
         <v>55</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>567</v>
+        <v>555</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>556</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>569</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>570</v>
+        <v>557</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>559</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="L56" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="L56" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B57" s="10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="5">
         <v>56</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>575</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>576</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>577</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>578</v>
-      </c>
+        <v>563</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
-        <v>579</v>
+        <v>560</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>580</v>
+        <v>561</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>248</v>
+        <v>364</v>
       </c>
       <c r="L57" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
         <v>133</v>
       </c>
@@ -7627,35 +7665,35 @@
         <v>57</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>582</v>
+        <v>566</v>
       </c>
       <c r="F58" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="G58" s="14" t="s">
-        <v>583</v>
-      </c>
       <c r="H58" s="14" t="s">
-        <v>584</v>
+        <v>569</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>585</v>
+        <v>570</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>587</v>
+        <v>572</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="20" t="s">
         <v>133</v>
       </c>
       <c r="B59" s="10">
@@ -7665,34 +7703,34 @@
         <v>58</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>589</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>590</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>591</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>592</v>
+        <v>573</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>577</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>593</v>
+        <v>578</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="L59" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+      <c r="L59" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
         <v>133</v>
       </c>
@@ -7703,35 +7741,35 @@
         <v>59</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>596</v>
+        <v>580</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>597</v>
+        <v>581</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>598</v>
+        <v>567</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>600</v>
+        <v>583</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>601</v>
+        <v>584</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A61" s="20" t="s">
+    <row r="61" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B61" s="10">
@@ -7741,34 +7779,34 @@
         <v>60</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>605</v>
+        <v>588</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>606</v>
+        <v>589</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>590</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>607</v>
+        <v>591</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>608</v>
+        <v>592</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>609</v>
+        <v>593</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>610</v>
+        <v>594</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
         <v>133</v>
       </c>
@@ -7779,32 +7817,34 @@
         <v>61</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>611</v>
+        <v>595</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>612</v>
+        <v>596</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>568</v>
+        <v>597</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>613</v>
-      </c>
-      <c r="H62" s="12"/>
+        <v>598</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>599</v>
+      </c>
       <c r="I62" s="4" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>248</v>
+        <v>602</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
         <v>133</v>
       </c>
@@ -7815,34 +7855,34 @@
         <v>62</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>618</v>
+        <v>567</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>619</v>
-      </c>
-      <c r="H63" s="12" t="s">
-        <v>620</v>
+        <v>605</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>606</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>133</v>
       </c>
@@ -7853,34 +7893,32 @@
         <v>63</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>618</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>626</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>627</v>
-      </c>
+        <v>567</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>623</v>
+        <v>248</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
         <v>133</v>
       </c>
@@ -7891,34 +7929,34 @@
         <v>64</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>633</v>
+        <v>618</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>619</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>609</v>
+        <v>621</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>610</v>
+        <v>622</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
         <v>133</v>
       </c>
@@ -7929,106 +7967,110 @@
         <v>65</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>568</v>
+        <v>617</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>640</v>
-      </c>
-      <c r="K66" s="4">
-        <v>7</v>
+        <v>621</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>622</v>
       </c>
       <c r="L66" s="10" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="255" x14ac:dyDescent="0.2">
-      <c r="A67" s="39" t="s">
-        <v>139</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="B67" s="10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C67" s="5">
         <v>66</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>645</v>
-      </c>
-      <c r="H67" s="12"/>
+        <v>630</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>632</v>
+      </c>
       <c r="I67" s="4" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="K67" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="L67" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="L67" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A68" s="39" t="s">
-        <v>139</v>
+    <row r="68" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="A68" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="B68" s="10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C68" s="5">
         <v>67</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>649</v>
+        <v>567</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>650</v>
-      </c>
-      <c r="H68" s="12"/>
+        <v>636</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>637</v>
+      </c>
       <c r="I68" s="4" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="K68" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="L68" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="K68" s="4">
+        <v>7</v>
+      </c>
+      <c r="L68" s="10" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
         <v>139</v>
       </c>
@@ -8039,20 +8081,20 @@
         <v>68</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="G69" s="14" t="s">
-        <v>654</v>
+        <v>643</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>145</v>
@@ -8064,158 +8106,156 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="136" x14ac:dyDescent="0.2">
-      <c r="A70" s="27" t="s">
-        <v>146</v>
+    <row r="70" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="A70" s="39" t="s">
+        <v>139</v>
       </c>
       <c r="B70" s="10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" s="5">
         <v>69</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>656</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>657</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>658</v>
-      </c>
-      <c r="H70" s="43" t="s">
-        <v>658</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>659</v>
-      </c>
-      <c r="J70" s="11" t="s">
-        <v>660</v>
-      </c>
-      <c r="K70" s="11">
-        <v>16</v>
+        <v>646</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="H70" s="12"/>
+      <c r="I70" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K70" s="47" t="s">
+        <v>138</v>
       </c>
       <c r="L70" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="221" x14ac:dyDescent="0.2">
-      <c r="A71" s="27" t="s">
-        <v>146</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="A71" s="39" t="s">
+        <v>139</v>
       </c>
       <c r="B71" s="10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" s="5">
         <v>70</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>661</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>662</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>663</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>664</v>
-      </c>
-      <c r="H71" s="43" t="s">
-        <v>664</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>659</v>
-      </c>
-      <c r="J71" s="11" t="s">
-        <v>660</v>
-      </c>
-      <c r="K71" s="11">
-        <v>16</v>
+        <v>650</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>653</v>
+      </c>
+      <c r="H71" s="12"/>
+      <c r="I71" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K71" s="47" t="s">
+        <v>138</v>
       </c>
       <c r="L71" s="15" t="s">
-        <v>386</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="136" x14ac:dyDescent="0.2">
-      <c r="A72" s="22" t="s">
-        <v>153</v>
+      <c r="A72" s="27" t="s">
+        <v>146</v>
       </c>
       <c r="B72" s="10">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C72" s="5">
         <v>71</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>668</v>
-      </c>
-      <c r="H72" s="11"/>
+        <v>657</v>
+      </c>
+      <c r="H72" s="43" t="s">
+        <v>657</v>
+      </c>
       <c r="I72" s="11" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>670</v>
-      </c>
-      <c r="K72" s="11" t="s">
-        <v>268</v>
+        <v>659</v>
+      </c>
+      <c r="K72" s="11">
+        <v>16</v>
       </c>
       <c r="L72" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B73" s="10">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C73" s="5">
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>672</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>673</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>674</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>675</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>676</v>
-      </c>
-      <c r="J73" s="10" t="s">
-        <v>942</v>
-      </c>
-      <c r="K73" s="10" t="s">
-        <v>677</v>
+        <v>661</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="H73" s="43" t="s">
+        <v>663</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>658</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>659</v>
+      </c>
+      <c r="K73" s="11">
+        <v>16</v>
       </c>
       <c r="L73" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A74" s="27" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="A74" s="22" t="s">
         <v>153</v>
       </c>
       <c r="B74" s="10">
@@ -8225,33 +8265,33 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>679</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>680</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>681</v>
-      </c>
-      <c r="H74" s="14"/>
-      <c r="I74" s="10" t="s">
-        <v>682</v>
-      </c>
-      <c r="J74" s="10" t="s">
-        <v>943</v>
-      </c>
-      <c r="K74" s="10" t="s">
-        <v>330</v>
+        <v>665</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="K74" s="11" t="s">
+        <v>268</v>
       </c>
       <c r="L74" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A75" s="22" t="s">
+    <row r="75" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="A75" s="27" t="s">
         <v>153</v>
       </c>
       <c r="B75" s="10">
@@ -8261,35 +8301,35 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>684</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>686</v>
-      </c>
-      <c r="H75" s="43" t="s">
-        <v>686</v>
-      </c>
-      <c r="I75" s="11" t="s">
-        <v>687</v>
-      </c>
-      <c r="J75" s="11" t="s">
-        <v>688</v>
-      </c>
-      <c r="K75" s="11" t="s">
-        <v>364</v>
+        <v>671</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>674</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>941</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>676</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="323" x14ac:dyDescent="0.2">
-      <c r="A76" s="22" t="s">
+    <row r="76" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A76" s="27" t="s">
         <v>153</v>
       </c>
       <c r="B76" s="10">
@@ -8299,110 +8339,108 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>689</v>
+        <v>677</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="G76" s="11"/>
-      <c r="H76" s="43" t="s">
-        <v>692</v>
-      </c>
-      <c r="I76" s="11" t="s">
-        <v>693</v>
-      </c>
-      <c r="J76" s="11" t="s">
-        <v>694</v>
-      </c>
-      <c r="K76" s="11" t="s">
-        <v>73</v>
+        <v>678</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="H76" s="14"/>
+      <c r="I76" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="J76" s="10" t="s">
+        <v>942</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>330</v>
       </c>
       <c r="L76" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
-        <v>695</v>
+        <v>153</v>
       </c>
       <c r="B77" s="10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C77" s="5">
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="H77" s="43" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>701</v>
-      </c>
-      <c r="K77" s="11">
-        <v>16</v>
+        <v>687</v>
+      </c>
+      <c r="K77" s="11" t="s">
+        <v>364</v>
       </c>
       <c r="L77" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="404" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="323" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
-        <v>695</v>
+        <v>153</v>
       </c>
       <c r="B78" s="10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C78" s="5">
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>704</v>
-      </c>
-      <c r="G78" s="43" t="s">
-        <v>705</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>172</v>
+        <v>692</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K78" s="15" t="s">
-        <v>706</v>
+        <v>693</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="L78" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8411,36 +8449,36 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>707</v>
+        <v>695</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>708</v>
+        <v>696</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>709</v>
-      </c>
-      <c r="G79" s="43" t="s">
-        <v>710</v>
+        <v>697</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>698</v>
       </c>
       <c r="H79" s="43" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="K79" s="15" t="s">
-        <v>182</v>
+        <v>700</v>
+      </c>
+      <c r="K79" s="11">
+        <v>16</v>
       </c>
       <c r="L79" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8449,36 +8487,36 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>714</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>715</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>716</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>717</v>
-      </c>
-      <c r="H80" s="14" t="s">
-        <v>718</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="J80" s="10" t="s">
-        <v>720</v>
+        <v>701</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="G80" s="43" t="s">
+        <v>704</v>
+      </c>
+      <c r="H80" s="43" t="s">
+        <v>704</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J80" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>515</v>
+        <v>705</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8487,34 +8525,36 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>721</v>
+        <v>706</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>722</v>
-      </c>
-      <c r="F81" s="10" t="s">
-        <v>723</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>724</v>
-      </c>
-      <c r="H81" s="12"/>
-      <c r="I81" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>708</v>
+      </c>
+      <c r="G81" s="43" t="s">
+        <v>709</v>
+      </c>
+      <c r="H81" s="43" t="s">
+        <v>710</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="J81" s="11" t="s">
         <v>712</v>
       </c>
-      <c r="J81" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="K81" s="4" t="s">
+      <c r="K81" s="15" t="s">
         <v>182</v>
       </c>
       <c r="L81" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8523,106 +8563,106 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>725</v>
+        <v>713</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>726</v>
+        <v>714</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>727</v>
+        <v>715</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>728</v>
-      </c>
-      <c r="H82" s="12"/>
+        <v>716</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>717</v>
+      </c>
       <c r="I82" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="J82" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="K82" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="J82" s="10" t="s">
+        <v>719</v>
+      </c>
+      <c r="K82" s="15" t="s">
         <v>515</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="102" x14ac:dyDescent="0.2">
-      <c r="A83" s="23" t="s">
-        <v>168</v>
+    <row r="83" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A83" s="22" t="s">
+        <v>694</v>
       </c>
       <c r="B83" s="10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C83" s="5">
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>730</v>
-      </c>
-      <c r="E83" s="46" t="s">
-        <v>731</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>732</v>
-      </c>
-      <c r="G83" s="43" t="s">
-        <v>733</v>
-      </c>
-      <c r="H83" s="43" t="s">
-        <v>733</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>721</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>722</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
-        <v>734</v>
+        <v>711</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>735</v>
+        <v>712</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>49</v>
+        <v>182</v>
       </c>
       <c r="L83" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="170" x14ac:dyDescent="0.2">
-      <c r="A84" s="23" t="s">
-        <v>168</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A84" s="22" t="s">
+        <v>694</v>
       </c>
       <c r="B84" s="10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C84" s="5">
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>736</v>
-      </c>
-      <c r="E84" s="46" t="s">
-        <v>737</v>
-      </c>
-      <c r="F84" s="46" t="s">
-        <v>738</v>
+        <v>724</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="F84" s="10" t="s">
+        <v>726</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>739</v>
+        <v>727</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>740</v>
+        <v>728</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>741</v>
+        <v>522</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>73</v>
+        <v>515</v>
       </c>
       <c r="L84" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" s="23" t="s">
         <v>168</v>
       </c>
@@ -8633,34 +8673,34 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>742</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>743</v>
-      </c>
-      <c r="F85" s="46" t="s">
-        <v>744</v>
-      </c>
-      <c r="G85" s="29" t="s">
-        <v>745</v>
-      </c>
-      <c r="H85" s="12" t="s">
-        <v>746</v>
+        <v>729</v>
+      </c>
+      <c r="E85" s="46" t="s">
+        <v>730</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="G85" s="43" t="s">
+        <v>732</v>
+      </c>
+      <c r="H85" s="43" t="s">
+        <v>732</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="L85" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
         <v>168</v>
       </c>
@@ -8671,108 +8711,108 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>747</v>
+        <v>735</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>748</v>
+        <v>736</v>
       </c>
       <c r="F86" s="46" t="s">
-        <v>749</v>
-      </c>
-      <c r="G86" s="43" t="s">
-        <v>750</v>
-      </c>
-      <c r="H86" s="43" t="s">
-        <v>750</v>
-      </c>
+        <v>737</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
-        <v>751</v>
+        <v>739</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>752</v>
+        <v>740</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>753</v>
+        <v>73</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="187" x14ac:dyDescent="0.2">
-      <c r="A87" s="22" t="s">
-        <v>175</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="A87" s="23" t="s">
+        <v>168</v>
       </c>
       <c r="B87" s="10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C87" s="5">
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>754</v>
-      </c>
-      <c r="E87" s="46" t="s">
-        <v>755</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>756</v>
+        <v>741</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>742</v>
+      </c>
+      <c r="F87" s="46" t="s">
+        <v>743</v>
       </c>
       <c r="G87" s="29" t="s">
-        <v>757</v>
+        <v>744</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>759</v>
+        <v>739</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>211</v>
+        <v>73</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="255" x14ac:dyDescent="0.2">
-      <c r="A88" s="22" t="s">
-        <v>175</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="A88" s="23" t="s">
+        <v>168</v>
       </c>
       <c r="B88" s="10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C88" s="5">
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>761</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>762</v>
-      </c>
-      <c r="F88" s="11" t="s">
-        <v>763</v>
-      </c>
-      <c r="G88" s="16" t="s">
-        <v>764</v>
-      </c>
-      <c r="H88" s="12"/>
+        <v>746</v>
+      </c>
+      <c r="E88" s="46" t="s">
+        <v>747</v>
+      </c>
+      <c r="F88" s="46" t="s">
+        <v>748</v>
+      </c>
+      <c r="G88" s="43" t="s">
+        <v>749</v>
+      </c>
+      <c r="H88" s="43" t="s">
+        <v>749</v>
+      </c>
       <c r="I88" s="4" t="s">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
       <c r="K88" s="4" t="s">
-        <v>767</v>
+        <v>752</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A89" s="22" t="s">
         <v>175</v>
       </c>
@@ -8783,32 +8823,34 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>768</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>769</v>
+        <v>753</v>
+      </c>
+      <c r="E89" s="46" t="s">
+        <v>754</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="G89" s="29" t="s">
-        <v>771</v>
-      </c>
-      <c r="H89" s="12"/>
+        <v>756</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>757</v>
+      </c>
       <c r="I89" s="4" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>767</v>
+        <v>211</v>
       </c>
       <c r="L89" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A90" s="22" t="s">
         <v>175</v>
       </c>
@@ -8819,105 +8861,103 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>773</v>
-      </c>
-      <c r="F90" s="10" t="s">
-        <v>774</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>775</v>
-      </c>
+        <v>761</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>762</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>763</v>
+      </c>
+      <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
-        <v>776</v>
+        <v>764</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
       <c r="K90" s="4" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B91" s="10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C91" s="5">
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>779</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>780</v>
-      </c>
-      <c r="F91" s="10" t="s">
-        <v>781</v>
-      </c>
-      <c r="G91" s="14" t="s">
-        <v>782</v>
-      </c>
-      <c r="H91" s="14"/>
+        <v>767</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="G91" s="29" t="s">
+        <v>770</v>
+      </c>
+      <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
-        <v>783</v>
+        <v>764</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>784</v>
+        <v>765</v>
       </c>
       <c r="K91" s="4" t="s">
-        <v>785</v>
+        <v>766</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A92" s="22" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B92" s="10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92" s="5">
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>786</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>787</v>
+        <v>771</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>772</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>788</v>
-      </c>
-      <c r="G92" s="12" t="s">
-        <v>789</v>
-      </c>
-      <c r="H92" s="14" t="s">
-        <v>790</v>
+        <v>773</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>774</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>791</v>
+        <v>775</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="K92" s="48" t="s">
-        <v>793</v>
+        <v>776</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>777</v>
       </c>
       <c r="L92" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A93" s="22" t="s">
         <v>183</v>
       </c>
@@ -8928,32 +8968,32 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>794</v>
+        <v>778</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>795</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>796</v>
-      </c>
-      <c r="G93" s="29" t="s">
-        <v>797</v>
-      </c>
-      <c r="H93" s="12"/>
+        <v>779</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="G93" s="14" t="s">
+        <v>781</v>
+      </c>
+      <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
-        <v>798</v>
+        <v>782</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>799</v>
-      </c>
-      <c r="K93" s="4">
-        <v>3</v>
+        <v>783</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>784</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="272" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
         <v>183</v>
       </c>
@@ -8964,32 +9004,34 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>800</v>
+        <v>785</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>801</v>
+        <v>786</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>802</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>803</v>
-      </c>
-      <c r="H94" s="12"/>
+        <v>787</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>788</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>789</v>
+      </c>
       <c r="I94" s="4" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>805</v>
-      </c>
-      <c r="K94" s="4" t="s">
-        <v>806</v>
+        <v>791</v>
+      </c>
+      <c r="K94" s="48" t="s">
+        <v>792</v>
       </c>
       <c r="L94" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>183</v>
       </c>
@@ -9000,34 +9042,32 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>807</v>
+        <v>793</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>808</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>809</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>810</v>
-      </c>
-      <c r="H95" s="10" t="s">
-        <v>811</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>795</v>
+      </c>
+      <c r="G95" s="29" t="s">
+        <v>796</v>
+      </c>
+      <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
-        <v>812</v>
+        <v>797</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>813</v>
-      </c>
-      <c r="K95" s="4" t="s">
-        <v>814</v>
+        <v>798</v>
+      </c>
+      <c r="K95" s="4">
+        <v>3</v>
       </c>
       <c r="L95" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" ht="388" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>183</v>
       </c>
@@ -9038,34 +9078,32 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>815</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>816</v>
-      </c>
-      <c r="F96" s="11" t="s">
-        <v>817</v>
-      </c>
-      <c r="G96" s="29" t="s">
-        <v>818</v>
-      </c>
-      <c r="H96" s="12" t="s">
-        <v>819</v>
-      </c>
+        <v>799</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>802</v>
+      </c>
+      <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
-        <v>820</v>
+        <v>803</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>821</v>
+        <v>804</v>
       </c>
       <c r="K96" s="4" t="s">
-        <v>822</v>
+        <v>805</v>
       </c>
       <c r="L96" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
         <v>183</v>
       </c>
@@ -9076,34 +9114,34 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>823</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>824</v>
-      </c>
-      <c r="F97" s="11" t="s">
-        <v>825</v>
-      </c>
-      <c r="G97" s="43" t="s">
-        <v>826</v>
-      </c>
-      <c r="H97" s="43" t="s">
-        <v>826</v>
+        <v>806</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>810</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>827</v>
+        <v>811</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>828</v>
-      </c>
-      <c r="K97" s="4">
-        <v>3</v>
+        <v>812</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>813</v>
       </c>
       <c r="L97" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="388" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
         <v>183</v>
       </c>
@@ -9114,104 +9152,104 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>829</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>830</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>831</v>
-      </c>
-      <c r="I98" s="48" t="s">
-        <v>832</v>
-      </c>
-      <c r="J98" s="48" t="s">
-        <v>833</v>
-      </c>
-      <c r="K98" s="48" t="s">
-        <v>100</v>
+        <v>814</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>815</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>816</v>
+      </c>
+      <c r="G98" s="29" t="s">
+        <v>817</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>818</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>821</v>
       </c>
       <c r="L98" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" ht="255" x14ac:dyDescent="0.2">
-      <c r="A99" s="8" t="s">
-        <v>190</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="A99" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="B99" s="10">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C99" s="5">
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>834</v>
+        <v>822</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>835</v>
+        <v>823</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>836</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>837</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="I99" s="11" t="s">
-        <v>839</v>
-      </c>
-      <c r="J99" s="11" t="s">
-        <v>944</v>
-      </c>
-      <c r="K99" s="11" t="s">
-        <v>840</v>
+        <v>824</v>
+      </c>
+      <c r="G99" s="43" t="s">
+        <v>825</v>
+      </c>
+      <c r="H99" s="43" t="s">
+        <v>825</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="K99" s="4">
+        <v>3</v>
       </c>
       <c r="L99" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" ht="187" x14ac:dyDescent="0.2">
-      <c r="A100" s="8" t="s">
-        <v>190</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="A100" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="B100" s="10">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C100" s="5">
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>841</v>
-      </c>
-      <c r="E100" s="11" t="s">
-        <v>842</v>
-      </c>
-      <c r="F100" s="11" t="s">
-        <v>843</v>
-      </c>
-      <c r="G100" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="H100" s="11" t="s">
-        <v>845</v>
-      </c>
-      <c r="I100" s="11" t="s">
-        <v>846</v>
-      </c>
-      <c r="J100" s="11" t="s">
-        <v>847</v>
-      </c>
-      <c r="K100" s="11" t="s">
-        <v>848</v>
+        <v>828</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="I100" s="48" t="s">
+        <v>831</v>
+      </c>
+      <c r="J100" s="48" t="s">
+        <v>832</v>
+      </c>
+      <c r="K100" s="48" t="s">
+        <v>100</v>
       </c>
       <c r="L100" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
         <v>190</v>
       </c>
@@ -9222,34 +9260,34 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>849</v>
+        <v>833</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>850</v>
+        <v>834</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>851</v>
+        <v>835</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>852</v>
+        <v>836</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>853</v>
+        <v>837</v>
       </c>
       <c r="I101" s="11" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="J101" s="11" t="s">
-        <v>855</v>
+        <v>943</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>515</v>
+        <v>839</v>
       </c>
       <c r="L101" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>190</v>
       </c>
@@ -9260,34 +9298,34 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>856</v>
+        <v>840</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>857</v>
+        <v>841</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>858</v>
-      </c>
-      <c r="G102" s="11" t="s">
-        <v>859</v>
+        <v>842</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>843</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>860</v>
+        <v>844</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>861</v>
+        <v>845</v>
       </c>
       <c r="J102" s="11" t="s">
-        <v>862</v>
+        <v>846</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>182</v>
+        <v>847</v>
       </c>
       <c r="L102" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>190</v>
       </c>
@@ -9298,34 +9336,34 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>866</v>
-      </c>
-      <c r="H103" s="14" t="s">
-        <v>867</v>
+        <v>851</v>
+      </c>
+      <c r="H103" s="10" t="s">
+        <v>852</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="J103" s="11" t="s">
-        <v>869</v>
+        <v>854</v>
       </c>
       <c r="K103" s="11" t="s">
-        <v>211</v>
+        <v>515</v>
       </c>
       <c r="L103" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>190</v>
       </c>
@@ -9336,146 +9374,146 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>870</v>
+        <v>855</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>871</v>
+        <v>856</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>872</v>
-      </c>
-      <c r="G104" s="10" t="s">
-        <v>873</v>
+        <v>857</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>858</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>874</v>
+        <v>859</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>875</v>
+        <v>860</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>876</v>
-      </c>
-      <c r="K104" s="11"/>
+        <v>861</v>
+      </c>
+      <c r="K104" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="L104" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B105" s="10">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C105" s="5">
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>877</v>
+        <v>862</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>878</v>
+        <v>863</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>879</v>
+        <v>864</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>880</v>
-      </c>
-      <c r="H105" s="10" t="s">
-        <v>881</v>
+        <v>865</v>
+      </c>
+      <c r="H105" s="14" t="s">
+        <v>866</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>882</v>
+        <v>867</v>
       </c>
       <c r="J105" s="11" t="s">
-        <v>883</v>
+        <v>868</v>
       </c>
       <c r="K105" s="11" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="L105" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B106" s="10">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C106" s="5">
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>884</v>
+        <v>869</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>885</v>
+        <v>870</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>886</v>
+        <v>871</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>887</v>
-      </c>
-      <c r="H106" s="14" t="s">
-        <v>888</v>
+        <v>872</v>
+      </c>
+      <c r="H106" s="11" t="s">
+        <v>873</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>889</v>
+        <v>874</v>
       </c>
       <c r="J106" s="11" t="s">
-        <v>890</v>
-      </c>
-      <c r="K106" s="11" t="s">
-        <v>182</v>
-      </c>
+        <v>875</v>
+      </c>
+      <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B107" s="10">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C107" s="5">
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>891</v>
+        <v>876</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>892</v>
+        <v>877</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>893</v>
+        <v>878</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>894</v>
-      </c>
-      <c r="H107" s="11" t="s">
-        <v>895</v>
+        <v>879</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>880</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>896</v>
+        <v>881</v>
       </c>
       <c r="J107" s="11" t="s">
-        <v>210</v>
+        <v>882</v>
       </c>
       <c r="K107" s="11" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="L107" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
         <v>205</v>
       </c>
@@ -9486,110 +9524,110 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>897</v>
+        <v>883</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>898</v>
+        <v>884</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>899</v>
+        <v>885</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>900</v>
-      </c>
-      <c r="H108" s="10" t="s">
-        <v>901</v>
+        <v>886</v>
+      </c>
+      <c r="H108" s="14" t="s">
+        <v>887</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>902</v>
+        <v>888</v>
       </c>
       <c r="J108" s="11" t="s">
-        <v>903</v>
+        <v>889</v>
       </c>
       <c r="K108" s="11" t="s">
-        <v>904</v>
+        <v>182</v>
       </c>
       <c r="L108" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B109" s="10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C109" s="5">
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>905</v>
+        <v>890</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>906</v>
+        <v>891</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>907</v>
-      </c>
-      <c r="G109" s="12" t="s">
-        <v>908</v>
-      </c>
-      <c r="H109" s="14" t="s">
-        <v>867</v>
+        <v>892</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>893</v>
+      </c>
+      <c r="H109" s="11" t="s">
+        <v>894</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>909</v>
+        <v>895</v>
       </c>
       <c r="J109" s="11" t="s">
-        <v>910</v>
+        <v>210</v>
       </c>
       <c r="K109" s="11" t="s">
-        <v>911</v>
+        <v>211</v>
       </c>
       <c r="L109" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B110" s="10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C110" s="5">
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>912</v>
+        <v>896</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>913</v>
+        <v>897</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>914</v>
+        <v>898</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>915</v>
-      </c>
-      <c r="H110" s="14" t="s">
-        <v>916</v>
+        <v>899</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>900</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>917</v>
+        <v>901</v>
       </c>
       <c r="J110" s="11" t="s">
-        <v>918</v>
+        <v>902</v>
       </c>
       <c r="K110" s="11" t="s">
-        <v>218</v>
+        <v>903</v>
       </c>
       <c r="L110" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
         <v>212</v>
       </c>
@@ -9600,34 +9638,34 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>919</v>
+        <v>904</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>920</v>
+        <v>905</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>921</v>
-      </c>
-      <c r="G111" s="13" t="s">
-        <v>922</v>
-      </c>
-      <c r="H111" s="11" t="s">
-        <v>923</v>
+        <v>906</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>907</v>
+      </c>
+      <c r="H111" s="14" t="s">
+        <v>866</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>924</v>
+        <v>908</v>
       </c>
       <c r="J111" s="11" t="s">
-        <v>210</v>
+        <v>909</v>
       </c>
       <c r="K111" s="11" t="s">
-        <v>211</v>
+        <v>910</v>
       </c>
       <c r="L111" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
         <v>212</v>
       </c>
@@ -9638,88 +9676,163 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>911</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>912</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>913</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>914</v>
+      </c>
+      <c r="H112" s="14" t="s">
+        <v>915</v>
+      </c>
+      <c r="I112" s="11" t="s">
+        <v>916</v>
+      </c>
+      <c r="J112" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="K112" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="L112" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B113" s="10">
+        <v>27</v>
+      </c>
+      <c r="C113" s="5">
+        <v>112</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>919</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="G113" s="13" t="s">
+        <v>921</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="I113" s="11" t="s">
+        <v>923</v>
+      </c>
+      <c r="J113" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="K113" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L113" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B114" s="10">
+        <v>27</v>
+      </c>
+      <c r="C114" s="5">
+        <v>113</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>924</v>
+      </c>
+      <c r="E114" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="F114" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="H114" s="11" t="s">
         <v>928</v>
       </c>
-      <c r="H112" s="11" t="s">
+      <c r="I114" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="I112" s="11" t="s">
+      <c r="J114" s="11" t="s">
         <v>930</v>
       </c>
-      <c r="J112" s="11" t="s">
-        <v>931</v>
-      </c>
-      <c r="K112" s="11" t="s">
+      <c r="K114" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="L112" s="15" t="s">
+      <c r="L114" s="15" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="55" t="s">
+    <row r="115" spans="1:12" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H114" s="12"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G115" s="12"/>
-      <c r="H115" s="12"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H116" s="12"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E118" s="15"/>
-      <c r="F118" s="15"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="15"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B125" s="15"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-    </row>
-    <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H118" s="12"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B127" s="15"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A113:XFD113"/>
+    <mergeCell ref="A115:XFD115"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H56" r:id="rId1" xr:uid="{E3E5EE19-390C-664B-BB84-8F07516336D5}"/>
-    <hyperlink ref="G58" r:id="rId2" xr:uid="{79725694-8018-C74D-A18D-0A759C387135}"/>
-    <hyperlink ref="H58" r:id="rId3" display="https://docs.microsoft.com/en-us/security-updates/securitybulletins/2017/ms17-010; " xr:uid="{BAE5451F-3D65-3340-823F-5831B8D023EE}"/>
-    <hyperlink ref="G59" r:id="rId4" xr:uid="{4D6CD9F0-BFA5-E848-A914-5C67E213F678}"/>
-    <hyperlink ref="H59" r:id="rId5" display="https://cve.mitre.org/cgi-bin/cvename.cgi?name=cve-2014-0160" xr:uid="{7F08741A-BD16-1E49-8989-D0EC113B9D3E}"/>
-    <hyperlink ref="G60" r:id="rId6" xr:uid="{1E36F908-7519-484C-85A8-822DF0FBC42D}"/>
-    <hyperlink ref="H60" r:id="rId7" xr:uid="{2FB8C147-AEEA-EC49-ADDB-81803C01EB2F}"/>
-    <hyperlink ref="G61" r:id="rId8" xr:uid="{D9B310EA-7E23-254B-ADE1-06F3B88CED5C}"/>
-    <hyperlink ref="H61" r:id="rId9" xr:uid="{0E53B227-0BB5-F54B-A9A1-588A9C946C35}"/>
-    <hyperlink ref="G62" r:id="rId10" xr:uid="{08D6DAB1-18FD-5643-BA47-7804B3669EFB}"/>
-    <hyperlink ref="G65" r:id="rId11" xr:uid="{DCE48871-BFCF-6B4A-BE57-304663B66573}"/>
-    <hyperlink ref="H65" r:id="rId12" display="https://www.tenable.com/plugins/nessus/77823 " xr:uid="{BF747F71-3ECF-2944-B87E-D77595FFBF7F}"/>
-    <hyperlink ref="H66" r:id="rId13" xr:uid="{77CC2867-2BAC-474C-9CC9-E6B06FEE8BCF}"/>
-    <hyperlink ref="G63" r:id="rId14" xr:uid="{731D6ABC-81D0-8D4F-9F9D-FE3D146708CA}"/>
-    <hyperlink ref="H64" r:id="rId15" xr:uid="{22133728-DEDB-5142-9DF5-F1BE54D7AAB6}"/>
-    <hyperlink ref="H80" r:id="rId16" location="session-id-properties " xr:uid="{58A25760-4DA5-B443-8B5E-9B5D3FC9E1A7}"/>
-    <hyperlink ref="H92" r:id="rId17" xr:uid="{C47382A9-4D26-A749-84E4-62C1B59DBAEC}"/>
+    <hyperlink ref="H58" r:id="rId1" xr:uid="{E3E5EE19-390C-664B-BB84-8F07516336D5}"/>
+    <hyperlink ref="G60" r:id="rId2" xr:uid="{79725694-8018-C74D-A18D-0A759C387135}"/>
+    <hyperlink ref="H60" r:id="rId3" display="https://docs.microsoft.com/en-us/security-updates/securitybulletins/2017/ms17-010; " xr:uid="{BAE5451F-3D65-3340-823F-5831B8D023EE}"/>
+    <hyperlink ref="G61" r:id="rId4" xr:uid="{4D6CD9F0-BFA5-E848-A914-5C67E213F678}"/>
+    <hyperlink ref="H61" r:id="rId5" display="https://cve.mitre.org/cgi-bin/cvename.cgi?name=cve-2014-0160" xr:uid="{7F08741A-BD16-1E49-8989-D0EC113B9D3E}"/>
+    <hyperlink ref="G62" r:id="rId6" xr:uid="{1E36F908-7519-484C-85A8-822DF0FBC42D}"/>
+    <hyperlink ref="H62" r:id="rId7" xr:uid="{2FB8C147-AEEA-EC49-ADDB-81803C01EB2F}"/>
+    <hyperlink ref="G63" r:id="rId8" xr:uid="{D9B310EA-7E23-254B-ADE1-06F3B88CED5C}"/>
+    <hyperlink ref="H63" r:id="rId9" xr:uid="{0E53B227-0BB5-F54B-A9A1-588A9C946C35}"/>
+    <hyperlink ref="G64" r:id="rId10" xr:uid="{08D6DAB1-18FD-5643-BA47-7804B3669EFB}"/>
+    <hyperlink ref="G67" r:id="rId11" xr:uid="{DCE48871-BFCF-6B4A-BE57-304663B66573}"/>
+    <hyperlink ref="H67" r:id="rId12" display="https://www.tenable.com/plugins/nessus/77823 " xr:uid="{BF747F71-3ECF-2944-B87E-D77595FFBF7F}"/>
+    <hyperlink ref="H68" r:id="rId13" xr:uid="{77CC2867-2BAC-474C-9CC9-E6B06FEE8BCF}"/>
+    <hyperlink ref="G65" r:id="rId14" xr:uid="{731D6ABC-81D0-8D4F-9F9D-FE3D146708CA}"/>
+    <hyperlink ref="H66" r:id="rId15" xr:uid="{22133728-DEDB-5142-9DF5-F1BE54D7AAB6}"/>
+    <hyperlink ref="H82" r:id="rId16" location="session-id-properties " xr:uid="{58A25760-4DA5-B443-8B5E-9B5D3FC9E1A7}"/>
+    <hyperlink ref="H94" r:id="rId17" xr:uid="{C47382A9-4D26-A749-84E4-62C1B59DBAEC}"/>
     <hyperlink ref="G18" r:id="rId18" xr:uid="{20CDB420-039D-4073-8B03-34EB73AB9D23}"/>
     <hyperlink ref="G19" r:id="rId19" xr:uid="{5ECE399F-56DC-4AFF-8846-25C0C21A2971}"/>
     <hyperlink ref="G21" r:id="rId20" xr:uid="{804C38DA-F955-475B-8351-09FF4836D2D0}"/>
@@ -9727,27 +9840,27 @@
     <hyperlink ref="G22" r:id="rId22" xr:uid="{F5961F24-DD55-4339-BA32-EC8A192206FC}"/>
     <hyperlink ref="G25" r:id="rId23" xr:uid="{9E023A42-E15B-4C66-A4FB-BE58ACC88978}"/>
     <hyperlink ref="H25" r:id="rId24" xr:uid="{54845AE6-8A6C-49F1-A45F-D2D479EE1358}"/>
-    <hyperlink ref="H103" r:id="rId25" xr:uid="{2FB2A55E-28DE-4C15-98CC-73BB7648A661}"/>
-    <hyperlink ref="H106" r:id="rId26" xr:uid="{2AEB1866-2293-486C-BA4D-76FD11A7420F}"/>
-    <hyperlink ref="H109" r:id="rId27" xr:uid="{A7D928B5-CA12-4564-8AB4-62738B801DD1}"/>
+    <hyperlink ref="H105" r:id="rId25" xr:uid="{2FB2A55E-28DE-4C15-98CC-73BB7648A661}"/>
+    <hyperlink ref="H108" r:id="rId26" xr:uid="{2AEB1866-2293-486C-BA4D-76FD11A7420F}"/>
+    <hyperlink ref="H111" r:id="rId27" xr:uid="{A7D928B5-CA12-4564-8AB4-62738B801DD1}"/>
     <hyperlink ref="G11" r:id="rId28" xr:uid="{9B5DE842-6B82-4467-AFEA-A81F388BC653}"/>
-    <hyperlink ref="G51" r:id="rId29" xr:uid="{A1DC0B20-B4FB-49E0-B1E3-5FF7F98C726C}"/>
-    <hyperlink ref="H51" r:id="rId30" xr:uid="{89D86FCF-1298-4B55-AD42-22F65DA42419}"/>
-    <hyperlink ref="G53" r:id="rId31" xr:uid="{962B4F4F-A783-4A2C-BEC7-6399217B56E9}"/>
-    <hyperlink ref="H53" r:id="rId32" xr:uid="{FEF5588E-F25F-4EBF-BA84-18C93FB7C1DF}"/>
-    <hyperlink ref="G52" r:id="rId33" xr:uid="{4F61F0AC-ACEB-472B-95DE-9C5B8E003D6E}"/>
-    <hyperlink ref="H52" r:id="rId34" xr:uid="{56042EEB-F706-4D44-988F-4DAF1E3D531B}"/>
-    <hyperlink ref="H71" r:id="rId35" xr:uid="{A2BC347A-A774-47C9-8872-CBBB3514C8C7}"/>
-    <hyperlink ref="H70" r:id="rId36" display="http://projects.webappsec.org/w/page/13246934/Improper%20Output%20Handling" xr:uid="{CB2FC2C4-6BCD-4584-BF52-937947D8A24C}"/>
-    <hyperlink ref="G97" r:id="rId37" xr:uid="{9D5C616F-628F-43EB-889F-779D8A853FF4}"/>
-    <hyperlink ref="H97" r:id="rId38" xr:uid="{5BD6E029-07B5-4603-8161-E1F706EB4730}"/>
-    <hyperlink ref="H75" r:id="rId39" xr:uid="{2E5795AD-3852-4C18-B930-F986C9802164}"/>
-    <hyperlink ref="H76" r:id="rId40" xr:uid="{E489A080-F4BD-47FC-8573-C2E936BE5954}"/>
-    <hyperlink ref="H77" r:id="rId41" xr:uid="{C1EBC70B-85F0-4064-9A36-0ED1076A3BFB}"/>
-    <hyperlink ref="H83" r:id="rId42" xr:uid="{8023BE1E-0091-4353-A35E-40AA5AAC869D}"/>
-    <hyperlink ref="G86" r:id="rId43" xr:uid="{BBFEEECF-B75F-43D9-83BD-2EE506846ABE}"/>
-    <hyperlink ref="H86" r:id="rId44" xr:uid="{E0C771FD-3F24-4775-93CA-5B24D6414AD3}"/>
-    <hyperlink ref="H110" r:id="rId45" xr:uid="{2996AAEE-F0E3-4E27-8055-0BDE2B6AB80F}"/>
+    <hyperlink ref="G53" r:id="rId29" xr:uid="{A1DC0B20-B4FB-49E0-B1E3-5FF7F98C726C}"/>
+    <hyperlink ref="H53" r:id="rId30" xr:uid="{89D86FCF-1298-4B55-AD42-22F65DA42419}"/>
+    <hyperlink ref="G55" r:id="rId31" xr:uid="{962B4F4F-A783-4A2C-BEC7-6399217B56E9}"/>
+    <hyperlink ref="H55" r:id="rId32" xr:uid="{FEF5588E-F25F-4EBF-BA84-18C93FB7C1DF}"/>
+    <hyperlink ref="G54" r:id="rId33" xr:uid="{4F61F0AC-ACEB-472B-95DE-9C5B8E003D6E}"/>
+    <hyperlink ref="H54" r:id="rId34" xr:uid="{56042EEB-F706-4D44-988F-4DAF1E3D531B}"/>
+    <hyperlink ref="H73" r:id="rId35" xr:uid="{A2BC347A-A774-47C9-8872-CBBB3514C8C7}"/>
+    <hyperlink ref="H72" r:id="rId36" display="http://projects.webappsec.org/w/page/13246934/Improper%20Output%20Handling" xr:uid="{CB2FC2C4-6BCD-4584-BF52-937947D8A24C}"/>
+    <hyperlink ref="G99" r:id="rId37" xr:uid="{9D5C616F-628F-43EB-889F-779D8A853FF4}"/>
+    <hyperlink ref="H99" r:id="rId38" xr:uid="{5BD6E029-07B5-4603-8161-E1F706EB4730}"/>
+    <hyperlink ref="H77" r:id="rId39" xr:uid="{2E5795AD-3852-4C18-B930-F986C9802164}"/>
+    <hyperlink ref="H78" r:id="rId40" xr:uid="{E489A080-F4BD-47FC-8573-C2E936BE5954}"/>
+    <hyperlink ref="H79" r:id="rId41" xr:uid="{C1EBC70B-85F0-4064-9A36-0ED1076A3BFB}"/>
+    <hyperlink ref="H85" r:id="rId42" xr:uid="{8023BE1E-0091-4353-A35E-40AA5AAC869D}"/>
+    <hyperlink ref="G88" r:id="rId43" xr:uid="{BBFEEECF-B75F-43D9-83BD-2EE506846ABE}"/>
+    <hyperlink ref="H88" r:id="rId44" xr:uid="{E0C771FD-3F24-4775-93CA-5B24D6414AD3}"/>
+    <hyperlink ref="H112" r:id="rId45" xr:uid="{2996AAEE-F0E3-4E27-8055-0BDE2B6AB80F}"/>
     <hyperlink ref="H11" r:id="rId46" xr:uid="{E7CC593B-381A-42C1-8235-E9FE8F4EBDE6}"/>
     <hyperlink ref="H10" r:id="rId47" xr:uid="{F3E53C64-A85C-4858-BECE-41030BDF79AC}"/>
     <hyperlink ref="G36" r:id="rId48" xr:uid="{3F4FD4EB-63A9-194F-9EEC-F032D5E47A97}"/>
@@ -9755,15 +9868,15 @@
     <hyperlink ref="G37" r:id="rId50" xr:uid="{E3339C55-C438-C343-8296-50A5BBB1E31B}"/>
     <hyperlink ref="H37" r:id="rId51" xr:uid="{8FB2D010-6C28-094A-8060-9D2127C6E67A}"/>
     <hyperlink ref="H32" r:id="rId52" xr:uid="{BC2EF8F6-F365-AE4D-AAAC-85DCDDF298B1}"/>
-    <hyperlink ref="G69" r:id="rId53" xr:uid="{23FD6DEA-3224-064C-899F-51BD412808E4}"/>
+    <hyperlink ref="G71" r:id="rId53" xr:uid="{23FD6DEA-3224-064C-899F-51BD412808E4}"/>
     <hyperlink ref="G30" r:id="rId54" display="https://www.microsoft.com/en-us/security/business/security-101/what-is-phishing?ef_id=b4f814899ed11b3c078676681374cbb9:G:s&amp;OCID=AIDcmmdamuj0pc_SEM_b4f814899ed11b3c078676681374cbb9:G:s&amp;msclkid=b4f814899ed11b3c078676681374cbb9 https://www.researchgate.net/publication/351945314_Testing_the_Susceptibility_of_Employees_to_Phishing_Emails " xr:uid="{C319C971-5FF7-4988-BE11-CB4E13A67D00}"/>
     <hyperlink ref="G31" r:id="rId55" xr:uid="{CCFE6F46-C6A3-4A2B-8856-D3C7E382DF59}"/>
-    <hyperlink ref="G73" r:id="rId56" xr:uid="{3CBDA1D9-4748-5643-8727-42343038D3B2}"/>
-    <hyperlink ref="H73" r:id="rId57" xr:uid="{39E12E3A-D714-154A-8F1E-087BF7C257C0}"/>
+    <hyperlink ref="G75" r:id="rId56" xr:uid="{3CBDA1D9-4748-5643-8727-42343038D3B2}"/>
+    <hyperlink ref="H75" r:id="rId57" xr:uid="{39E12E3A-D714-154A-8F1E-087BF7C257C0}"/>
     <hyperlink ref="G6" r:id="rId58" display="https://docs.microsoft.com/en-us/previous-versions/windows/it-pro/windows-server-2008-R2-and-2008/dd560653(v=ws.10)https://docs.microsoft.com/en-us/previous-versions/windows/it-pro/windows-server-2008-R2-and-2008/jj865676(v=ws.10)https://www.securew2.com/blog/why-ntlm-authentication-is-vulnerablehttps://securityboulevard.com/2018/10/the-security-risks-of-ntlm-proceed-with-caution/https://www.calcomsoftware.com/ntlm-security-weaknesses/ " xr:uid="{4E820C75-00EE-2241-9933-10EF05514CAF}"/>
     <hyperlink ref="G7" r:id="rId59" xr:uid="{3A3F0AC4-D3F6-CF4D-9BD5-66D84EA59160}"/>
-    <hyperlink ref="G88" r:id="rId60" location=":~:text=Insecure%20SSL%2FTLS%20Protocol%20Using%20insecure%20and%20deprecated%20protocols,and%20POODLE%20%28Padding%20Oracle%20On%20Downgraded%20Legacy%20Encryption%29. " xr:uid="{917C86E2-CF4D-AA49-8F5C-64B9882073CC}"/>
-    <hyperlink ref="G83" r:id="rId61" xr:uid="{22A28A6D-4A94-4EBC-A45B-399D3089371E}"/>
+    <hyperlink ref="G90" r:id="rId60" location=":~:text=Insecure%20SSL%2FTLS%20Protocol%20Using%20insecure%20and%20deprecated%20protocols,and%20POODLE%20%28Padding%20Oracle%20On%20Downgraded%20Legacy%20Encryption%29. " xr:uid="{917C86E2-CF4D-AA49-8F5C-64B9882073CC}"/>
+    <hyperlink ref="G85" r:id="rId61" xr:uid="{22A28A6D-4A94-4EBC-A45B-399D3089371E}"/>
     <hyperlink ref="H13" r:id="rId62" display="https://blog.fox-it.com/2018/04/26/escalating-privileges-with-acls-in-active-directory/ https://book.hacktricks.xyz/windows-hardening/active-directory-methodology/acl-persistence-abuse https://wald0.com/?p=112 https://msdn.microsoft.com/en-us/library/windows/desktop/aa379557(v=vs.85).aspx " xr:uid="{ED344202-07BF-4354-91DF-1162658C70AE}"/>
     <hyperlink ref="G13" r:id="rId63" xr:uid="{C4CF194C-DC8E-4116-B40A-318AF1DD4328}"/>
   </hyperlinks>
@@ -9776,6 +9889,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -9907,22 +10035,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9938,21 +10068,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Miscellaneous updates throughout the app and fixes to the ptp.py script
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ED047B-AF1A-BB4C-BDA9-862528ACE9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05980C1-A667-644D-8DB0-82891DD5927A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="2620" windowWidth="34820" windowHeight="19640" activeTab="3" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="24500" yWindow="2640" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -1491,12 +1491,6 @@
     <t>Malicious File Download</t>
   </si>
   <si>
-    <t>A malicious payload is a payload that bypasses host protections and downloads successfully on a user’s system. Dangerous file types that are frequently sent by email include .exe, .doc, .xls, .xlsx, .pdf, .docx, .rtf, .xlsm, and .vbs. When delivering malicious payloads, these potentially malicious files can also be contained in other file types, such as compressed or archived files, disk images, and scripts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement employee cybersecurity training; perform continuous virus scanning, file scanning, and inspection; continuously monitor the network; and implement spam filters/phishing detection systems, firewalls, and zero-trust policies. </t>
-  </si>
-  <si>
     <t>https://www.certifiedcio.com/2021/04/22/malicious-downloads/ https://www.statista.com/statistics/1238996/top-malware-by-file-type/</t>
   </si>
   <si>
@@ -1515,12 +1509,6 @@
     <t>Malicious File Execution</t>
   </si>
   <si>
-    <t xml:space="preserve">After downloading (through an email attachment or direct link), malicious files can be executed with or without user interaction. This malicious file execution can happen if the user’s system mistakenly believes the malicious payload to be legitimate, or the malicious file might successfully bypass any security measure(s) in place to detect and prevent it from running. The attacker might obfuscate these files to improve the chances of their successful execution, which may allow the attacker to gain a foothold in the organization’s system and carry out attacks that would compromise the confidentiality, integrity, and availability (CIA) of the system. Common malicious file types used are .exe, .hta, .js, .dll, and .cpl. </t>
-  </si>
-  <si>
-    <t>Use an antivirus program and set up a firewall to detect malware. Disable macro scripts in Microsoft Office files that are transmitted in email. Use a domain reputation service to detect and block suspicious or malicious domains. Use browser and application sandboxes or remote virtual environments to mitigate browser or other application exploitation.</t>
-  </si>
-  <si>
     <t>https://www.cisa.gov/uscert/ncas/alerts/aa21-200b https://attack.mitre.org/techniques/T1204/002/</t>
   </si>
   <si>
@@ -1528,9 +1516,6 @@
   </si>
   <si>
     <t>Malicious Code Execution Within Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A user may download a document that contains malicious software from phishing email or an insecure website. The document might contain a malicious or embedded (and heavily obfuscated) macro, script, or Object Linking and Embedding (OLE). With OLE, the malicious code is installed from an external website after it is triggered. The execution of the malicious code can be with or without user interaction, depending on the type. Once the malware is installed, the attacker can gain a foothold on the user’s system. </t>
   </si>
   <si>
     <t>Use a domain reputation service to detect and block suspicious or malicious domains. Enforce a Group Policy setting that disables macro from executing through protected view or protected editing, preventing macros from running automatically. Keep up to date with patches. Use file sanitization techniques (e.g., converting to another format, which can retain valuable information while eliminating embedded malware and stripping out embedded objects in document). Create blocklists. Perform static and dynamic analyses of downloaded documents.</t>
@@ -3228,6 +3213,21 @@
   </si>
   <si>
     <t>Implement a review process for files and systems to identify insecure handling of PII, PHI, and other sensitive information. Properly secure or remove the information. Conduct periodic scans of systems using automated tools to determine whether sensitive data is present on the system in cleartext. User awareness training outlining best practices for sensitive information storage can be effective, but does not guarantee secure storage.</t>
+  </si>
+  <si>
+    <t>A malicious payload is a payload that bypasses host protections and downloads successfully on a user’s system. Dangerous file types that are frequently sent by email include EXE, PIF, DLL, ISO, IMG, HTA, JS, CPL, BIN, PY, PDF, DOC, DOCX, XLS, XLSX, XLSM, RTF, and VBS. When delivering malicious payloads, these potentially malicious files can also be contained in other file types, such as compressed or archived files, disk images, and scripts, or inflated to a large size to circumvent browser or email client security checks.</t>
+  </si>
+  <si>
+    <t>Implement employee cybersecurity training; perform continuous virus scanning, file scanning, and inspection; continuously monitor the network; and implement spam filters/phishing detection systems, firewalls, and zero-trust policies. Unless there is a business need for EXE, PIF, DLL, ISO, IMG, HTA, JS, CPL, BIN, PY, PDF, DOC, DOCX, XLS, XLSX, XLSM, RTF, VBS, or other commonly malicious file types to download, it is recommended to prevent users from downloading these types of files through use of policies and security solutions.</t>
+  </si>
+  <si>
+    <t>After downloading (through an email attachment or direct link), malicious files can be executed with or without user interaction. This malicious file execution can happen if the user’s system mistakenly believes the malicious payload to be legitimate, or the malicious file might successfully bypass any security measure(s) in place to detect and prevent it from running. The attacker might obfuscate these files to improve the chances of their successful execution, which may allow the attacker to gain a foothold in the organization’s system and carry out attacks that would compromise the confidentiality, integrity, and availability (CIA) of the system. Common malicious file types used are EXE, PIF, DLL, ISO, IMG, HTA, JS, CPL, BIN, PY, and VBS.</t>
+  </si>
+  <si>
+    <t>Use an antivirus program and set up a firewall to detect malware. Disable macro scripts in Microsoft Office files that are transmitted in email. Use a domain reputation service to detect and block suspicious or malicious domains. Use browser and application sandboxes or remote virtual environments to mitigate browser or other application exploitation. Unless there is a business need for EXE, PIF, DLL, ISO, IMG, HTA, JS, CPL, BIN, PY, VBS, or other commonly malicious file types to execute or mount on systems, it is recommended to prevent users from executing or mounting these types of files through use of policies and security solutions.</t>
+  </si>
+  <si>
+    <t>A user may download a document that contains malicious software from a phishing email or an insecure website. The document might contain a malicious and heavily obfuscated macro, script, or embedded object via Object Linking and Embedding (OLE). OLEs can install malicious code from an external website after it is triggered. The execution of the malicious code can be with or without user interaction, depending on the type. Once the malware is installed, an attacker can gain a foothold on the user’s system under the context of a valid domain user.</t>
   </si>
 </sst>
 </file>
@@ -4280,7 +4280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDF0EF5-6DED-0A40-A55B-9157B9D1CA48}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -4295,9 +4295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43849457-AD8B-FC4F-883C-916F9AD054DA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4448,8 +4446,8 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4532,7 +4530,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4567,7 +4565,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4602,7 +4600,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4638,7 +4636,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4676,7 +4674,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4748,7 +4746,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4932,7 +4930,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -4968,7 +4966,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5517,9 +5515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE6EBA3-B14F-E947-A615-39B9D02994B2}">
   <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5729,7 +5727,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>37</v>
       </c>
@@ -5980,7 +5978,7 @@
         <v>294</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>295</v>
@@ -6065,7 +6063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>50</v>
       </c>
@@ -6094,7 +6092,7 @@
         <v>317</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6167,7 +6165,7 @@
         <v>329</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>330</v>
@@ -6700,7 +6698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>101</v>
       </c>
@@ -6714,25 +6712,25 @@
         <v>421</v>
       </c>
       <c r="E32" s="10" t="s">
+        <v>954</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>955</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="H32" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="I32" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="J32" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>426</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>428</v>
       </c>
       <c r="L32" s="15" t="s">
         <v>54</v>
@@ -6749,20 +6747,20 @@
         <v>32</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>430</v>
+        <v>956</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>431</v>
+        <v>957</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>106</v>
@@ -6785,20 +6783,20 @@
         <v>33</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>435</v>
+        <v>958</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>106</v>
@@ -6821,20 +6819,20 @@
         <v>34</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>106</v>
@@ -6857,25 +6855,25 @@
         <v>35</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="K36" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>448</v>
       </c>
       <c r="L36" s="15" t="s">
         <v>43</v>
@@ -6892,22 +6890,22 @@
         <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>452</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>453</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>454</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>210</v>
@@ -6930,19 +6928,19 @@
         <v>37</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>210</v>
@@ -6965,25 +6963,25 @@
         <v>38</v>
       </c>
       <c r="D39" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="K39" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>465</v>
       </c>
       <c r="L39" s="15" t="s">
         <v>43</v>
@@ -7000,25 +6998,25 @@
         <v>39</v>
       </c>
       <c r="D40" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="K40" s="4" t="s">
         <v>467</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>469</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>472</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>43</v>
@@ -7035,25 +7033,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="J41" s="4" t="s">
         <v>474</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>475</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>476</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>479</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>196</v>
@@ -7073,28 +7071,28 @@
         <v>41</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="J42" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="K42" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>487</v>
       </c>
       <c r="L42" s="15" t="s">
         <v>54</v>
@@ -7111,28 +7109,28 @@
         <v>42</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="J43" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="K43" s="4" t="s">
         <v>490</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>495</v>
       </c>
       <c r="L43" s="15" t="s">
         <v>296</v>
@@ -7149,28 +7147,28 @@
         <v>43</v>
       </c>
       <c r="D44" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="I44" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="J44" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="K44" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>503</v>
       </c>
       <c r="L44" s="15" t="s">
         <v>43</v>
@@ -7187,22 +7185,22 @@
         <v>44</v>
       </c>
       <c r="D45" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>504</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>507</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>509</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>342</v>
@@ -7225,26 +7223,26 @@
         <v>45</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="4" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L46" s="15" t="s">
         <v>43</v>
@@ -7261,28 +7259,28 @@
         <v>46</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>514</v>
+      </c>
+      <c r="H47" s="29" t="s">
+        <v>515</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="J47" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>519</v>
-      </c>
-      <c r="H47" s="29" t="s">
-        <v>520</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>522</v>
-      </c>
       <c r="K47" s="4" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L47" s="15" t="s">
         <v>43</v>
@@ -7299,26 +7297,26 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>955</v>
+        <v>950</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>956</v>
+        <v>951</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>957</v>
+        <v>952</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>946</v>
+        <v>941</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
+        <v>943</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>948</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>952</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>953</v>
       </c>
       <c r="L48" s="15" t="s">
         <v>54</v>
@@ -7335,29 +7333,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>958</v>
+        <v>953</v>
       </c>
       <c r="G49" s="29" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>949</v>
       </c>
-      <c r="J49" s="4" t="s">
-        <v>951</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>954</v>
-      </c>
       <c r="L49" s="15" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="221" x14ac:dyDescent="0.2">
@@ -7371,26 +7369,26 @@
         <v>49</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="4" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="L50" s="15" t="s">
         <v>43</v>
@@ -7407,26 +7405,26 @@
         <v>50</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="H51" s="29"/>
       <c r="I51" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="L51" s="15" t="s">
         <v>43</v>
@@ -7443,26 +7441,26 @@
         <v>51</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="H52" s="29"/>
       <c r="I52" s="4" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="L52" s="15" t="s">
         <v>43</v>
@@ -7479,28 +7477,28 @@
         <v>52</v>
       </c>
       <c r="D53" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="G53" s="43" t="s">
+        <v>539</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>539</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="J53" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="K53" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="G53" s="43" t="s">
-        <v>544</v>
-      </c>
-      <c r="H53" s="43" t="s">
-        <v>544</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>546</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="L53" s="15" t="s">
         <v>54</v>
@@ -7517,28 +7515,28 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="G54" s="43" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="H54" s="43" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="L54" s="15" t="s">
         <v>54</v>
@@ -7555,28 +7553,28 @@
         <v>54</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G55" s="43" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="H55" s="43" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="L55" s="15" t="s">
         <v>54</v>
@@ -7593,25 +7591,25 @@
         <v>55</v>
       </c>
       <c r="D56" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="I56" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="J56" s="4" t="s">
         <v>556</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>557</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>560</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>561</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>364</v>
@@ -7631,21 +7629,21 @@
         <v>56</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>364</v>
@@ -7665,28 +7663,28 @@
         <v>57</v>
       </c>
       <c r="D58" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="I58" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="J58" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="K58" s="4" t="s">
         <v>567</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>569</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>54</v>
@@ -7703,25 +7701,25 @@
         <v>58</v>
       </c>
       <c r="D59" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="J59" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>575</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>576</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>577</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>579</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>248</v>
@@ -7741,28 +7739,28 @@
         <v>59</v>
       </c>
       <c r="D60" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="K60" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>582</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>583</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>54</v>
@@ -7779,28 +7777,28 @@
         <v>60</v>
       </c>
       <c r="D61" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="J61" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="K61" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>590</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>591</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>594</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>54</v>
@@ -7817,28 +7815,28 @@
         <v>61</v>
       </c>
       <c r="D62" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="J62" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="K62" s="4" t="s">
         <v>597</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>598</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>599</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>602</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>54</v>
@@ -7855,28 +7853,28 @@
         <v>62</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="J63" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="K63" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="G63" s="14" t="s">
-        <v>605</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>606</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>608</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>54</v>
@@ -7893,23 +7891,23 @@
         <v>63</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>248</v>
@@ -7929,28 +7927,28 @@
         <v>64</v>
       </c>
       <c r="D65" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="I65" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="J65" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="K65" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>618</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>619</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>622</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>54</v>
@@ -7967,28 +7965,28 @@
         <v>65</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="F66" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="K66" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>625</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>626</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>622</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>54</v>
@@ -8005,28 +8003,28 @@
         <v>66</v>
       </c>
       <c r="D67" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>625</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="I67" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="E67" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>630</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>631</v>
-      </c>
-      <c r="H67" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>633</v>
-      </c>
       <c r="J67" s="4" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>54</v>
@@ -8043,31 +8041,31 @@
         <v>67</v>
       </c>
       <c r="D68" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="J68" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>635</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>637</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>638</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>639</v>
       </c>
       <c r="K68" s="4">
         <v>7</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="255" x14ac:dyDescent="0.2">
@@ -8081,20 +8079,20 @@
         <v>68</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="4" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>145</v>
@@ -8117,20 +8115,20 @@
         <v>69</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="4" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>145</v>
@@ -8153,20 +8151,20 @@
         <v>70</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="4" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>145</v>
@@ -8189,25 +8187,25 @@
         <v>71</v>
       </c>
       <c r="D72" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="H72" s="43" t="s">
+        <v>652</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="J72" s="11" t="s">
         <v>654</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>655</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>656</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>657</v>
-      </c>
-      <c r="H72" s="43" t="s">
-        <v>657</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>658</v>
-      </c>
-      <c r="J72" s="11" t="s">
-        <v>659</v>
       </c>
       <c r="K72" s="11">
         <v>16</v>
@@ -8227,25 +8225,25 @@
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="H73" s="43" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="J73" s="11" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="K73" s="11">
         <v>16</v>
@@ -8265,23 +8263,23 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="K74" s="11" t="s">
         <v>268</v>
@@ -8301,28 +8299,28 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="I75" s="10" t="s">
         <v>670</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="J75" s="10" t="s">
+        <v>936</v>
+      </c>
+      <c r="K75" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F75" s="10" t="s">
-        <v>672</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>673</v>
-      </c>
-      <c r="H75" s="14" t="s">
-        <v>674</v>
-      </c>
-      <c r="I75" s="10" t="s">
-        <v>675</v>
-      </c>
-      <c r="J75" s="10" t="s">
-        <v>941</v>
-      </c>
-      <c r="K75" s="10" t="s">
-        <v>676</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
@@ -8339,23 +8337,23 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="H76" s="14"/>
       <c r="I76" s="10" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
       <c r="K76" s="10" t="s">
         <v>330</v>
@@ -8375,25 +8373,25 @@
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>678</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>679</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>680</v>
+      </c>
+      <c r="H77" s="43" t="s">
+        <v>680</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>681</v>
+      </c>
+      <c r="J77" s="11" t="s">
         <v>682</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>684</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="H77" s="43" t="s">
-        <v>685</v>
-      </c>
-      <c r="I77" s="11" t="s">
-        <v>686</v>
-      </c>
-      <c r="J77" s="11" t="s">
-        <v>687</v>
       </c>
       <c r="K77" s="11" t="s">
         <v>364</v>
@@ -8413,23 +8411,23 @@
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>73</v>
@@ -8440,7 +8438,7 @@
     </row>
     <row r="79" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8449,25 +8447,25 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="H79" s="43" t="s">
+        <v>693</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="J79" s="11" t="s">
         <v>695</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>696</v>
-      </c>
-      <c r="F79" s="11" t="s">
-        <v>697</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>698</v>
-      </c>
-      <c r="H79" s="43" t="s">
-        <v>698</v>
-      </c>
-      <c r="I79" s="11" t="s">
-        <v>699</v>
-      </c>
-      <c r="J79" s="11" t="s">
-        <v>700</v>
       </c>
       <c r="K79" s="11">
         <v>16</v>
@@ -8478,7 +8476,7 @@
     </row>
     <row r="80" spans="1:12" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8487,19 +8485,19 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="G80" s="43" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="H80" s="43" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>172</v>
@@ -8508,7 +8506,7 @@
         <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
@@ -8516,7 +8514,7 @@
     </row>
     <row r="81" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8525,25 +8523,25 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="G81" s="43" t="s">
+        <v>704</v>
+      </c>
+      <c r="H81" s="43" t="s">
+        <v>705</v>
+      </c>
+      <c r="I81" s="11" t="s">
         <v>706</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="J81" s="11" t="s">
         <v>707</v>
-      </c>
-      <c r="F81" s="11" t="s">
-        <v>708</v>
-      </c>
-      <c r="G81" s="43" t="s">
-        <v>709</v>
-      </c>
-      <c r="H81" s="43" t="s">
-        <v>710</v>
-      </c>
-      <c r="I81" s="11" t="s">
-        <v>711</v>
-      </c>
-      <c r="J81" s="11" t="s">
-        <v>712</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>182</v>
@@ -8554,7 +8552,7 @@
     </row>
     <row r="82" spans="1:12" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8563,28 +8561,28 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>712</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="J82" s="10" t="s">
         <v>714</v>
       </c>
-      <c r="F82" s="10" t="s">
-        <v>715</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>716</v>
-      </c>
-      <c r="H82" s="14" t="s">
-        <v>717</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>718</v>
-      </c>
-      <c r="J82" s="10" t="s">
-        <v>719</v>
-      </c>
       <c r="K82" s="15" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>43</v>
@@ -8592,7 +8590,7 @@
     </row>
     <row r="83" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B83" s="10">
         <v>20</v>
@@ -8601,23 +8599,23 @@
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>182</v>
@@ -8628,7 +8626,7 @@
     </row>
     <row r="84" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B84" s="10">
         <v>20</v>
@@ -8637,26 +8635,26 @@
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>43</v>
@@ -8673,25 +8671,25 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
+        <v>724</v>
+      </c>
+      <c r="E85" s="46" t="s">
+        <v>725</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>726</v>
+      </c>
+      <c r="G85" s="43" t="s">
+        <v>727</v>
+      </c>
+      <c r="H85" s="43" t="s">
+        <v>727</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>729</v>
-      </c>
-      <c r="E85" s="46" t="s">
-        <v>730</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>731</v>
-      </c>
-      <c r="G85" s="43" t="s">
-        <v>732</v>
-      </c>
-      <c r="H85" s="43" t="s">
-        <v>732</v>
-      </c>
-      <c r="I85" s="4" t="s">
-        <v>733</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>734</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>49</v>
@@ -8711,23 +8709,23 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="F86" s="46" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>73</v>
@@ -8747,25 +8745,25 @@
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="F87" s="46" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="G87" s="29" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>73</v>
@@ -8785,28 +8783,28 @@
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
+        <v>741</v>
+      </c>
+      <c r="E88" s="46" t="s">
+        <v>742</v>
+      </c>
+      <c r="F88" s="46" t="s">
+        <v>743</v>
+      </c>
+      <c r="G88" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="H88" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="K88" s="4" t="s">
         <v>747</v>
-      </c>
-      <c r="F88" s="46" t="s">
-        <v>748</v>
-      </c>
-      <c r="G88" s="43" t="s">
-        <v>749</v>
-      </c>
-      <c r="H88" s="43" t="s">
-        <v>749</v>
-      </c>
-      <c r="I88" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>751</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>752</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
@@ -8823,25 +8821,25 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
+        <v>748</v>
+      </c>
+      <c r="E89" s="46" t="s">
+        <v>749</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>750</v>
+      </c>
+      <c r="G89" s="29" t="s">
+        <v>751</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>752</v>
+      </c>
+      <c r="I89" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="J89" s="4" t="s">
         <v>754</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>755</v>
-      </c>
-      <c r="G89" s="29" t="s">
-        <v>756</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>757</v>
-      </c>
-      <c r="I89" s="4" t="s">
-        <v>758</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>759</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>211</v>
@@ -8861,26 +8859,26 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="G90" s="16" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="K90" s="4" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
@@ -8897,26 +8895,26 @@
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="G91" s="29" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="K91" s="4" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
@@ -8933,25 +8931,25 @@
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>771</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="K92" s="4" t="s">
         <v>772</v>
-      </c>
-      <c r="F92" s="10" t="s">
-        <v>773</v>
-      </c>
-      <c r="G92" s="10" t="s">
-        <v>774</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>775</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>776</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>777</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>43</v>
@@ -8968,26 +8966,26 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
@@ -9004,28 +9002,28 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>784</v>
+      </c>
+      <c r="I94" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="J94" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="K94" s="48" t="s">
         <v>787</v>
-      </c>
-      <c r="G94" s="12" t="s">
-        <v>788</v>
-      </c>
-      <c r="H94" s="14" t="s">
-        <v>789</v>
-      </c>
-      <c r="I94" s="4" t="s">
-        <v>790</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>791</v>
-      </c>
-      <c r="K94" s="48" t="s">
-        <v>792</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>54</v>
@@ -9042,23 +9040,23 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="G95" s="29" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="K95" s="4">
         <v>3</v>
@@ -9078,26 +9076,26 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="K96" s="4" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>43</v>
@@ -9114,28 +9112,28 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>802</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>803</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>804</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>805</v>
+      </c>
+      <c r="I97" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="J97" s="4" t="s">
         <v>807</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="K97" s="4" t="s">
         <v>808</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>809</v>
-      </c>
-      <c r="H97" s="10" t="s">
-        <v>810</v>
-      </c>
-      <c r="I97" s="4" t="s">
-        <v>811</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>812</v>
-      </c>
-      <c r="K97" s="4" t="s">
-        <v>813</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>386</v>
@@ -9152,28 +9150,28 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>810</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>811</v>
+      </c>
+      <c r="G98" s="29" t="s">
+        <v>812</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>813</v>
+      </c>
+      <c r="I98" s="4" t="s">
         <v>814</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="J98" s="4" t="s">
         <v>815</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="K98" s="4" t="s">
         <v>816</v>
-      </c>
-      <c r="G98" s="29" t="s">
-        <v>817</v>
-      </c>
-      <c r="H98" s="12" t="s">
-        <v>818</v>
-      </c>
-      <c r="I98" s="4" t="s">
-        <v>819</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>820</v>
-      </c>
-      <c r="K98" s="4" t="s">
-        <v>821</v>
       </c>
       <c r="L98" s="15" t="s">
         <v>386</v>
@@ -9190,25 +9188,25 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>818</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>819</v>
+      </c>
+      <c r="G99" s="43" t="s">
+        <v>820</v>
+      </c>
+      <c r="H99" s="43" t="s">
+        <v>820</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>822</v>
-      </c>
-      <c r="E99" s="11" t="s">
-        <v>823</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>824</v>
-      </c>
-      <c r="G99" s="43" t="s">
-        <v>825</v>
-      </c>
-      <c r="H99" s="43" t="s">
-        <v>825</v>
-      </c>
-      <c r="I99" s="4" t="s">
-        <v>826</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>827</v>
       </c>
       <c r="K99" s="4">
         <v>3</v>
@@ -9228,19 +9226,19 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="I100" s="48" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="J100" s="48" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="K100" s="48" t="s">
         <v>100</v>
@@ -9260,28 +9258,28 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>830</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="I101" s="11" t="s">
         <v>833</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="J101" s="11" t="s">
+        <v>938</v>
+      </c>
+      <c r="K101" s="11" t="s">
         <v>834</v>
-      </c>
-      <c r="F101" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="G101" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="H101" s="10" t="s">
-        <v>837</v>
-      </c>
-      <c r="I101" s="11" t="s">
-        <v>838</v>
-      </c>
-      <c r="J101" s="11" t="s">
-        <v>943</v>
-      </c>
-      <c r="K101" s="11" t="s">
-        <v>839</v>
       </c>
       <c r="L101" s="15" t="s">
         <v>386</v>
@@ -9298,28 +9296,28 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>836</v>
+      </c>
+      <c r="F102" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="H102" s="11" t="s">
+        <v>839</v>
+      </c>
+      <c r="I102" s="11" t="s">
         <v>840</v>
       </c>
-      <c r="E102" s="11" t="s">
+      <c r="J102" s="11" t="s">
         <v>841</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="K102" s="11" t="s">
         <v>842</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>843</v>
-      </c>
-      <c r="H102" s="11" t="s">
-        <v>844</v>
-      </c>
-      <c r="I102" s="11" t="s">
-        <v>845</v>
-      </c>
-      <c r="J102" s="11" t="s">
-        <v>846</v>
-      </c>
-      <c r="K102" s="11" t="s">
-        <v>847</v>
       </c>
       <c r="L102" s="15" t="s">
         <v>386</v>
@@ -9336,28 +9334,28 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>845</v>
+      </c>
+      <c r="G103" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="H103" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="I103" s="11" t="s">
         <v>848</v>
       </c>
-      <c r="E103" s="11" t="s">
+      <c r="J103" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="F103" s="11" t="s">
-        <v>850</v>
-      </c>
-      <c r="G103" s="10" t="s">
-        <v>851</v>
-      </c>
-      <c r="H103" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="I103" s="11" t="s">
-        <v>853</v>
-      </c>
-      <c r="J103" s="11" t="s">
-        <v>854</v>
-      </c>
       <c r="K103" s="11" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L103" s="15" t="s">
         <v>43</v>
@@ -9374,25 +9372,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>852</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="H104" s="11" t="s">
+        <v>854</v>
+      </c>
+      <c r="I104" s="11" t="s">
         <v>855</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="J104" s="11" t="s">
         <v>856</v>
-      </c>
-      <c r="F104" s="11" t="s">
-        <v>857</v>
-      </c>
-      <c r="G104" s="11" t="s">
-        <v>858</v>
-      </c>
-      <c r="H104" s="11" t="s">
-        <v>859</v>
-      </c>
-      <c r="I104" s="11" t="s">
-        <v>860</v>
-      </c>
-      <c r="J104" s="11" t="s">
-        <v>861</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>182</v>
@@ -9412,25 +9410,25 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
+        <v>857</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>858</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="H105" s="14" t="s">
+        <v>861</v>
+      </c>
+      <c r="I105" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="J105" s="11" t="s">
         <v>863</v>
-      </c>
-      <c r="F105" s="11" t="s">
-        <v>864</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>865</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>866</v>
-      </c>
-      <c r="I105" s="11" t="s">
-        <v>867</v>
-      </c>
-      <c r="J105" s="11" t="s">
-        <v>868</v>
       </c>
       <c r="K105" s="11" t="s">
         <v>211</v>
@@ -9450,25 +9448,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
+        <v>864</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>865</v>
+      </c>
+      <c r="F106" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="G106" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="H106" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="I106" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="J106" s="11" t="s">
         <v>870</v>
-      </c>
-      <c r="F106" s="11" t="s">
-        <v>871</v>
-      </c>
-      <c r="G106" s="10" t="s">
-        <v>872</v>
-      </c>
-      <c r="H106" s="11" t="s">
-        <v>873</v>
-      </c>
-      <c r="I106" s="11" t="s">
-        <v>874</v>
-      </c>
-      <c r="J106" s="11" t="s">
-        <v>875</v>
       </c>
       <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
@@ -9486,25 +9484,25 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
+        <v>871</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>872</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>873</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="I107" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="J107" s="11" t="s">
         <v>877</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>878</v>
-      </c>
-      <c r="G107" s="10" t="s">
-        <v>879</v>
-      </c>
-      <c r="H107" s="10" t="s">
-        <v>880</v>
-      </c>
-      <c r="I107" s="11" t="s">
-        <v>881</v>
-      </c>
-      <c r="J107" s="11" t="s">
-        <v>882</v>
       </c>
       <c r="K107" s="11" t="s">
         <v>167</v>
@@ -9524,25 +9522,25 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
+        <v>878</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>879</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>880</v>
+      </c>
+      <c r="G108" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="H108" s="14" t="s">
+        <v>882</v>
+      </c>
+      <c r="I108" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>884</v>
-      </c>
-      <c r="F108" s="11" t="s">
-        <v>885</v>
-      </c>
-      <c r="G108" s="10" t="s">
-        <v>886</v>
-      </c>
-      <c r="H108" s="14" t="s">
-        <v>887</v>
-      </c>
-      <c r="I108" s="11" t="s">
-        <v>888</v>
-      </c>
-      <c r="J108" s="11" t="s">
-        <v>889</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>182</v>
@@ -9562,22 +9560,22 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
+        <v>885</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>886</v>
+      </c>
+      <c r="F109" s="11" t="s">
+        <v>887</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>888</v>
+      </c>
+      <c r="H109" s="11" t="s">
+        <v>889</v>
+      </c>
+      <c r="I109" s="11" t="s">
         <v>890</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>891</v>
-      </c>
-      <c r="F109" s="11" t="s">
-        <v>892</v>
-      </c>
-      <c r="G109" s="10" t="s">
-        <v>893</v>
-      </c>
-      <c r="H109" s="11" t="s">
-        <v>894</v>
-      </c>
-      <c r="I109" s="11" t="s">
-        <v>895</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>210</v>
@@ -9600,28 +9598,28 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
+        <v>891</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>892</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>893</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>894</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="I110" s="11" t="s">
         <v>896</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="J110" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="K110" s="11" t="s">
         <v>898</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>899</v>
-      </c>
-      <c r="H110" s="10" t="s">
-        <v>900</v>
-      </c>
-      <c r="I110" s="11" t="s">
-        <v>901</v>
-      </c>
-      <c r="J110" s="11" t="s">
-        <v>902</v>
-      </c>
-      <c r="K110" s="11" t="s">
-        <v>903</v>
       </c>
       <c r="L110" s="15" t="s">
         <v>43</v>
@@ -9638,28 +9636,28 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>900</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>901</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>902</v>
+      </c>
+      <c r="H111" s="14" t="s">
+        <v>861</v>
+      </c>
+      <c r="I111" s="11" t="s">
+        <v>903</v>
+      </c>
+      <c r="J111" s="11" t="s">
         <v>904</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="K111" s="11" t="s">
         <v>905</v>
-      </c>
-      <c r="F111" s="11" t="s">
-        <v>906</v>
-      </c>
-      <c r="G111" s="12" t="s">
-        <v>907</v>
-      </c>
-      <c r="H111" s="14" t="s">
-        <v>866</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>908</v>
-      </c>
-      <c r="J111" s="11" t="s">
-        <v>909</v>
-      </c>
-      <c r="K111" s="11" t="s">
-        <v>910</v>
       </c>
       <c r="L111" s="15" t="s">
         <v>386</v>
@@ -9676,25 +9674,25 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>908</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>909</v>
+      </c>
+      <c r="H112" s="14" t="s">
+        <v>910</v>
+      </c>
+      <c r="I112" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="J112" s="11" t="s">
         <v>912</v>
-      </c>
-      <c r="F112" s="11" t="s">
-        <v>913</v>
-      </c>
-      <c r="G112" s="10" t="s">
-        <v>914</v>
-      </c>
-      <c r="H112" s="14" t="s">
-        <v>915</v>
-      </c>
-      <c r="I112" s="11" t="s">
-        <v>916</v>
-      </c>
-      <c r="J112" s="11" t="s">
-        <v>917</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>218</v>
@@ -9714,22 +9712,22 @@
         <v>112</v>
       </c>
       <c r="D113" s="10" t="s">
+        <v>913</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>915</v>
+      </c>
+      <c r="G113" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="I113" s="11" t="s">
         <v>918</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>919</v>
-      </c>
-      <c r="F113" s="11" t="s">
-        <v>920</v>
-      </c>
-      <c r="G113" s="13" t="s">
-        <v>921</v>
-      </c>
-      <c r="H113" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="I113" s="11" t="s">
-        <v>923</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>210</v>
@@ -9752,25 +9750,25 @@
         <v>113</v>
       </c>
       <c r="D114" s="10" t="s">
+        <v>919</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>921</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="H114" s="11" t="s">
+        <v>923</v>
+      </c>
+      <c r="I114" s="11" t="s">
         <v>924</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="J114" s="11" t="s">
         <v>925</v>
-      </c>
-      <c r="F114" s="11" t="s">
-        <v>926</v>
-      </c>
-      <c r="G114" s="11" t="s">
-        <v>927</v>
-      </c>
-      <c r="H114" s="11" t="s">
-        <v>928</v>
-      </c>
-      <c r="I114" s="11" t="s">
-        <v>929</v>
-      </c>
-      <c r="J114" s="11" t="s">
-        <v>930</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>67</v>
@@ -9889,21 +9887,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -10035,24 +10018,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10068,4 +10049,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to findings repository remediation language
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05980C1-A667-644D-8DB0-82891DD5927A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB536CFB-D266-A340-BA9E-4D06548F8A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24500" yWindow="2640" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="27020" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="963">
   <si>
     <t>Finding_Category_ID</t>
   </si>
@@ -1856,9 +1856,6 @@
     <t>The Link-Local Multicast Name Resolution (LLMNR) protocol is used for alternate host identification if the default host identification system is not working. However, LLMNR can allow an impersonator to respond to unqualified domain name system (DNS) requests (i.e., those that lack a fully qualified domain name) posing as various authenticated services (e.g., Server Message Block [SMB] servers, web proxies, Remote Desktop Protocol [RDP]). The victim computer and/or user would then respond to the impersonating system with username and password credentials that can be relayed to another valid service, which can be captured, brute-force cracked, or both.</t>
   </si>
   <si>
-    <t>Disable the LLMNR protocol.</t>
-  </si>
-  <si>
     <t>https://kb.ndsu.edu/page.php?id=106754</t>
   </si>
   <si>
@@ -1879,9 +1876,6 @@
     <t>The NetBIOS Name Service (NBT-NS) is a backup host-identification system. An impersonator can use NBT-NS to intercept Windows credentials.</t>
   </si>
   <si>
-    <t>Disable NBT-NS.</t>
-  </si>
-  <si>
     <t>Multicast Domain Name System Enabled</t>
   </si>
   <si>
@@ -1930,9 +1924,6 @@
     <t>BlueKeep is a remote code execution vulnerability that exists in Remote Desktop Protocol (RDP). An unauthenticated attacker can use RDP to connect to the target system and send specially crafted requests. This pre-authentication vulnerability requires no user interaction. An attacker who exploits this vulnerability can execute arbitrary code on the target system and install programs; view, change, or delete data; or create new accounts with full user rights.</t>
   </si>
   <si>
-    <t>Update Windows on the affected hosts.</t>
-  </si>
-  <si>
     <t>https://msrc.microsoft.com/update-guide/en-US/vulnerability/CVE-2019-0708 https://www.tenable.com/blog/cve-2019-0708-bluekeep-exploits-could-be-around-the-corner</t>
   </si>
   <si>
@@ -1954,9 +1945,6 @@
     <t xml:space="preserve">A vulnerability in the DresDren-Wireless RouTer (DD-WRT) firmware on a router allows information about the router to be disclosed that can lead to further compromise of a wireless network. An attacker can find the media access control (MAC) addresses of router interfaces, connected clients, and sometimes the Global Positioning System (GPS) coordinates, if the router is registered with Google location services. </t>
   </si>
   <si>
-    <t xml:space="preserve">Update the DD-WRT firmware on routers to the latest version. </t>
-  </si>
-  <si>
     <t>https://www.tenable.com/plugins/nessus/51394, https://www.exploit-db.com/exploits/15842</t>
   </si>
   <si>
@@ -1996,9 +1984,6 @@
     <t xml:space="preserve">Heartbleed is a vulnerability that affects outdated versions of the Open Secure Sockets (OpenSSL) cryptographic software library Transport Layer Security/Datagram Transport Layer Security (TLS/DTLS) protocols. When exploited, this vulnerability leaks memory content from the communication between the server and client, resulting in information disclosure and/or data exfiltration.  </t>
   </si>
   <si>
-    <t>Update OpenSSL on the affected hosts.</t>
-  </si>
-  <si>
     <t>https://heartbleed.com/</t>
   </si>
   <si>
@@ -2020,9 +2005,6 @@
     <t>Log4Shell is a remote code execution vulnerability of Apache Log4j V2, versions older than version 2.15.0 (excluding security releases) that do not protect JNDI features from attacker-controlled Lightweight directory access protocol (LDAP), and other Java Naming and Directory Interface-related (JNDI-related) endpoints. When message lookup substitution is enabled, an attacker with control over log messages or log message parameters can execute arbitrary code loaded from LDAP servers.</t>
   </si>
   <si>
-    <t>Upgrade to a version of Apache Log4j that is version 2.16.0 or higher.</t>
-  </si>
-  <si>
     <t>https://cert-portal.siemens.com/productcert/pdf/ssa-397453.pdf</t>
   </si>
   <si>
@@ -2078,9 +2060,6 @@
   </si>
   <si>
     <t>ProxyLogon is a series of vulnerabilities in Microsoft Exchange Server that are caused by the improper validation of Uniform Resource Identifier (URI) requests to port 443, an inconsistency in backend and frontend handling of the msExchLogonMailbox header, and the improper validation of user filepath input from PowerShell to the DDIService. Attackers can exploit these vulnerabilities to perform remote code execution, bypass authentication, impersonate an administrator, upload arbitrary files, and execute arbitrary code with administrator privileges.</t>
-  </si>
-  <si>
-    <t>Update the affected installations of Microsoft Exchange Server.</t>
   </si>
   <si>
     <t xml:space="preserve">https://devco.re/blog/2021/08/06/a-new-attack-surface-on-MS-exchange-part-1-ProxyLogon/ </t>
@@ -2121,9 +2100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Shellshock is a remote code-execution vulnerability that affects hosts that run outdated versions of Bash that are also susceptible to command injection by manipulating environmental variables. </t>
-  </si>
-  <si>
-    <t>Update Bash on the affected hosts.</t>
   </si>
   <si>
     <t>https://www.tenable.com/plugins/nessus/77823</t>
@@ -3228,6 +3204,42 @@
   </si>
   <si>
     <t>A user may download a document that contains malicious software from a phishing email or an insecure website. The document might contain a malicious and heavily obfuscated macro, script, or embedded object via Object Linking and Embedding (OLE). OLEs can install malicious code from an external website after it is triggered. The execution of the malicious code can be with or without user interaction, depending on the type. Once the malware is installed, an attacker can gain a foothold on the user’s system under the context of a valid domain user.</t>
+  </si>
+  <si>
+    <t>Disable the LLMNR protocol. If disabling LLMNR is not feasible, limit its use as much as possible.</t>
+  </si>
+  <si>
+    <t>Disable NBT-NS. If disabling NBT-NS is not feasible, limit its use as much as possible.</t>
+  </si>
+  <si>
+    <t>Update Windows on the affected hosts. A set of patches is available for this vulnerability, that should be applied to the vulnerable systems. Consider disabling Server Message Block version 1 (SMBv1) and enabling a more up-to-date version of SMB.</t>
+  </si>
+  <si>
+    <t>Update Windows on the affected hosts. A set of patches is available for this vulnerability, that should be applied to the vulnerable systems.</t>
+  </si>
+  <si>
+    <t>Update Windows on the affected hosts. A set of patches is available for this vulnerability, that should be applied to the vulnerable systems. Consider disabling Remote Desktop Protocol (RDP) if it is not needed.</t>
+  </si>
+  <si>
+    <t>Maintain up-to-date firmware on routers and configure information pages to be password protected using a strong, unique password.</t>
+  </si>
+  <si>
+    <t>Upgrade OpenSSL version on the affected hosts. If upgrading is not possible, consider disabling the vulnerable component when compiling OpenSSL.</t>
+  </si>
+  <si>
+    <t>Upgrade Apache Log4j to version 2.16.0 or higher. If Apache Log4j is not needed, consider removing all vulnerable instances.</t>
+  </si>
+  <si>
+    <t>Microsoft has released security updates that mitigate this vulnerability which should be applied to the affected systems. If applying the security updates is not feasible and the print server is only used directly via attached devices, consider disabling the Print Spooler service and configuring Group Policy to prevent inbound remote printing.</t>
+  </si>
+  <si>
+    <t>Update the affected installations of Microsoft Exchange Server in order to apply the relevant security patches. Remove unnecessary instances of Microsoft Exchange to minimize attack surface.</t>
+  </si>
+  <si>
+    <t>Update Bash on the affected systems.</t>
+  </si>
+  <si>
+    <t>Microsoft has released security updates that mitigate this vulnerability which should be applied to the affected systems. Enable secure RPC enforcement mode, if feasible.</t>
   </si>
 </sst>
 </file>
@@ -4530,7 +4542,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4565,7 +4577,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4600,7 +4612,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4636,7 +4648,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4674,7 +4686,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4746,7 +4758,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4930,7 +4942,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -4966,7 +4978,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5517,7 +5529,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5978,7 +5990,7 @@
         <v>294</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>295</v>
@@ -6092,7 +6104,7 @@
         <v>317</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6165,7 +6177,7 @@
         <v>329</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>330</v>
@@ -6712,10 +6724,10 @@
         <v>421</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="F32" s="45" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>422</v>
@@ -6750,10 +6762,10 @@
         <v>427</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>428</v>
@@ -6786,7 +6798,7 @@
         <v>430</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>431</v>
@@ -7297,26 +7309,26 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="L48" s="15" t="s">
         <v>54</v>
@@ -7333,29 +7345,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="G49" s="29" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="221" x14ac:dyDescent="0.2">
@@ -7385,7 +7397,7 @@
         <v>522</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>482</v>
@@ -7483,22 +7495,22 @@
         <v>537</v>
       </c>
       <c r="F53" s="11" t="s">
+        <v>951</v>
+      </c>
+      <c r="G53" s="43" t="s">
         <v>538</v>
       </c>
-      <c r="G53" s="43" t="s">
+      <c r="H53" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="H53" s="43" t="s">
-        <v>539</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>542</v>
       </c>
       <c r="L53" s="15" t="s">
         <v>54</v>
@@ -7515,28 +7527,28 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>544</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>545</v>
+        <v>952</v>
       </c>
       <c r="G54" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="H54" s="43" t="s">
-        <v>539</v>
-      </c>
-      <c r="I54" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>542</v>
       </c>
       <c r="L54" s="15" t="s">
         <v>54</v>
@@ -7553,28 +7565,28 @@
         <v>54</v>
       </c>
       <c r="D55" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="F55" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="G55" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="F55" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="G55" s="43" t="s">
-        <v>549</v>
-      </c>
       <c r="H55" s="43" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="I55" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="K55" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>542</v>
       </c>
       <c r="L55" s="15" t="s">
         <v>54</v>
@@ -7591,25 +7603,25 @@
         <v>55</v>
       </c>
       <c r="D56" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="F56" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="G56" s="12" t="s">
         <v>551</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="H56" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="I56" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="J56" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>556</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>364</v>
@@ -7629,21 +7641,21 @@
         <v>56</v>
       </c>
       <c r="D57" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="F57" s="10" t="s">
         <v>557</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>559</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>364</v>
@@ -7663,28 +7675,28 @@
         <v>57</v>
       </c>
       <c r="D58" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>955</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="H58" s="14" t="s">
         <v>561</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="I58" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="G58" s="10" t="s">
+      <c r="J58" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="K58" s="4" t="s">
         <v>564</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>567</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>54</v>
@@ -7701,25 +7713,25 @@
         <v>58</v>
       </c>
       <c r="D59" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>956</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="H59" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="I59" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="J59" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>574</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>248</v>
@@ -7739,28 +7751,28 @@
         <v>59</v>
       </c>
       <c r="D60" s="10" t="s">
+        <v>571</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>953</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>573</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="I60" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="J60" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="F60" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="G60" s="14" t="s">
+      <c r="K60" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>578</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>580</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>581</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>54</v>
@@ -7777,28 +7789,28 @@
         <v>60</v>
       </c>
       <c r="D61" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>957</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="J61" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="K61" s="4" t="s">
         <v>584</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>585</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>586</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>587</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>588</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>589</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>54</v>
@@ -7815,28 +7827,28 @@
         <v>61</v>
       </c>
       <c r="D62" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>958</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="J62" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="K62" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>592</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>593</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>596</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>597</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>54</v>
@@ -7853,34 +7865,34 @@
         <v>62</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>954</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="K63" s="4" t="s">
         <v>598</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>599</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="G63" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>601</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>604</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>133</v>
       </c>
@@ -7891,23 +7903,23 @@
         <v>63</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>562</v>
+        <v>959</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>248</v>
@@ -7927,28 +7939,28 @@
         <v>64</v>
       </c>
       <c r="D65" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>960</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>607</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="K65" s="4" t="s">
         <v>610</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>611</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>612</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>613</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>617</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>54</v>
@@ -7965,28 +7977,28 @@
         <v>65</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>612</v>
+        <v>960</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>54</v>
@@ -8003,28 +8015,28 @@
         <v>66</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>625</v>
+        <v>961</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>54</v>
@@ -8041,31 +8053,31 @@
         <v>67</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>562</v>
+        <v>962</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="K68" s="4">
         <v>7</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="255" x14ac:dyDescent="0.2">
@@ -8079,20 +8091,20 @@
         <v>68</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="4" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>145</v>
@@ -8115,20 +8127,20 @@
         <v>69</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="4" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>145</v>
@@ -8151,20 +8163,20 @@
         <v>70</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="4" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>145</v>
@@ -8187,25 +8199,25 @@
         <v>71</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="H72" s="43" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="K72" s="11">
         <v>16</v>
@@ -8225,25 +8237,25 @@
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="H73" s="43" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="J73" s="11" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="K73" s="11">
         <v>16</v>
@@ -8263,23 +8275,23 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="K74" s="11" t="s">
         <v>268</v>
@@ -8299,28 +8311,28 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
@@ -8337,23 +8349,23 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="H76" s="14"/>
       <c r="I76" s="10" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="K76" s="10" t="s">
         <v>330</v>
@@ -8373,25 +8385,25 @@
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="H77" s="43" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="K77" s="11" t="s">
         <v>364</v>
@@ -8411,23 +8423,23 @@
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>73</v>
@@ -8438,7 +8450,7 @@
     </row>
     <row r="79" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8447,25 +8459,25 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="H79" s="43" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="K79" s="11">
         <v>16</v>
@@ -8476,7 +8488,7 @@
     </row>
     <row r="80" spans="1:12" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8485,19 +8497,19 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="G80" s="43" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="H80" s="43" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>172</v>
@@ -8506,7 +8518,7 @@
         <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
@@ -8514,7 +8526,7 @@
     </row>
     <row r="81" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8523,25 +8535,25 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="G81" s="43" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="H81" s="43" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>182</v>
@@ -8552,7 +8564,7 @@
     </row>
     <row r="82" spans="1:12" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8561,25 +8573,25 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="K82" s="15" t="s">
         <v>510</v>
@@ -8590,7 +8602,7 @@
     </row>
     <row r="83" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B83" s="10">
         <v>20</v>
@@ -8599,23 +8611,23 @@
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>182</v>
@@ -8626,7 +8638,7 @@
     </row>
     <row r="84" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B84" s="10">
         <v>20</v>
@@ -8635,20 +8647,20 @@
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>517</v>
@@ -8671,25 +8683,25 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="G85" s="43" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="H85" s="43" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>49</v>
@@ -8709,23 +8721,23 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="F86" s="46" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>73</v>
@@ -8745,25 +8757,25 @@
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="F87" s="46" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="G87" s="29" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>73</v>
@@ -8783,28 +8795,28 @@
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="E88" s="46" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="F88" s="46" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="G88" s="43" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="H88" s="43" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="K88" s="4" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
@@ -8821,25 +8833,25 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E89" s="46" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="G89" s="29" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>211</v>
@@ -8859,26 +8871,26 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="G90" s="16" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="K90" s="4" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
@@ -8895,26 +8907,26 @@
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="G91" s="29" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="K91" s="4" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
@@ -8931,25 +8943,25 @@
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="K92" s="4" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>43</v>
@@ -8966,26 +8978,26 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
@@ -9002,28 +9014,28 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="G94" s="12" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="H94" s="14" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="K94" s="48" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>54</v>
@@ -9040,23 +9052,23 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="G95" s="29" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="K95" s="4">
         <v>3</v>
@@ -9076,26 +9088,26 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="K96" s="4" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>43</v>
@@ -9112,28 +9124,28 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="K97" s="4" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>386</v>
@@ -9150,28 +9162,28 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="G98" s="29" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="H98" s="12" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="K98" s="4" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="L98" s="15" t="s">
         <v>386</v>
@@ -9188,25 +9200,25 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="G99" s="43" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="H99" s="43" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="I99" s="4" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="K99" s="4">
         <v>3</v>
@@ -9226,19 +9238,19 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="I100" s="48" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="J100" s="48" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="K100" s="48" t="s">
         <v>100</v>
@@ -9258,28 +9270,28 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="I101" s="11" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="J101" s="11" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="L101" s="15" t="s">
         <v>386</v>
@@ -9296,28 +9308,28 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="J102" s="11" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="L102" s="15" t="s">
         <v>386</v>
@@ -9334,25 +9346,25 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="J103" s="11" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="K103" s="11" t="s">
         <v>510</v>
@@ -9372,25 +9384,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="G104" s="11" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>182</v>
@@ -9410,25 +9422,25 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="H105" s="14" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="J105" s="11" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="K105" s="11" t="s">
         <v>211</v>
@@ -9448,25 +9460,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="H106" s="11" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="J106" s="11" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
@@ -9484,25 +9496,25 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="J107" s="11" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="K107" s="11" t="s">
         <v>167</v>
@@ -9522,25 +9534,25 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="H108" s="14" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="J108" s="11" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>182</v>
@@ -9560,22 +9572,22 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="H109" s="11" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>210</v>
@@ -9598,28 +9610,28 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="H110" s="10" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="J110" s="11" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="K110" s="11" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="L110" s="15" t="s">
         <v>43</v>
@@ -9636,28 +9648,28 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="G111" s="12" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="H111" s="14" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="J111" s="11" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="K111" s="11" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="L111" s="15" t="s">
         <v>386</v>
@@ -9674,25 +9686,25 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="J112" s="11" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>218</v>
@@ -9712,22 +9724,22 @@
         <v>112</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="G113" s="13" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>210</v>
@@ -9750,25 +9762,25 @@
         <v>113</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>67</v>
@@ -9887,6 +9899,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -10018,22 +10039,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10051,19 +10071,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to report template, KEV catalog import, phishing service dates, and JSON output
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB536CFB-D266-A340-BA9E-4D06548F8A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482EA1F3-4807-3D47-8F4F-D92EB26EEADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27020" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -717,9 +716,6 @@
     <t xml:space="preserve">System management establishes policies, standards, and procedures to protect and improve the information security (in this case wireless security) of the organization. Weak system management can result if the wireless network is not continuously monitored or managed by system administration, if wireless security procedures are not in place to protect all access points on the network, and if insecure default policies or configurations of wireless devices and security controls are used on the network. </t>
   </si>
   <si>
-    <t xml:space="preserve">Establish policies and procedures that identify organization's the wireless technology assets. Define measures for threat/risk mitigation. Set encryption standards. Check the effectiveness of the policies, controls, and procedures in place (e.g., audits and continuous monitoring). Ensure the system administrator manages and continuously improves the system based on the new risks or vulnerabilities identified to its wireless security. </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.researchgate.net/publication/228864040_Wireless_Network_Security_Vulnerabilities_Threats_and_Countermeasures https://www.myrasecurity.com/en/information-security-management-system-isms/ https://www.securitymetrics.com/blog/wireless-access-point-protection-finding-rogue-wi-fi-networks </t>
   </si>
   <si>
@@ -3240,6 +3236,9 @@
   </si>
   <si>
     <t>Microsoft has released security updates that mitigate this vulnerability which should be applied to the affected systems. Enable secure RPC enforcement mode, if feasible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Establish policies and procedures that identify the organization's wireless technology assets. Define measures for threat/risk mitigation. Set encryption standards. Check the effectiveness of the policies, controls, and procedures in place (e.g., audits and continuous monitoring). Ensure the system administrator manages and continuously improves the system based on the new risks or vulnerabilities identified to its wireless security. </t>
   </si>
 </sst>
 </file>
@@ -4542,7 +4541,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4577,7 +4576,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4612,7 +4611,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4648,7 +4647,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4686,7 +4685,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4722,7 +4721,7 @@
         <v>72</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>73</v>
@@ -4758,7 +4757,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4942,7 +4941,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -4978,7 +4977,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5402,22 +5401,22 @@
         <v>198</v>
       </c>
       <c r="F26" s="10" t="s">
+        <v>962</v>
+      </c>
+      <c r="G26" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="H26" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="I26" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="J26" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="K26" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>43</v>
@@ -5434,26 +5433,26 @@
         <v>26</v>
       </c>
       <c r="D27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="F27" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="G27" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>208</v>
       </c>
       <c r="H27" s="15"/>
       <c r="I27" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="K27" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>43</v>
@@ -5470,26 +5469,26 @@
         <v>27</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="G28" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="K28" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>218</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>43</v>
@@ -5557,10 +5556,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -5598,28 +5597,28 @@
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="15" t="s">
         <v>227</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>228</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>43</v>
@@ -5636,28 +5635,28 @@
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>54</v>
@@ -5674,28 +5673,28 @@
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>240</v>
-      </c>
       <c r="H4" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>54</v>
@@ -5712,28 +5711,28 @@
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="J5" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>247</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>248</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>43</v>
@@ -5750,22 +5749,22 @@
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>167</v>
@@ -5785,25 +5784,25 @@
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="I7" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="15" t="s">
         <v>260</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>261</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>54</v>
@@ -5820,28 +5819,28 @@
         <v>7</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="H8" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="H8" s="43" t="s">
-        <v>265</v>
-      </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>268</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>54</v>
@@ -5858,28 +5857,28 @@
         <v>8</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>54</v>
@@ -5896,28 +5895,28 @@
         <v>9</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="15" t="s">
         <v>281</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>282</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>54</v>
@@ -5934,28 +5933,28 @@
         <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="43" t="s">
         <v>285</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="H11" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="I11" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="15" t="s">
         <v>288</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>289</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>54</v>
@@ -5972,31 +5971,31 @@
         <v>11</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="44" t="s">
         <v>292</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="H12" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>293</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="J12" s="10" t="s">
+        <v>924</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>925</v>
-      </c>
-      <c r="K12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>295</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="340" x14ac:dyDescent="0.2">
@@ -6010,28 +6009,28 @@
         <v>12</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="J13" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="15" t="s">
         <v>303</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>304</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>43</v>
@@ -6048,28 +6047,28 @@
         <v>13</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="15" t="s">
         <v>310</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>311</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>54</v>
@@ -6086,25 +6085,25 @@
         <v>14</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>317</v>
-      </c>
       <c r="J15" s="10" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6124,28 +6123,28 @@
         <v>15</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="I16" s="15" t="s">
+      <c r="J16" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>323</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>324</v>
       </c>
       <c r="L16" s="15" t="s">
         <v>54</v>
@@ -6162,25 +6161,25 @@
         <v>16</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="11" t="s">
+        <v>926</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>329</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>927</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>330</v>
       </c>
       <c r="L17" s="15" t="s">
         <v>54</v>
@@ -6197,25 +6196,25 @@
         <v>17</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="H18" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="J18" s="11" t="s">
         <v>336</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>337</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>196</v>
@@ -6235,23 +6234,23 @@
         <v>18</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="14" t="s">
         <v>340</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>341</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
         <v>72</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K19" s="11" t="s">
         <v>73</v>
@@ -6271,25 +6270,25 @@
         <v>19</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>348</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>349</v>
       </c>
       <c r="K20" s="11" t="s">
         <v>167</v>
@@ -6309,28 +6308,28 @@
         <v>20</v>
       </c>
       <c r="D21" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="43" t="s">
         <v>352</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="H21" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="H21" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="I21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>355</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>356</v>
       </c>
       <c r="L21" s="15" t="s">
         <v>43</v>
@@ -6347,28 +6346,28 @@
         <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="G22" s="43" t="s">
+      <c r="H22" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="J22" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>363</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>364</v>
       </c>
       <c r="L22" s="15" t="s">
         <v>43</v>
@@ -6385,25 +6384,25 @@
         <v>22</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="F23" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="I23" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="J23" s="11" t="s">
         <v>370</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>371</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>73</v>
@@ -6423,28 +6422,28 @@
         <v>23</v>
       </c>
       <c r="D24" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H24" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="I24" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="J24" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>378</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>379</v>
       </c>
       <c r="L24" s="15" t="s">
         <v>54</v>
@@ -6461,31 +6460,31 @@
         <v>24</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="43" t="s">
         <v>382</v>
       </c>
-      <c r="G25" s="43" t="s">
+      <c r="H25" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>383</v>
       </c>
-      <c r="H25" s="43" t="s">
-        <v>383</v>
-      </c>
-      <c r="I25" s="15" t="s">
+      <c r="J25" s="11" t="s">
         <v>384</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>385</v>
       </c>
       <c r="K25" s="11">
         <v>7</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="153" x14ac:dyDescent="0.2">
@@ -6499,28 +6498,28 @@
         <v>25</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="G26" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="H26" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="I26" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>393</v>
-      </c>
       <c r="K26" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L26" s="15" t="s">
         <v>43</v>
@@ -6537,28 +6536,28 @@
         <v>26</v>
       </c>
       <c r="D27" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="H27" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="I27" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>399</v>
-      </c>
       <c r="J27" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L27" s="15" t="s">
         <v>43</v>
@@ -6575,28 +6574,28 @@
         <v>27</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="H28" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>404</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L28" s="15" t="s">
         <v>43</v>
@@ -6613,24 +6612,24 @@
         <v>28</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>407</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L29" s="15" t="s">
         <v>43</v>
@@ -6647,20 +6646,20 @@
         <v>29</v>
       </c>
       <c r="D30" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="45" t="s">
         <v>409</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="G30" s="14" t="s">
         <v>410</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>411</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>99</v>
@@ -6683,28 +6682,28 @@
         <v>30</v>
       </c>
       <c r="D31" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="F31" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="G31" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="I31" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="L31" s="15" t="s">
         <v>54</v>
@@ -6721,28 +6720,28 @@
         <v>31</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>945</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>946</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>947</v>
-      </c>
-      <c r="G32" s="13" t="s">
+      <c r="H32" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="I32" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="J32" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>425</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>426</v>
       </c>
       <c r="L32" s="15" t="s">
         <v>54</v>
@@ -6759,20 +6758,20 @@
         <v>32</v>
       </c>
       <c r="D33" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>947</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>948</v>
+      </c>
+      <c r="G33" s="13" t="s">
         <v>427</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>948</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>949</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>428</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>106</v>
@@ -6795,20 +6794,20 @@
         <v>33</v>
       </c>
       <c r="D34" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>949</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>950</v>
-      </c>
-      <c r="F34" s="10" t="s">
+      <c r="G34" s="13" t="s">
         <v>431</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>432</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>106</v>
@@ -6831,20 +6830,20 @@
         <v>34</v>
       </c>
       <c r="D35" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="G35" s="13" t="s">
         <v>435</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>436</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>106</v>
@@ -6867,25 +6866,25 @@
         <v>35</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="F36" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="G36" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="I36" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="L36" s="15" t="s">
         <v>43</v>
@@ -6902,31 +6901,31 @@
         <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="G37" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="H37" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="I37" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>449</v>
-      </c>
       <c r="J37" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="K37" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="L37" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="356" x14ac:dyDescent="0.2">
@@ -6940,25 +6939,25 @@
         <v>37</v>
       </c>
       <c r="D38" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="H38" s="10" t="s">
-        <v>453</v>
-      </c>
       <c r="I38" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J38" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="L38" s="15" t="s">
         <v>43</v>
@@ -6975,25 +6974,25 @@
         <v>38</v>
       </c>
       <c r="D39" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="F39" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="G39" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="I39" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>460</v>
       </c>
       <c r="L39" s="15" t="s">
         <v>43</v>
@@ -7010,25 +7009,25 @@
         <v>39</v>
       </c>
       <c r="D40" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="G40" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="I40" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="J40" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>466</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>467</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>43</v>
@@ -7045,25 +7044,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="F41" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="G41" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="H41" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="I41" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>473</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>474</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>196</v>
@@ -7083,28 +7082,28 @@
         <v>41</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="F42" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="G42" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="H42" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="I42" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>482</v>
       </c>
       <c r="L42" s="15" t="s">
         <v>54</v>
@@ -7121,31 +7120,31 @@
         <v>42</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="H43" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="I43" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>490</v>
-      </c>
       <c r="L43" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="255" x14ac:dyDescent="0.2">
@@ -7159,28 +7158,28 @@
         <v>43</v>
       </c>
       <c r="D44" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="F44" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="G44" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="H44" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="I44" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="J44" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>497</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>498</v>
       </c>
       <c r="L44" s="15" t="s">
         <v>43</v>
@@ -7197,25 +7196,25 @@
         <v>44</v>
       </c>
       <c r="D45" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="F45" s="11" t="s">
         <v>500</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="G45" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="I45" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>504</v>
-      </c>
       <c r="J45" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>73</v>
@@ -7235,26 +7234,26 @@
         <v>45</v>
       </c>
       <c r="D46" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>505</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="F46" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="G46" s="12" t="s">
         <v>507</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>508</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="K46" s="4" t="s">
         <v>509</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>510</v>
       </c>
       <c r="L46" s="15" t="s">
         <v>43</v>
@@ -7271,28 +7270,28 @@
         <v>46</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="F47" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="G47" s="29" t="s">
         <v>513</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="H47" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="I47" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>517</v>
-      </c>
       <c r="K47" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L47" s="15" t="s">
         <v>43</v>
@@ -7309,26 +7308,26 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>941</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>942</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>943</v>
       </c>
-      <c r="F48" s="11" t="s">
-        <v>944</v>
-      </c>
       <c r="G48" s="29" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="J48" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>939</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>940</v>
       </c>
       <c r="L48" s="15" t="s">
         <v>54</v>
@@ -7345,29 +7344,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>930</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>944</v>
+      </c>
+      <c r="G49" s="29" t="s">
         <v>931</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>934</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>945</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>932</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="221" x14ac:dyDescent="0.2">
@@ -7381,26 +7380,26 @@
         <v>49</v>
       </c>
       <c r="D50" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>518</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="G50" s="29" t="s">
         <v>520</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>521</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L50" s="15" t="s">
         <v>43</v>
@@ -7417,26 +7416,26 @@
         <v>50</v>
       </c>
       <c r="D51" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>524</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="G51" s="29" t="s">
         <v>525</v>
-      </c>
-      <c r="G51" s="29" t="s">
-        <v>526</v>
       </c>
       <c r="H51" s="29"/>
       <c r="I51" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>528</v>
       </c>
       <c r="L51" s="15" t="s">
         <v>43</v>
@@ -7453,26 +7452,26 @@
         <v>51</v>
       </c>
       <c r="D52" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="F52" s="10" t="s">
         <v>530</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="G52" s="29" t="s">
         <v>531</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>532</v>
       </c>
       <c r="H52" s="29"/>
       <c r="I52" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="J52" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="K52" s="4" t="s">
         <v>534</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>535</v>
       </c>
       <c r="L52" s="15" t="s">
         <v>43</v>
@@ -7489,28 +7488,28 @@
         <v>52</v>
       </c>
       <c r="D53" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>536</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="F53" s="11" t="s">
+        <v>950</v>
+      </c>
+      <c r="G53" s="43" t="s">
         <v>537</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>951</v>
-      </c>
-      <c r="G53" s="43" t="s">
+      <c r="H53" s="43" t="s">
+        <v>537</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="H53" s="43" t="s">
-        <v>538</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="L53" s="15" t="s">
         <v>54</v>
@@ -7527,28 +7526,28 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>542</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>543</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G54" s="43" t="s">
+        <v>537</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>537</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="H54" s="43" t="s">
-        <v>538</v>
-      </c>
-      <c r="I54" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="L54" s="15" t="s">
         <v>54</v>
@@ -7565,28 +7564,28 @@
         <v>54</v>
       </c>
       <c r="D55" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>545</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="G55" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="G55" s="43" t="s">
-        <v>547</v>
-      </c>
       <c r="H55" s="43" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I55" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="K55" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="L55" s="15" t="s">
         <v>54</v>
@@ -7603,28 +7602,28 @@
         <v>55</v>
       </c>
       <c r="D56" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="F56" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="G56" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="H56" s="12" t="s">
         <v>551</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="I56" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="J56" s="4" t="s">
-        <v>554</v>
-      </c>
       <c r="K56" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L56" s="15" t="s">
         <v>54</v>
@@ -7641,24 +7640,24 @@
         <v>56</v>
       </c>
       <c r="D57" s="10" t="s">
+        <v>554</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>555</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="F57" s="10" t="s">
         <v>556</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>557</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="J57" s="4" t="s">
-        <v>554</v>
-      </c>
       <c r="K57" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L57" s="15" t="s">
         <v>54</v>
@@ -7675,28 +7674,28 @@
         <v>57</v>
       </c>
       <c r="D58" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="E58" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="F58" s="10" t="s">
+        <v>954</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>955</v>
-      </c>
-      <c r="G58" s="10" t="s">
+      <c r="H58" s="14" t="s">
         <v>560</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="I58" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>564</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>54</v>
@@ -7713,28 +7712,28 @@
         <v>58</v>
       </c>
       <c r="D59" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="F59" s="11" t="s">
+        <v>955</v>
+      </c>
+      <c r="G59" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="F59" s="11" t="s">
-        <v>956</v>
-      </c>
-      <c r="G59" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>567</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="I59" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="J59" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="J59" s="4" t="s">
-        <v>570</v>
-      </c>
       <c r="K59" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L59" s="15" t="s">
         <v>43</v>
@@ -7751,28 +7750,28 @@
         <v>59</v>
       </c>
       <c r="D60" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="F60" s="10" t="s">
+        <v>952</v>
+      </c>
+      <c r="G60" s="14" t="s">
         <v>572</v>
       </c>
-      <c r="F60" s="10" t="s">
-        <v>953</v>
-      </c>
-      <c r="G60" s="14" t="s">
+      <c r="H60" s="14" t="s">
         <v>573</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="I60" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="J60" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>577</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>54</v>
@@ -7789,28 +7788,28 @@
         <v>60</v>
       </c>
       <c r="D61" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="F61" s="10" t="s">
+        <v>956</v>
+      </c>
+      <c r="G61" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="F61" s="10" t="s">
-        <v>957</v>
-      </c>
-      <c r="G61" s="16" t="s">
+      <c r="H61" s="14" t="s">
         <v>580</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="I61" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>584</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>54</v>
@@ -7827,28 +7826,28 @@
         <v>61</v>
       </c>
       <c r="D62" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>585</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="F62" s="10" t="s">
+        <v>957</v>
+      </c>
+      <c r="G62" s="14" t="s">
         <v>586</v>
       </c>
-      <c r="F62" s="10" t="s">
-        <v>958</v>
-      </c>
-      <c r="G62" s="14" t="s">
+      <c r="H62" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="H62" s="14" t="s">
+      <c r="I62" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="K62" s="4" t="s">
         <v>590</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>591</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>54</v>
@@ -7865,28 +7864,28 @@
         <v>62</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="E63" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="F63" s="10" t="s">
+        <v>953</v>
+      </c>
+      <c r="G63" s="14" t="s">
         <v>593</v>
       </c>
-      <c r="F63" s="10" t="s">
-        <v>954</v>
-      </c>
-      <c r="G63" s="14" t="s">
+      <c r="H63" s="14" t="s">
         <v>594</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="I63" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>597</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>598</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>54</v>
@@ -7903,26 +7902,26 @@
         <v>63</v>
       </c>
       <c r="D64" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E64" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="F64" s="10" t="s">
+        <v>958</v>
+      </c>
+      <c r="G64" s="14" t="s">
         <v>600</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>959</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>601</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>603</v>
-      </c>
       <c r="K64" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>54</v>
@@ -7939,28 +7938,28 @@
         <v>64</v>
       </c>
       <c r="D65" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="E65" s="10" t="s">
         <v>604</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="F65" s="10" t="s">
+        <v>959</v>
+      </c>
+      <c r="G65" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="F65" s="10" t="s">
-        <v>960</v>
-      </c>
-      <c r="G65" s="14" t="s">
+      <c r="H65" s="12" t="s">
         <v>606</v>
       </c>
-      <c r="H65" s="12" t="s">
+      <c r="I65" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="J65" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="K65" s="4" t="s">
         <v>609</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>610</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>54</v>
@@ -7977,28 +7976,28 @@
         <v>65</v>
       </c>
       <c r="D66" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="E66" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="F66" s="10" t="s">
+        <v>959</v>
+      </c>
+      <c r="G66" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="F66" s="10" t="s">
-        <v>960</v>
-      </c>
-      <c r="G66" s="10" t="s">
+      <c r="H66" s="14" t="s">
         <v>613</v>
       </c>
-      <c r="H66" s="14" t="s">
+      <c r="I66" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="I66" s="4" t="s">
-        <v>615</v>
-      </c>
       <c r="J66" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="K66" s="4" t="s">
         <v>609</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>610</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>54</v>
@@ -8015,28 +8014,28 @@
         <v>66</v>
       </c>
       <c r="D67" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="E67" s="10" t="s">
         <v>616</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="10" t="s">
+        <v>960</v>
+      </c>
+      <c r="G67" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="F67" s="10" t="s">
-        <v>961</v>
-      </c>
-      <c r="G67" s="14" t="s">
+      <c r="H67" s="14" t="s">
         <v>618</v>
       </c>
-      <c r="H67" s="14" t="s">
+      <c r="I67" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="I67" s="4" t="s">
-        <v>620</v>
-      </c>
       <c r="J67" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="K67" s="4" t="s">
         <v>597</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>598</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>54</v>
@@ -8053,31 +8052,31 @@
         <v>67</v>
       </c>
       <c r="D68" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="E68" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="F68" s="10" t="s">
+        <v>961</v>
+      </c>
+      <c r="G68" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="F68" s="10" t="s">
-        <v>962</v>
-      </c>
-      <c r="G68" s="10" t="s">
+      <c r="H68" s="14" t="s">
         <v>623</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="I68" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="I68" s="4" t="s">
+      <c r="J68" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>626</v>
       </c>
       <c r="K68" s="4">
         <v>7</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="255" x14ac:dyDescent="0.2">
@@ -8091,20 +8090,20 @@
         <v>68</v>
       </c>
       <c r="D69" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>628</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="F69" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="G69" s="10" t="s">
         <v>630</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>631</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>145</v>
@@ -8127,20 +8126,20 @@
         <v>69</v>
       </c>
       <c r="D70" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="F70" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="G70" s="10" t="s">
         <v>635</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>636</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>145</v>
@@ -8163,20 +8162,20 @@
         <v>70</v>
       </c>
       <c r="D71" s="10" t="s">
+        <v>636</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="F71" s="10" t="s">
         <v>638</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="G71" s="14" t="s">
         <v>639</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>640</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>145</v>
@@ -8199,25 +8198,25 @@
         <v>71</v>
       </c>
       <c r="D72" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="E72" s="11" t="s">
         <v>641</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>643</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="H72" s="43" t="s">
+        <v>643</v>
+      </c>
+      <c r="I72" s="11" t="s">
         <v>644</v>
       </c>
-      <c r="H72" s="43" t="s">
-        <v>644</v>
-      </c>
-      <c r="I72" s="11" t="s">
+      <c r="J72" s="11" t="s">
         <v>645</v>
-      </c>
-      <c r="J72" s="11" t="s">
-        <v>646</v>
       </c>
       <c r="K72" s="11">
         <v>16</v>
@@ -8237,31 +8236,31 @@
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
+        <v>646</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>647</v>
       </c>
-      <c r="E73" s="11" t="s">
+      <c r="F73" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>649</v>
       </c>
-      <c r="G73" s="11" t="s">
-        <v>650</v>
-      </c>
       <c r="H73" s="43" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I73" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="J73" s="11" t="s">
         <v>645</v>
-      </c>
-      <c r="J73" s="11" t="s">
-        <v>646</v>
       </c>
       <c r="K73" s="11">
         <v>16</v>
       </c>
       <c r="L73" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="136" x14ac:dyDescent="0.2">
@@ -8275,26 +8274,26 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
+        <v>650</v>
+      </c>
+      <c r="E74" s="11" t="s">
         <v>651</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="F74" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="G74" s="11" t="s">
         <v>653</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>654</v>
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>655</v>
       </c>
-      <c r="J74" s="11" t="s">
-        <v>656</v>
-      </c>
       <c r="K74" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L74" s="15" t="s">
         <v>43</v>
@@ -8311,28 +8310,28 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>657</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="F75" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="G75" s="14" t="s">
         <v>659</v>
       </c>
-      <c r="G75" s="14" t="s">
+      <c r="H75" s="14" t="s">
         <v>660</v>
       </c>
-      <c r="H75" s="14" t="s">
+      <c r="I75" s="10" t="s">
         <v>661</v>
       </c>
-      <c r="I75" s="10" t="s">
+      <c r="J75" s="10" t="s">
+        <v>927</v>
+      </c>
+      <c r="K75" s="10" t="s">
         <v>662</v>
-      </c>
-      <c r="J75" s="10" t="s">
-        <v>928</v>
-      </c>
-      <c r="K75" s="10" t="s">
-        <v>663</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
@@ -8349,26 +8348,26 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>664</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="F76" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="G76" s="14" t="s">
         <v>666</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>667</v>
       </c>
       <c r="H76" s="14"/>
       <c r="I76" s="10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L76" s="15" t="s">
         <v>43</v>
@@ -8385,28 +8384,28 @@
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>669</v>
       </c>
-      <c r="E77" s="11" t="s">
+      <c r="F77" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="G77" s="11" t="s">
         <v>671</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="H77" s="43" t="s">
+        <v>671</v>
+      </c>
+      <c r="I77" s="11" t="s">
         <v>672</v>
       </c>
-      <c r="H77" s="43" t="s">
-        <v>672</v>
-      </c>
-      <c r="I77" s="11" t="s">
+      <c r="J77" s="11" t="s">
         <v>673</v>
       </c>
-      <c r="J77" s="11" t="s">
-        <v>674</v>
-      </c>
       <c r="K77" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L77" s="15" t="s">
         <v>43</v>
@@ -8423,23 +8422,23 @@
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>675</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="F78" s="11" t="s">
         <v>676</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>677</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
+        <v>677</v>
+      </c>
+      <c r="I78" s="11" t="s">
         <v>678</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="J78" s="11" t="s">
         <v>679</v>
-      </c>
-      <c r="J78" s="11" t="s">
-        <v>680</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>73</v>
@@ -8450,7 +8449,7 @@
     </row>
     <row r="79" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8459,25 +8458,25 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="F79" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="H79" s="43" t="s">
+        <v>684</v>
+      </c>
+      <c r="I79" s="11" t="s">
         <v>685</v>
       </c>
-      <c r="H79" s="43" t="s">
-        <v>685</v>
-      </c>
-      <c r="I79" s="11" t="s">
+      <c r="J79" s="11" t="s">
         <v>686</v>
-      </c>
-      <c r="J79" s="11" t="s">
-        <v>687</v>
       </c>
       <c r="K79" s="11">
         <v>16</v>
@@ -8488,7 +8487,7 @@
     </row>
     <row r="80" spans="1:12" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8497,19 +8496,19 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="F80" s="11" t="s">
         <v>689</v>
       </c>
-      <c r="F80" s="11" t="s">
+      <c r="G80" s="43" t="s">
         <v>690</v>
       </c>
-      <c r="G80" s="43" t="s">
-        <v>691</v>
-      </c>
       <c r="H80" s="43" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>172</v>
@@ -8518,7 +8517,7 @@
         <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
@@ -8526,7 +8525,7 @@
     </row>
     <row r="81" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8535,25 +8534,25 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
+        <v>692</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="F81" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="G81" s="43" t="s">
         <v>695</v>
       </c>
-      <c r="G81" s="43" t="s">
+      <c r="H81" s="43" t="s">
         <v>696</v>
       </c>
-      <c r="H81" s="43" t="s">
+      <c r="I81" s="11" t="s">
         <v>697</v>
       </c>
-      <c r="I81" s="11" t="s">
+      <c r="J81" s="11" t="s">
         <v>698</v>
-      </c>
-      <c r="J81" s="11" t="s">
-        <v>699</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>182</v>
@@ -8564,7 +8563,7 @@
     </row>
     <row r="82" spans="1:12" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8573,28 +8572,28 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="F82" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="G82" s="10" t="s">
         <v>702</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="H82" s="14" t="s">
         <v>703</v>
       </c>
-      <c r="H82" s="14" t="s">
+      <c r="I82" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="10" t="s">
         <v>705</v>
       </c>
-      <c r="J82" s="10" t="s">
-        <v>706</v>
-      </c>
       <c r="K82" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>43</v>
@@ -8602,7 +8601,7 @@
     </row>
     <row r="83" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B83" s="10">
         <v>20</v>
@@ -8611,23 +8610,23 @@
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="E83" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="F83" s="10" t="s">
         <v>708</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="G83" s="10" t="s">
         <v>709</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>710</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>698</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>699</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>182</v>
@@ -8638,7 +8637,7 @@
     </row>
     <row r="84" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B84" s="10">
         <v>20</v>
@@ -8647,26 +8646,26 @@
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>711</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="F84" s="10" t="s">
         <v>712</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="G84" s="10" t="s">
         <v>713</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>714</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>43</v>
@@ -8683,25 +8682,25 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="E85" s="46" t="s">
         <v>716</v>
       </c>
-      <c r="E85" s="46" t="s">
+      <c r="F85" s="11" t="s">
         <v>717</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="G85" s="43" t="s">
         <v>718</v>
       </c>
-      <c r="G85" s="43" t="s">
+      <c r="H85" s="43" t="s">
+        <v>718</v>
+      </c>
+      <c r="I85" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="H85" s="43" t="s">
-        <v>719</v>
-      </c>
-      <c r="I85" s="4" t="s">
+      <c r="J85" s="4" t="s">
         <v>720</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>721</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>49</v>
@@ -8721,29 +8720,29 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="E86" s="46" t="s">
         <v>722</v>
       </c>
-      <c r="E86" s="46" t="s">
+      <c r="F86" s="46" t="s">
         <v>723</v>
       </c>
-      <c r="F86" s="46" t="s">
+      <c r="G86" s="10" t="s">
         <v>724</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>725</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>726</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>727</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="221" x14ac:dyDescent="0.2">
@@ -8757,31 +8756,31 @@
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>728</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="F87" s="46" t="s">
         <v>729</v>
       </c>
-      <c r="F87" s="46" t="s">
+      <c r="G87" s="29" t="s">
         <v>730</v>
       </c>
-      <c r="G87" s="29" t="s">
+      <c r="H87" s="12" t="s">
         <v>731</v>
       </c>
-      <c r="H87" s="12" t="s">
-        <v>732</v>
-      </c>
       <c r="I87" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>726</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>727</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="187" x14ac:dyDescent="0.2">
@@ -8795,28 +8794,28 @@
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
+        <v>732</v>
+      </c>
+      <c r="E88" s="46" t="s">
         <v>733</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="F88" s="46" t="s">
         <v>734</v>
       </c>
-      <c r="F88" s="46" t="s">
+      <c r="G88" s="43" t="s">
         <v>735</v>
       </c>
-      <c r="G88" s="43" t="s">
+      <c r="H88" s="43" t="s">
+        <v>735</v>
+      </c>
+      <c r="I88" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="H88" s="43" t="s">
-        <v>736</v>
-      </c>
-      <c r="I88" s="4" t="s">
+      <c r="J88" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="J88" s="4" t="s">
+      <c r="K88" s="4" t="s">
         <v>738</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>739</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
@@ -8833,28 +8832,28 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="E89" s="46" t="s">
         <v>740</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="F89" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="G89" s="29" t="s">
         <v>742</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="H89" s="12" t="s">
         <v>743</v>
       </c>
-      <c r="H89" s="12" t="s">
+      <c r="I89" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="J89" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="J89" s="4" t="s">
-        <v>746</v>
-      </c>
       <c r="K89" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L89" s="15" t="s">
         <v>43</v>
@@ -8871,26 +8870,26 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
+        <v>746</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>747</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>748</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="G90" s="16" t="s">
         <v>749</v>
-      </c>
-      <c r="G90" s="16" t="s">
-        <v>750</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>752</v>
-      </c>
-      <c r="K90" s="4" t="s">
-        <v>753</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
@@ -8907,26 +8906,26 @@
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="E91" s="11" t="s">
         <v>754</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="F91" s="11" t="s">
         <v>755</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="G91" s="29" t="s">
         <v>756</v>
-      </c>
-      <c r="G91" s="29" t="s">
-        <v>757</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="K91" s="4" t="s">
         <v>752</v>
-      </c>
-      <c r="K91" s="4" t="s">
-        <v>753</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
@@ -8943,25 +8942,25 @@
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
+        <v>757</v>
+      </c>
+      <c r="E92" s="11" t="s">
         <v>758</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="F92" s="10" t="s">
         <v>759</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="G92" s="10" t="s">
         <v>760</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="I92" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>763</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>764</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>43</v>
@@ -8978,26 +8977,26 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>765</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="F93" s="10" t="s">
         <v>766</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="G93" s="14" t="s">
         <v>767</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>768</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="J93" s="4" t="s">
+      <c r="K93" s="4" t="s">
         <v>770</v>
-      </c>
-      <c r="K93" s="4" t="s">
-        <v>771</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
@@ -9014,28 +9013,28 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="E94" s="10" t="s">
         <v>772</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="10" t="s">
         <v>773</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="G94" s="12" t="s">
         <v>774</v>
       </c>
-      <c r="G94" s="12" t="s">
+      <c r="H94" s="14" t="s">
         <v>775</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="I94" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="J94" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="J94" s="4" t="s">
+      <c r="K94" s="48" t="s">
         <v>778</v>
-      </c>
-      <c r="K94" s="48" t="s">
-        <v>779</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>54</v>
@@ -9052,23 +9051,23 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>780</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="F95" s="11" t="s">
         <v>781</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="G95" s="29" t="s">
         <v>782</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>783</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>784</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>785</v>
       </c>
       <c r="K95" s="4">
         <v>3</v>
@@ -9088,26 +9087,26 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>786</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="F96" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="G96" s="10" t="s">
         <v>788</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>789</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="K96" s="4" t="s">
         <v>791</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>792</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>43</v>
@@ -9124,31 +9123,31 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="E97" s="10" t="s">
         <v>793</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="F97" s="10" t="s">
         <v>794</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="G97" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="G97" s="10" t="s">
+      <c r="H97" s="10" t="s">
         <v>796</v>
       </c>
-      <c r="H97" s="10" t="s">
+      <c r="I97" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="J97" s="4" t="s">
         <v>798</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="K97" s="4" t="s">
         <v>799</v>
       </c>
-      <c r="K97" s="4" t="s">
-        <v>800</v>
-      </c>
       <c r="L97" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="388" x14ac:dyDescent="0.2">
@@ -9162,31 +9161,31 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>801</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="F98" s="11" t="s">
         <v>802</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="G98" s="29" t="s">
         <v>803</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="H98" s="12" t="s">
         <v>804</v>
       </c>
-      <c r="H98" s="12" t="s">
+      <c r="I98" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="J98" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="K98" s="4" t="s">
         <v>807</v>
       </c>
-      <c r="K98" s="4" t="s">
-        <v>808</v>
-      </c>
       <c r="L98" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="136" x14ac:dyDescent="0.2">
@@ -9200,25 +9199,25 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>809</v>
       </c>
-      <c r="E99" s="11" t="s">
+      <c r="F99" s="11" t="s">
         <v>810</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="G99" s="43" t="s">
         <v>811</v>
       </c>
-      <c r="G99" s="43" t="s">
+      <c r="H99" s="43" t="s">
+        <v>811</v>
+      </c>
+      <c r="I99" s="4" t="s">
         <v>812</v>
       </c>
-      <c r="H99" s="43" t="s">
-        <v>812</v>
-      </c>
-      <c r="I99" s="4" t="s">
+      <c r="J99" s="4" t="s">
         <v>813</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>814</v>
       </c>
       <c r="K99" s="4">
         <v>3</v>
@@ -9238,19 +9237,19 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="E100" s="10" t="s">
         <v>815</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="F100" s="10" t="s">
         <v>816</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="I100" s="48" t="s">
         <v>817</v>
       </c>
-      <c r="I100" s="48" t="s">
+      <c r="J100" s="48" t="s">
         <v>818</v>
-      </c>
-      <c r="J100" s="48" t="s">
-        <v>819</v>
       </c>
       <c r="K100" s="48" t="s">
         <v>100</v>
@@ -9270,31 +9269,31 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>820</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="F101" s="11" t="s">
         <v>821</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="10" t="s">
         <v>822</v>
       </c>
-      <c r="G101" s="10" t="s">
+      <c r="H101" s="10" t="s">
         <v>823</v>
       </c>
-      <c r="H101" s="10" t="s">
+      <c r="I101" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="I101" s="11" t="s">
+      <c r="J101" s="11" t="s">
+        <v>929</v>
+      </c>
+      <c r="K101" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="J101" s="11" t="s">
-        <v>930</v>
-      </c>
-      <c r="K101" s="11" t="s">
-        <v>826</v>
-      </c>
       <c r="L101" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="187" x14ac:dyDescent="0.2">
@@ -9308,31 +9307,31 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="E102" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="E102" s="11" t="s">
+      <c r="F102" s="11" t="s">
         <v>828</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="G102" s="10" t="s">
         <v>829</v>
       </c>
-      <c r="G102" s="10" t="s">
+      <c r="H102" s="11" t="s">
         <v>830</v>
       </c>
-      <c r="H102" s="11" t="s">
+      <c r="I102" s="11" t="s">
         <v>831</v>
       </c>
-      <c r="I102" s="11" t="s">
+      <c r="J102" s="11" t="s">
         <v>832</v>
       </c>
-      <c r="J102" s="11" t="s">
+      <c r="K102" s="11" t="s">
         <v>833</v>
       </c>
-      <c r="K102" s="11" t="s">
-        <v>834</v>
-      </c>
       <c r="L102" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="204" x14ac:dyDescent="0.2">
@@ -9346,28 +9345,28 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="E103" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>836</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="G103" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>838</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="I103" s="11" t="s">
         <v>839</v>
       </c>
-      <c r="I103" s="11" t="s">
+      <c r="J103" s="11" t="s">
         <v>840</v>
       </c>
-      <c r="J103" s="11" t="s">
-        <v>841</v>
-      </c>
       <c r="K103" s="11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L103" s="15" t="s">
         <v>43</v>
@@ -9384,25 +9383,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="E104" s="11" t="s">
         <v>842</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="F104" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="G104" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="G104" s="11" t="s">
+      <c r="H104" s="11" t="s">
         <v>845</v>
       </c>
-      <c r="H104" s="11" t="s">
+      <c r="I104" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="I104" s="11" t="s">
+      <c r="J104" s="11" t="s">
         <v>847</v>
-      </c>
-      <c r="J104" s="11" t="s">
-        <v>848</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>182</v>
@@ -9422,28 +9421,28 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="E105" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="F105" s="11" t="s">
         <v>850</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="G105" s="10" t="s">
         <v>851</v>
       </c>
-      <c r="G105" s="10" t="s">
+      <c r="H105" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H105" s="14" t="s">
+      <c r="I105" s="11" t="s">
         <v>853</v>
       </c>
-      <c r="I105" s="11" t="s">
+      <c r="J105" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="J105" s="11" t="s">
-        <v>855</v>
-      </c>
       <c r="K105" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L105" s="15" t="s">
         <v>43</v>
@@ -9460,25 +9459,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>856</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="F106" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="G106" s="10" t="s">
         <v>858</v>
       </c>
-      <c r="G106" s="10" t="s">
+      <c r="H106" s="11" t="s">
         <v>859</v>
       </c>
-      <c r="H106" s="11" t="s">
+      <c r="I106" s="11" t="s">
         <v>860</v>
       </c>
-      <c r="I106" s="11" t="s">
+      <c r="J106" s="11" t="s">
         <v>861</v>
-      </c>
-      <c r="J106" s="11" t="s">
-        <v>862</v>
       </c>
       <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
@@ -9496,25 +9495,25 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
+        <v>862</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>863</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="F107" s="11" t="s">
         <v>864</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="G107" s="10" t="s">
         <v>865</v>
       </c>
-      <c r="G107" s="10" t="s">
+      <c r="H107" s="10" t="s">
         <v>866</v>
       </c>
-      <c r="H107" s="10" t="s">
+      <c r="I107" s="11" t="s">
         <v>867</v>
       </c>
-      <c r="I107" s="11" t="s">
+      <c r="J107" s="11" t="s">
         <v>868</v>
-      </c>
-      <c r="J107" s="11" t="s">
-        <v>869</v>
       </c>
       <c r="K107" s="11" t="s">
         <v>167</v>
@@ -9525,7 +9524,7 @@
     </row>
     <row r="108" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B108" s="10">
         <v>26</v>
@@ -9534,25 +9533,25 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
+        <v>869</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>870</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="F108" s="11" t="s">
         <v>871</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="G108" s="10" t="s">
         <v>872</v>
       </c>
-      <c r="G108" s="10" t="s">
+      <c r="H108" s="14" t="s">
         <v>873</v>
       </c>
-      <c r="H108" s="14" t="s">
+      <c r="I108" s="11" t="s">
         <v>874</v>
       </c>
-      <c r="I108" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>875</v>
-      </c>
-      <c r="J108" s="11" t="s">
-        <v>876</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>182</v>
@@ -9563,7 +9562,7 @@
     </row>
     <row r="109" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B109" s="10">
         <v>26</v>
@@ -9572,28 +9571,28 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
+        <v>876</v>
+      </c>
+      <c r="E109" s="11" t="s">
         <v>877</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="F109" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="G109" s="10" t="s">
         <v>879</v>
       </c>
-      <c r="G109" s="10" t="s">
+      <c r="H109" s="11" t="s">
         <v>880</v>
       </c>
-      <c r="H109" s="11" t="s">
+      <c r="I109" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="I109" s="11" t="s">
-        <v>882</v>
-      </c>
       <c r="J109" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="K109" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="K109" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="L109" s="15" t="s">
         <v>43</v>
@@ -9601,7 +9600,7 @@
     </row>
     <row r="110" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B110" s="10">
         <v>26</v>
@@ -9610,28 +9609,28 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
+        <v>882</v>
+      </c>
+      <c r="E110" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="F110" s="11" t="s">
         <v>884</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="G110" s="10" t="s">
         <v>885</v>
       </c>
-      <c r="G110" s="10" t="s">
+      <c r="H110" s="10" t="s">
         <v>886</v>
       </c>
-      <c r="H110" s="10" t="s">
+      <c r="I110" s="11" t="s">
         <v>887</v>
       </c>
-      <c r="I110" s="11" t="s">
+      <c r="J110" s="11" t="s">
         <v>888</v>
       </c>
-      <c r="J110" s="11" t="s">
+      <c r="K110" s="11" t="s">
         <v>889</v>
-      </c>
-      <c r="K110" s="11" t="s">
-        <v>890</v>
       </c>
       <c r="L110" s="15" t="s">
         <v>43</v>
@@ -9639,7 +9638,7 @@
     </row>
     <row r="111" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B111" s="10">
         <v>27</v>
@@ -9648,36 +9647,36 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>890</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>891</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="F111" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="F111" s="11" t="s">
+      <c r="G111" s="12" t="s">
         <v>893</v>
       </c>
-      <c r="G111" s="12" t="s">
+      <c r="H111" s="14" t="s">
+        <v>852</v>
+      </c>
+      <c r="I111" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="H111" s="14" t="s">
-        <v>853</v>
-      </c>
-      <c r="I111" s="11" t="s">
+      <c r="J111" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="J111" s="11" t="s">
+      <c r="K111" s="11" t="s">
         <v>896</v>
       </c>
-      <c r="K111" s="11" t="s">
-        <v>897</v>
-      </c>
       <c r="L111" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B112" s="10">
         <v>27</v>
@@ -9686,28 +9685,28 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="F112" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="G112" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="14" t="s">
         <v>901</v>
       </c>
-      <c r="H112" s="14" t="s">
+      <c r="I112" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="I112" s="11" t="s">
+      <c r="J112" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="J112" s="11" t="s">
-        <v>904</v>
-      </c>
       <c r="K112" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L112" s="15" t="s">
         <v>54</v>
@@ -9715,7 +9714,7 @@
     </row>
     <row r="113" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B113" s="10">
         <v>27</v>
@@ -9724,28 +9723,28 @@
         <v>112</v>
       </c>
       <c r="D113" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>905</v>
       </c>
-      <c r="E113" s="11" t="s">
+      <c r="F113" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="F113" s="11" t="s">
+      <c r="G113" s="13" t="s">
         <v>907</v>
       </c>
-      <c r="G113" s="13" t="s">
+      <c r="H113" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="H113" s="11" t="s">
+      <c r="I113" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="I113" s="11" t="s">
-        <v>910</v>
-      </c>
       <c r="J113" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="K113" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="K113" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="L113" s="15" t="s">
         <v>43</v>
@@ -9753,7 +9752,7 @@
     </row>
     <row r="114" spans="1:12" ht="238" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B114" s="10">
         <v>27</v>
@@ -9762,31 +9761,31 @@
         <v>113</v>
       </c>
       <c r="D114" s="10" t="s">
+        <v>910</v>
+      </c>
+      <c r="E114" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="F114" s="11" t="s">
         <v>912</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="G114" s="11" t="s">
+      <c r="H114" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="H114" s="11" t="s">
+      <c r="I114" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="I114" s="11" t="s">
+      <c r="J114" s="11" t="s">
         <v>916</v>
-      </c>
-      <c r="J114" s="11" t="s">
-        <v>917</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>67</v>
       </c>
       <c r="L114" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9899,12 +9898,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10040,15 +10036,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10072,10 +10072,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to risk scoring terminology and placeholders
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482EA1F3-4807-3D47-8F4F-D92EB26EEADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7198A9-CF94-3B43-9B36-899121BC3293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27020" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="16380" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="964">
   <si>
     <t>Finding_Category_ID</t>
   </si>
@@ -3239,6 +3239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Establish policies and procedures that identify the organization's wireless technology assets. Define measures for threat/risk mitigation. Set encryption standards. Check the effectiveness of the policies, controls, and procedures in place (e.g., audits and continuous monitoring). Ensure the system administrator manages and continuously improves the system based on the new risks or vulnerabilities identified to its wireless security. </t>
+  </si>
+  <si>
+    <t>Likelihood</t>
   </si>
 </sst>
 </file>
@@ -4454,7 +4457,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228C06AC-317E-5044-B7A5-92100984FDF0}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4477,7 +4480,7 @@
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -4514,8 +4517,11 @@
       <c r="L1" s="53" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M1" s="5" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
@@ -4549,8 +4555,11 @@
       <c r="L2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
@@ -4584,8 +4593,11 @@
       <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
@@ -4619,8 +4631,11 @@
       <c r="L4" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -4655,8 +4670,11 @@
       <c r="L5" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="388" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="388" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -4693,8 +4711,11 @@
       <c r="L6" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -4729,8 +4750,11 @@
       <c r="L7" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -4765,8 +4789,11 @@
       <c r="L8" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -4801,8 +4828,11 @@
       <c r="L9" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -4839,8 +4869,11 @@
       <c r="L10" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -4875,8 +4908,11 @@
       <c r="L11" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -4913,8 +4949,11 @@
       <c r="L12" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>16</v>
       </c>
@@ -4949,8 +4988,11 @@
       <c r="L13" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>16</v>
       </c>
@@ -4985,8 +5027,11 @@
       <c r="L14" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
@@ -5021,8 +5066,11 @@
       <c r="L15" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>16</v>
       </c>
@@ -5059,8 +5107,11 @@
       <c r="L16" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>16</v>
       </c>
@@ -5093,8 +5144,11 @@
       <c r="L17" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
@@ -5131,8 +5185,11 @@
       <c r="L18" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
         <v>20</v>
       </c>
@@ -5166,8 +5223,11 @@
       <c r="L19" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -5204,8 +5264,11 @@
       <c r="L20" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -5239,8 +5302,11 @@
       <c r="L21" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -5274,8 +5340,11 @@
       <c r="L22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -5312,8 +5381,11 @@
       <c r="L23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -5347,8 +5419,11 @@
       <c r="L24" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>24</v>
       </c>
@@ -5383,8 +5458,11 @@
       <c r="L25" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -5421,8 +5499,11 @@
       <c r="L26" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>24</v>
       </c>
@@ -5457,8 +5538,11 @@
       <c r="L27" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
@@ -5493,8 +5577,11 @@
       <c r="L28" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>28</v>
       </c>
@@ -5524,11 +5611,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE6EBA3-B14F-E947-A615-39B9D02994B2}">
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5548,7 +5635,7 @@
     <col min="16384" max="16384" width="8" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -5585,8 +5672,11 @@
       <c r="L1" s="42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="M1" s="42" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -5623,8 +5713,11 @@
       <c r="L2" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+      <c r="M2" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>37</v>
       </c>
@@ -5661,8 +5754,11 @@
       <c r="L3" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M3" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>37</v>
       </c>
@@ -5699,8 +5795,11 @@
       <c r="L4" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M4" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>37</v>
       </c>
@@ -5737,8 +5836,11 @@
       <c r="L5" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M5" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>37</v>
       </c>
@@ -5772,8 +5874,11 @@
       <c r="L6" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M6" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
@@ -5807,8 +5912,11 @@
       <c r="L7" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M7" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>37</v>
       </c>
@@ -5845,8 +5953,11 @@
       <c r="L8" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M8" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>44</v>
       </c>
@@ -5883,8 +5994,11 @@
       <c r="L9" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M9" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>44</v>
       </c>
@@ -5921,8 +6035,11 @@
       <c r="L10" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M10" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>44</v>
       </c>
@@ -5959,8 +6076,11 @@
       <c r="L11" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M11" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>44</v>
       </c>
@@ -5997,8 +6117,11 @@
       <c r="L12" s="15" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+      <c r="M12" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>50</v>
       </c>
@@ -6035,8 +6158,11 @@
       <c r="L13" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="404" x14ac:dyDescent="0.2">
+      <c r="M13" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>50</v>
       </c>
@@ -6073,8 +6199,11 @@
       <c r="L14" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M14" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>50</v>
       </c>
@@ -6111,8 +6240,11 @@
       <c r="L15" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M15" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
         <v>50</v>
       </c>
@@ -6149,8 +6281,11 @@
       <c r="L16" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="404" x14ac:dyDescent="0.2">
+      <c r="M16" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>50</v>
       </c>
@@ -6184,8 +6319,11 @@
       <c r="L17" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M17" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>55</v>
       </c>
@@ -6222,8 +6360,11 @@
       <c r="L18" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M18" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>68</v>
       </c>
@@ -6258,8 +6399,11 @@
       <c r="L19" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="388" x14ac:dyDescent="0.2">
+      <c r="M19" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="388" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>68</v>
       </c>
@@ -6296,8 +6440,11 @@
       <c r="L20" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M20" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>74</v>
       </c>
@@ -6334,8 +6481,11 @@
       <c r="L21" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M21" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>74</v>
       </c>
@@ -6372,8 +6522,11 @@
       <c r="L22" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M22" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
         <v>74</v>
       </c>
@@ -6410,8 +6563,11 @@
       <c r="L23" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M23" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>74</v>
       </c>
@@ -6448,8 +6604,11 @@
       <c r="L24" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="M24" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>74</v>
       </c>
@@ -6486,8 +6645,11 @@
       <c r="L25" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M25" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>80</v>
       </c>
@@ -6524,8 +6686,11 @@
       <c r="L26" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M26" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>80</v>
       </c>
@@ -6562,8 +6727,11 @@
       <c r="L27" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M27" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>80</v>
       </c>
@@ -6600,8 +6768,11 @@
       <c r="L28" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M28" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>80</v>
       </c>
@@ -6634,8 +6805,11 @@
       <c r="L29" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+      <c r="M29" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>94</v>
       </c>
@@ -6670,8 +6844,11 @@
       <c r="L30" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M30" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>94</v>
       </c>
@@ -6708,8 +6885,11 @@
       <c r="L31" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M31" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>101</v>
       </c>
@@ -6746,8 +6926,11 @@
       <c r="L32" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M32" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>101</v>
       </c>
@@ -6782,8 +6965,11 @@
       <c r="L33" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="M33" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>101</v>
       </c>
@@ -6818,8 +7004,11 @@
       <c r="L34" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M34" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>101</v>
       </c>
@@ -6854,8 +7043,11 @@
       <c r="L35" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M35" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>108</v>
       </c>
@@ -6889,8 +7081,11 @@
       <c r="L36" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M36" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>108</v>
       </c>
@@ -6927,8 +7122,11 @@
       <c r="L37" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+      <c r="M37" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="356" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>108</v>
       </c>
@@ -6962,8 +7160,11 @@
       <c r="L38" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+      <c r="M38" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>108</v>
       </c>
@@ -6997,8 +7198,11 @@
       <c r="L39" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="M39" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>108</v>
       </c>
@@ -7032,8 +7236,11 @@
       <c r="L40" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+      <c r="M40" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>114</v>
       </c>
@@ -7070,8 +7277,11 @@
       <c r="L41" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M41" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>114</v>
       </c>
@@ -7108,8 +7318,11 @@
       <c r="L42" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M42" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>114</v>
       </c>
@@ -7146,8 +7359,11 @@
       <c r="L43" s="15" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M43" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
         <v>114</v>
       </c>
@@ -7184,8 +7400,11 @@
       <c r="L44" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="372" x14ac:dyDescent="0.2">
+      <c r="M44" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="372" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>114</v>
       </c>
@@ -7222,8 +7441,11 @@
       <c r="L45" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M45" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
         <v>114</v>
       </c>
@@ -7258,8 +7480,11 @@
       <c r="L46" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="M46" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>114</v>
       </c>
@@ -7296,8 +7521,11 @@
       <c r="L47" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M47" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>120</v>
       </c>
@@ -7332,8 +7560,11 @@
       <c r="L48" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M48" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>120</v>
       </c>
@@ -7368,8 +7599,11 @@
       <c r="L49" s="15" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M49" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>120</v>
       </c>
@@ -7404,8 +7638,11 @@
       <c r="L50" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M50" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
         <v>120</v>
       </c>
@@ -7440,8 +7677,11 @@
       <c r="L51" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M51" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
         <v>120</v>
       </c>
@@ -7476,8 +7716,11 @@
       <c r="L52" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M52" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
         <v>126</v>
       </c>
@@ -7514,8 +7757,11 @@
       <c r="L53" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="M53" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>126</v>
       </c>
@@ -7552,8 +7798,11 @@
       <c r="L54" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M54" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>126</v>
       </c>
@@ -7590,8 +7839,11 @@
       <c r="L55" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M55" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
         <v>126</v>
       </c>
@@ -7628,8 +7880,11 @@
       <c r="L56" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M56" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
         <v>126</v>
       </c>
@@ -7662,8 +7917,11 @@
       <c r="L57" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M57" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
         <v>133</v>
       </c>
@@ -7700,8 +7958,11 @@
       <c r="L58" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M58" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
         <v>133</v>
       </c>
@@ -7738,8 +7999,11 @@
       <c r="L59" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M59" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
         <v>133</v>
       </c>
@@ -7776,8 +8040,11 @@
       <c r="L60" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M60" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>133</v>
       </c>
@@ -7814,8 +8081,11 @@
       <c r="L61" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M61" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
         <v>133</v>
       </c>
@@ -7852,8 +8122,11 @@
       <c r="L62" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="M62" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
         <v>133</v>
       </c>
@@ -7890,8 +8163,11 @@
       <c r="L63" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M63" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>133</v>
       </c>
@@ -7926,8 +8202,11 @@
       <c r="L64" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M64" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
         <v>133</v>
       </c>
@@ -7964,8 +8243,11 @@
       <c r="L65" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M65" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
         <v>133</v>
       </c>
@@ -8002,8 +8284,11 @@
       <c r="L66" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M66" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
         <v>133</v>
       </c>
@@ -8040,8 +8325,11 @@
       <c r="L67" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M67" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
         <v>133</v>
       </c>
@@ -8078,8 +8366,11 @@
       <c r="L68" s="10" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M68" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
         <v>139</v>
       </c>
@@ -8114,8 +8405,11 @@
       <c r="L69" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="M69" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
         <v>139</v>
       </c>
@@ -8150,8 +8444,11 @@
       <c r="L70" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M70" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A71" s="39" t="s">
         <v>139</v>
       </c>
@@ -8186,8 +8483,11 @@
       <c r="L71" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M71" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A72" s="27" t="s">
         <v>146</v>
       </c>
@@ -8224,8 +8524,11 @@
       <c r="L72" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M72" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
         <v>146</v>
       </c>
@@ -8262,8 +8565,11 @@
       <c r="L73" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M73" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
         <v>153</v>
       </c>
@@ -8298,8 +8604,11 @@
       <c r="L74" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M74" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="s">
         <v>153</v>
       </c>
@@ -8336,8 +8645,11 @@
       <c r="L75" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M75" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">
         <v>153</v>
       </c>
@@ -8372,8 +8684,11 @@
       <c r="L76" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M76" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
         <v>153</v>
       </c>
@@ -8410,8 +8725,11 @@
       <c r="L77" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+      <c r="M77" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
         <v>153</v>
       </c>
@@ -8446,8 +8764,11 @@
       <c r="L78" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M78" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
         <v>680</v>
       </c>
@@ -8484,8 +8805,11 @@
       <c r="L79" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="404" x14ac:dyDescent="0.2">
+      <c r="M79" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
         <v>680</v>
       </c>
@@ -8522,8 +8846,11 @@
       <c r="L80" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="M80" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
         <v>680</v>
       </c>
@@ -8560,8 +8887,11 @@
       <c r="L81" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="340" x14ac:dyDescent="0.2">
+      <c r="M81" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
         <v>680</v>
       </c>
@@ -8598,8 +8928,11 @@
       <c r="L82" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M82" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
         <v>680</v>
       </c>
@@ -8634,8 +8967,11 @@
       <c r="L83" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M83" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
         <v>680</v>
       </c>
@@ -8670,8 +9006,11 @@
       <c r="L84" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="M84" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" s="23" t="s">
         <v>168</v>
       </c>
@@ -8708,8 +9047,11 @@
       <c r="L85" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M85" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
         <v>168</v>
       </c>
@@ -8744,8 +9086,11 @@
       <c r="L86" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M86" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A87" s="23" t="s">
         <v>168</v>
       </c>
@@ -8782,8 +9127,11 @@
       <c r="L87" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M87" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A88" s="23" t="s">
         <v>168</v>
       </c>
@@ -8820,8 +9168,11 @@
       <c r="L88" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M88" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A89" s="22" t="s">
         <v>175</v>
       </c>
@@ -8858,8 +9209,11 @@
       <c r="L89" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M89" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A90" s="22" t="s">
         <v>175</v>
       </c>
@@ -8894,8 +9248,11 @@
       <c r="L90" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+      <c r="M90" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="356" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
         <v>175</v>
       </c>
@@ -8930,8 +9287,11 @@
       <c r="L91" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+      <c r="M91" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A92" s="22" t="s">
         <v>175</v>
       </c>
@@ -8965,8 +9325,11 @@
       <c r="L92" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M92" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A93" s="22" t="s">
         <v>183</v>
       </c>
@@ -9001,8 +9364,11 @@
       <c r="L93" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+      <c r="M93" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
         <v>183</v>
       </c>
@@ -9039,8 +9405,11 @@
       <c r="L94" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" ht="289" x14ac:dyDescent="0.2">
+      <c r="M94" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="289" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>183</v>
       </c>
@@ -9075,8 +9444,11 @@
       <c r="L95" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+      <c r="M95" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="356" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>183</v>
       </c>
@@ -9111,8 +9483,11 @@
       <c r="L96" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="M96" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
         <v>183</v>
       </c>
@@ -9149,8 +9524,11 @@
       <c r="L97" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" ht="388" x14ac:dyDescent="0.2">
+      <c r="M97" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="388" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
         <v>183</v>
       </c>
@@ -9187,8 +9565,11 @@
       <c r="L98" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M98" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A99" s="22" t="s">
         <v>183</v>
       </c>
@@ -9225,8 +9606,11 @@
       <c r="L99" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M99" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A100" s="22" t="s">
         <v>183</v>
       </c>
@@ -9257,8 +9641,11 @@
       <c r="L100" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="M100" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
         <v>190</v>
       </c>
@@ -9295,8 +9682,11 @@
       <c r="L101" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M101" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>190</v>
       </c>
@@ -9333,8 +9723,11 @@
       <c r="L102" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M102" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>190</v>
       </c>
@@ -9371,8 +9764,11 @@
       <c r="L103" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+      <c r="M103" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>190</v>
       </c>
@@ -9409,8 +9805,11 @@
       <c r="L104" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="M104" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
         <v>190</v>
       </c>
@@ -9447,8 +9846,11 @@
       <c r="L105" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="M105" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
         <v>190</v>
       </c>
@@ -9483,8 +9885,11 @@
       <c r="L106" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M106" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
         <v>197</v>
       </c>
@@ -9521,8 +9926,11 @@
       <c r="L107" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M107" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
         <v>204</v>
       </c>
@@ -9559,8 +9967,11 @@
       <c r="L108" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="M108" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
         <v>204</v>
       </c>
@@ -9597,8 +10008,11 @@
       <c r="L109" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M109" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
         <v>204</v>
       </c>
@@ -9635,8 +10049,11 @@
       <c r="L110" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="M110" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
         <v>211</v>
       </c>
@@ -9673,8 +10090,11 @@
       <c r="L111" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" ht="221" x14ac:dyDescent="0.2">
+      <c r="M111" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
         <v>211</v>
       </c>
@@ -9711,8 +10131,11 @@
       <c r="L112" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="M112" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
         <v>211</v>
       </c>
@@ -9749,8 +10172,11 @@
       <c r="L113" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="M113" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
         <v>211</v>
       </c>
@@ -9787,34 +10213,37 @@
       <c r="L114" s="15" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M114" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H116" s="12"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H118" s="12"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E120" s="15"/>
       <c r="F120" s="15"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="15"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B127" s="15"/>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
@@ -9898,12 +10327,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -10035,6 +10458,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10045,15 +10474,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10071,6 +10491,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Corrected typo in findings repository
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/dev/rva-reporting-engine/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/external-version/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7198A9-CF94-3B43-9B36-899121BC3293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B57523-7E67-C147-A534-8414CBF09FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16380" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
@@ -871,9 +871,6 @@
     <t>NTLM Authentication Enabled</t>
   </si>
   <si>
-    <t xml:space="preserve">Windows New Technology LAN Manager (NTLM) authentication, introduced in Windows NT 3.1, validates whether a user is who they claim to be. A successor of LanMan (LM), NTLM authentication continues to use insecure methods through a hashing process of credentials. NTLM authentication also lacks effective support for smart cards and other multifactor authentication (MFA) solutions. If an attacker can obtain a username and a hash, they can conduct attacks such as Pass-the-Hash. On the client side, password hashes are stored in SYSTEM and Sequence Alignment Map (SAM) files, readable by anyone with administrator access. On the server side, password hashes are stored in the NTDS.dit file on the domain controller and are susceptible to DCSync attacks.  </t>
-  </si>
-  <si>
     <t>Since NTLM authentication has been replaced by Kerberos as the default authentication mechanism with the release of Windows 2000, organizations must disable NTLM authentication on systems that support it and modify the Group Policy settings to restrict NTLM. If necessary, create exception lists to allow specific servers access with NTLM authentication. Ensure that NTLMv1 is always disabled. Audit all NTLM traffic.</t>
   </si>
   <si>
@@ -3242,6 +3239,9 @@
   </si>
   <si>
     <t>Likelihood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows New Technology LAN Manager (NTLM) authentication, introduced in Windows NT 3.1, validates whether a user is who they claim to be. A successor of LanMan (LM), NTLM authentication continues to use insecure methods through a hashing process of credentials. NTLM authentication also lacks effective support for smart cards and other multifactor authentication (MFA) solutions. If an attacker can obtain a username and a hash, they can conduct attacks such as Pass-the-Hash. On the client side, password hashes are stored in SYSTEM and Security Account Manager (SAM) files, readable by anyone with administrator access. On the server side, password hashes are stored in the NTDS.dit file on the domain controller and are susceptible to DCSync attacks.  </t>
   </si>
 </sst>
 </file>
@@ -4518,7 +4518,7 @@
         <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="187" x14ac:dyDescent="0.2">
@@ -4547,7 +4547,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4585,7 +4585,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4623,7 +4623,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4662,7 +4662,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4703,7 +4703,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4742,7 +4742,7 @@
         <v>72</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>73</v>
@@ -4781,7 +4781,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4980,7 +4980,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -5019,7 +5019,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5479,7 +5479,7 @@
         <v>198</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>199</v>
@@ -5673,10 +5673,10 @@
         <v>36</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -5854,19 +5854,19 @@
         <v>248</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>963</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>252</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>167</v>
@@ -5889,25 +5889,25 @@
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="I7" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>54</v>
@@ -5927,28 +5927,28 @@
         <v>7</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="H8" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="H8" s="43" t="s">
-        <v>264</v>
-      </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>267</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>54</v>
@@ -5968,28 +5968,28 @@
         <v>8</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>274</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>54</v>
@@ -6009,28 +6009,28 @@
         <v>9</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="15" t="s">
         <v>280</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>281</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>54</v>
@@ -6050,28 +6050,28 @@
         <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="H11" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="I11" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="15" t="s">
         <v>287</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>288</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>54</v>
@@ -6091,31 +6091,31 @@
         <v>11</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="H12" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>292</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="J12" s="10" t="s">
+        <v>923</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>924</v>
-      </c>
-      <c r="K12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>294</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="M12" s="15">
         <v>50</v>
@@ -6132,28 +6132,28 @@
         <v>12</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="J13" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="15" t="s">
         <v>302</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>303</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>43</v>
@@ -6173,28 +6173,28 @@
         <v>13</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="15" t="s">
         <v>309</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>310</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>54</v>
@@ -6214,25 +6214,25 @@
         <v>14</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>316</v>
-      </c>
       <c r="J15" s="10" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6255,28 +6255,28 @@
         <v>15</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="I16" s="15" t="s">
+      <c r="J16" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>322</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>323</v>
       </c>
       <c r="L16" s="15" t="s">
         <v>54</v>
@@ -6296,25 +6296,25 @@
         <v>16</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="11" t="s">
+        <v>925</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>328</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>926</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>329</v>
       </c>
       <c r="L17" s="15" t="s">
         <v>54</v>
@@ -6334,25 +6334,25 @@
         <v>17</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="H18" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="J18" s="11" t="s">
         <v>335</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>336</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>196</v>
@@ -6375,23 +6375,23 @@
         <v>18</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="14" t="s">
         <v>339</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>340</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
         <v>72</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K19" s="11" t="s">
         <v>73</v>
@@ -6414,25 +6414,25 @@
         <v>19</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>347</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>348</v>
       </c>
       <c r="K20" s="11" t="s">
         <v>167</v>
@@ -6455,28 +6455,28 @@
         <v>20</v>
       </c>
       <c r="D21" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="43" t="s">
         <v>351</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="H21" s="43" t="s">
+        <v>351</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="H21" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="I21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>354</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>355</v>
       </c>
       <c r="L21" s="15" t="s">
         <v>43</v>
@@ -6496,28 +6496,28 @@
         <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="43" t="s">
         <v>358</v>
       </c>
-      <c r="G22" s="43" t="s">
+      <c r="H22" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="J22" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>363</v>
       </c>
       <c r="L22" s="15" t="s">
         <v>43</v>
@@ -6537,25 +6537,25 @@
         <v>22</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="F23" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="I23" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="J23" s="11" t="s">
         <v>369</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>370</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>73</v>
@@ -6578,28 +6578,28 @@
         <v>23</v>
       </c>
       <c r="D24" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H24" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="I24" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="J24" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>377</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>378</v>
       </c>
       <c r="L24" s="15" t="s">
         <v>54</v>
@@ -6619,31 +6619,31 @@
         <v>24</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="43" t="s">
         <v>381</v>
       </c>
-      <c r="G25" s="43" t="s">
+      <c r="H25" s="43" t="s">
+        <v>381</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="H25" s="43" t="s">
-        <v>382</v>
-      </c>
-      <c r="I25" s="15" t="s">
+      <c r="J25" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>384</v>
       </c>
       <c r="K25" s="11">
         <v>7</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M25" s="15">
         <v>50</v>
@@ -6660,28 +6660,28 @@
         <v>25</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="G26" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="H26" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="I26" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>392</v>
-      </c>
       <c r="K26" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L26" s="15" t="s">
         <v>43</v>
@@ -6701,28 +6701,28 @@
         <v>26</v>
       </c>
       <c r="D27" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="H27" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="I27" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>398</v>
-      </c>
       <c r="J27" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L27" s="15" t="s">
         <v>43</v>
@@ -6742,28 +6742,28 @@
         <v>27</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="H28" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>403</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L28" s="15" t="s">
         <v>43</v>
@@ -6783,24 +6783,24 @@
         <v>28</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>405</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>406</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L29" s="15" t="s">
         <v>43</v>
@@ -6820,20 +6820,20 @@
         <v>29</v>
       </c>
       <c r="D30" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="45" t="s">
         <v>408</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="G30" s="14" t="s">
         <v>409</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>410</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>99</v>
@@ -6859,28 +6859,28 @@
         <v>30</v>
       </c>
       <c r="D31" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="F31" s="45" t="s">
         <v>413</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="G31" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="I31" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>419</v>
       </c>
       <c r="L31" s="15" t="s">
         <v>54</v>
@@ -6900,28 +6900,28 @@
         <v>31</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>944</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>945</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>945</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>946</v>
-      </c>
-      <c r="G32" s="13" t="s">
+      <c r="H32" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="I32" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="J32" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>424</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>425</v>
       </c>
       <c r="L32" s="15" t="s">
         <v>54</v>
@@ -6941,20 +6941,20 @@
         <v>32</v>
       </c>
       <c r="D33" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>946</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>947</v>
+      </c>
+      <c r="G33" s="13" t="s">
         <v>426</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>947</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>948</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>427</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>106</v>
@@ -6980,20 +6980,20 @@
         <v>33</v>
       </c>
       <c r="D34" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>948</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>949</v>
-      </c>
-      <c r="F34" s="10" t="s">
+      <c r="G34" s="13" t="s">
         <v>430</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>431</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>106</v>
@@ -7019,20 +7019,20 @@
         <v>34</v>
       </c>
       <c r="D35" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="G35" s="13" t="s">
         <v>434</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>435</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>106</v>
@@ -7058,25 +7058,25 @@
         <v>35</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="F36" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="G36" s="14" t="s">
         <v>438</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="I36" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>442</v>
       </c>
       <c r="L36" s="15" t="s">
         <v>43</v>
@@ -7096,22 +7096,22 @@
         <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="G37" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="H37" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="I37" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>448</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>209</v>
@@ -7120,7 +7120,7 @@
         <v>210</v>
       </c>
       <c r="L37" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M37" s="15">
         <v>50</v>
@@ -7137,19 +7137,19 @@
         <v>37</v>
       </c>
       <c r="D38" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="H38" s="10" t="s">
-        <v>452</v>
-      </c>
       <c r="I38" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>209</v>
@@ -7175,25 +7175,25 @@
         <v>38</v>
       </c>
       <c r="D39" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="F39" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="G39" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="I39" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>459</v>
       </c>
       <c r="L39" s="15" t="s">
         <v>43</v>
@@ -7213,25 +7213,25 @@
         <v>39</v>
       </c>
       <c r="D40" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="G40" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="I40" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="J40" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>466</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>43</v>
@@ -7251,25 +7251,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="F41" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="G41" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="H41" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="I41" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>472</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>473</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>196</v>
@@ -7292,28 +7292,28 @@
         <v>41</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="F42" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="G42" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="H42" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="I42" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>480</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>481</v>
       </c>
       <c r="L42" s="15" t="s">
         <v>54</v>
@@ -7333,31 +7333,31 @@
         <v>42</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="H43" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="I43" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>489</v>
-      </c>
       <c r="L43" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M43" s="15">
         <v>50</v>
@@ -7374,28 +7374,28 @@
         <v>43</v>
       </c>
       <c r="D44" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>490</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="F44" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="G44" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="H44" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="I44" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="J44" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>496</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>497</v>
       </c>
       <c r="L44" s="15" t="s">
         <v>43</v>
@@ -7415,25 +7415,25 @@
         <v>44</v>
       </c>
       <c r="D45" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>498</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="F45" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="G45" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="I45" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>503</v>
-      </c>
       <c r="J45" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>73</v>
@@ -7456,26 +7456,26 @@
         <v>45</v>
       </c>
       <c r="D46" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>504</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="F46" s="11" t="s">
         <v>505</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="G46" s="12" t="s">
         <v>506</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>507</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="K46" s="4" t="s">
         <v>508</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>509</v>
       </c>
       <c r="L46" s="15" t="s">
         <v>43</v>
@@ -7495,28 +7495,28 @@
         <v>46</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="F47" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="G47" s="29" t="s">
         <v>512</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="H47" s="29" t="s">
         <v>513</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="I47" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>516</v>
-      </c>
       <c r="K47" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L47" s="15" t="s">
         <v>43</v>
@@ -7536,26 +7536,26 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>940</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>942</v>
       </c>
-      <c r="F48" s="11" t="s">
-        <v>943</v>
-      </c>
       <c r="G48" s="29" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="J48" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>938</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>939</v>
       </c>
       <c r="L48" s="15" t="s">
         <v>54</v>
@@ -7575,29 +7575,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>929</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>932</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>943</v>
+      </c>
+      <c r="G49" s="29" t="s">
         <v>930</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>933</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>944</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>931</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="M49" s="15">
         <v>50</v>
@@ -7614,26 +7614,26 @@
         <v>49</v>
       </c>
       <c r="D50" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>518</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="G50" s="29" t="s">
         <v>519</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>520</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L50" s="15" t="s">
         <v>43</v>
@@ -7653,26 +7653,26 @@
         <v>50</v>
       </c>
       <c r="D51" s="10" t="s">
+        <v>521</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="G51" s="29" t="s">
         <v>524</v>
-      </c>
-      <c r="G51" s="29" t="s">
-        <v>525</v>
       </c>
       <c r="H51" s="29"/>
       <c r="I51" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>526</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>527</v>
       </c>
       <c r="L51" s="15" t="s">
         <v>43</v>
@@ -7692,26 +7692,26 @@
         <v>51</v>
       </c>
       <c r="D52" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="F52" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="G52" s="29" t="s">
         <v>530</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>531</v>
       </c>
       <c r="H52" s="29"/>
       <c r="I52" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="J52" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="K52" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>534</v>
       </c>
       <c r="L52" s="15" t="s">
         <v>43</v>
@@ -7731,28 +7731,28 @@
         <v>52</v>
       </c>
       <c r="D53" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="F53" s="11" t="s">
+        <v>949</v>
+      </c>
+      <c r="G53" s="43" t="s">
         <v>536</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>950</v>
-      </c>
-      <c r="G53" s="43" t="s">
+      <c r="H53" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="H53" s="43" t="s">
-        <v>537</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>540</v>
       </c>
       <c r="L53" s="15" t="s">
         <v>54</v>
@@ -7772,28 +7772,28 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>542</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G54" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="H54" s="43" t="s">
-        <v>537</v>
-      </c>
-      <c r="I54" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>540</v>
       </c>
       <c r="L54" s="15" t="s">
         <v>54</v>
@@ -7813,28 +7813,28 @@
         <v>54</v>
       </c>
       <c r="D55" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="G55" s="43" t="s">
         <v>545</v>
       </c>
-      <c r="G55" s="43" t="s">
-        <v>546</v>
-      </c>
       <c r="H55" s="43" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I55" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="K55" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>540</v>
       </c>
       <c r="L55" s="15" t="s">
         <v>54</v>
@@ -7854,28 +7854,28 @@
         <v>55</v>
       </c>
       <c r="D56" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="F56" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="G56" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="H56" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="I56" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="J56" s="4" t="s">
-        <v>553</v>
-      </c>
       <c r="K56" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L56" s="15" t="s">
         <v>54</v>
@@ -7895,24 +7895,24 @@
         <v>56</v>
       </c>
       <c r="D57" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>554</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="F57" s="10" t="s">
         <v>555</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>556</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="J57" s="4" t="s">
-        <v>553</v>
-      </c>
       <c r="K57" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L57" s="15" t="s">
         <v>54</v>
@@ -7932,28 +7932,28 @@
         <v>57</v>
       </c>
       <c r="D58" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="E58" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="F58" s="10" t="s">
+        <v>953</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>954</v>
-      </c>
-      <c r="G58" s="10" t="s">
+      <c r="H58" s="14" t="s">
         <v>559</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="I58" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>562</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>563</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>54</v>
@@ -7973,25 +7973,25 @@
         <v>58</v>
       </c>
       <c r="D59" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="F59" s="11" t="s">
+        <v>954</v>
+      </c>
+      <c r="G59" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="F59" s="11" t="s">
-        <v>955</v>
-      </c>
-      <c r="G59" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="I59" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="J59" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>569</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>247</v>
@@ -8014,28 +8014,28 @@
         <v>59</v>
       </c>
       <c r="D60" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>570</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="F60" s="10" t="s">
+        <v>951</v>
+      </c>
+      <c r="G60" s="14" t="s">
         <v>571</v>
       </c>
-      <c r="F60" s="10" t="s">
-        <v>952</v>
-      </c>
-      <c r="G60" s="14" t="s">
+      <c r="H60" s="14" t="s">
         <v>572</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="I60" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="J60" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>575</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>576</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>54</v>
@@ -8055,28 +8055,28 @@
         <v>60</v>
       </c>
       <c r="D61" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="F61" s="10" t="s">
+        <v>955</v>
+      </c>
+      <c r="G61" s="16" t="s">
         <v>578</v>
       </c>
-      <c r="F61" s="10" t="s">
-        <v>956</v>
-      </c>
-      <c r="G61" s="16" t="s">
+      <c r="H61" s="14" t="s">
         <v>579</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="I61" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>54</v>
@@ -8096,28 +8096,28 @@
         <v>61</v>
       </c>
       <c r="D62" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="F62" s="10" t="s">
+        <v>956</v>
+      </c>
+      <c r="G62" s="14" t="s">
         <v>585</v>
       </c>
-      <c r="F62" s="10" t="s">
-        <v>957</v>
-      </c>
-      <c r="G62" s="14" t="s">
+      <c r="H62" s="14" t="s">
         <v>586</v>
       </c>
-      <c r="H62" s="14" t="s">
+      <c r="I62" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="K62" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>54</v>
@@ -8137,28 +8137,28 @@
         <v>62</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="E63" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="F63" s="10" t="s">
+        <v>952</v>
+      </c>
+      <c r="G63" s="14" t="s">
         <v>592</v>
       </c>
-      <c r="F63" s="10" t="s">
-        <v>953</v>
-      </c>
-      <c r="G63" s="14" t="s">
+      <c r="H63" s="14" t="s">
         <v>593</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="I63" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>596</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>597</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>54</v>
@@ -8178,23 +8178,23 @@
         <v>63</v>
       </c>
       <c r="D64" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="E64" s="10" t="s">
         <v>598</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="F64" s="10" t="s">
+        <v>957</v>
+      </c>
+      <c r="G64" s="14" t="s">
         <v>599</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>958</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>600</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>601</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>602</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>247</v>
@@ -8217,28 +8217,28 @@
         <v>64</v>
       </c>
       <c r="D65" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="E65" s="10" t="s">
         <v>603</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="F65" s="10" t="s">
+        <v>958</v>
+      </c>
+      <c r="G65" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="F65" s="10" t="s">
-        <v>959</v>
-      </c>
-      <c r="G65" s="14" t="s">
+      <c r="H65" s="12" t="s">
         <v>605</v>
       </c>
-      <c r="H65" s="12" t="s">
+      <c r="I65" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="J65" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="K65" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>54</v>
@@ -8258,28 +8258,28 @@
         <v>65</v>
       </c>
       <c r="D66" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="E66" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="F66" s="10" t="s">
+        <v>958</v>
+      </c>
+      <c r="G66" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="F66" s="10" t="s">
-        <v>959</v>
-      </c>
-      <c r="G66" s="10" t="s">
+      <c r="H66" s="14" t="s">
         <v>612</v>
       </c>
-      <c r="H66" s="14" t="s">
+      <c r="I66" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="I66" s="4" t="s">
-        <v>614</v>
-      </c>
       <c r="J66" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="K66" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>54</v>
@@ -8299,28 +8299,28 @@
         <v>66</v>
       </c>
       <c r="D67" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="E67" s="10" t="s">
         <v>615</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="10" t="s">
+        <v>959</v>
+      </c>
+      <c r="G67" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F67" s="10" t="s">
-        <v>960</v>
-      </c>
-      <c r="G67" s="14" t="s">
+      <c r="H67" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="H67" s="14" t="s">
+      <c r="I67" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="I67" s="4" t="s">
-        <v>619</v>
-      </c>
       <c r="J67" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="K67" s="4" t="s">
         <v>596</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>597</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>54</v>
@@ -8340,31 +8340,31 @@
         <v>67</v>
       </c>
       <c r="D68" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="E68" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="F68" s="10" t="s">
+        <v>960</v>
+      </c>
+      <c r="G68" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="F68" s="10" t="s">
-        <v>961</v>
-      </c>
-      <c r="G68" s="10" t="s">
+      <c r="H68" s="14" t="s">
         <v>622</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="I68" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="I68" s="4" t="s">
+      <c r="J68" s="4" t="s">
         <v>624</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>625</v>
       </c>
       <c r="K68" s="4">
         <v>7</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="M68" s="15">
         <v>50</v>
@@ -8381,20 +8381,20 @@
         <v>68</v>
       </c>
       <c r="D69" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="F69" s="10" t="s">
         <v>628</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="G69" s="10" t="s">
         <v>629</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>630</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>145</v>
@@ -8420,20 +8420,20 @@
         <v>69</v>
       </c>
       <c r="D70" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>632</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="F70" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="G70" s="10" t="s">
         <v>634</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>635</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>145</v>
@@ -8459,20 +8459,20 @@
         <v>70</v>
       </c>
       <c r="D71" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="F71" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="G71" s="14" t="s">
         <v>638</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>639</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>145</v>
@@ -8498,25 +8498,25 @@
         <v>71</v>
       </c>
       <c r="D72" s="10" t="s">
+        <v>639</v>
+      </c>
+      <c r="E72" s="11" t="s">
         <v>640</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>641</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="H72" s="43" t="s">
+        <v>642</v>
+      </c>
+      <c r="I72" s="11" t="s">
         <v>643</v>
       </c>
-      <c r="H72" s="43" t="s">
-        <v>643</v>
-      </c>
-      <c r="I72" s="11" t="s">
+      <c r="J72" s="11" t="s">
         <v>644</v>
-      </c>
-      <c r="J72" s="11" t="s">
-        <v>645</v>
       </c>
       <c r="K72" s="11">
         <v>16</v>
@@ -8539,31 +8539,31 @@
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>646</v>
       </c>
-      <c r="E73" s="11" t="s">
+      <c r="F73" s="11" t="s">
         <v>647</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="G73" s="11" t="s">
-        <v>649</v>
-      </c>
       <c r="H73" s="43" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I73" s="11" t="s">
+        <v>643</v>
+      </c>
+      <c r="J73" s="11" t="s">
         <v>644</v>
-      </c>
-      <c r="J73" s="11" t="s">
-        <v>645</v>
       </c>
       <c r="K73" s="11">
         <v>16</v>
       </c>
       <c r="L73" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M73" s="15">
         <v>50</v>
@@ -8580,26 +8580,26 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="E74" s="11" t="s">
         <v>650</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="F74" s="11" t="s">
         <v>651</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="G74" s="11" t="s">
         <v>652</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>653</v>
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>654</v>
       </c>
-      <c r="J74" s="11" t="s">
-        <v>655</v>
-      </c>
       <c r="K74" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L74" s="15" t="s">
         <v>43</v>
@@ -8619,28 +8619,28 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>656</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="F75" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="G75" s="14" t="s">
         <v>658</v>
       </c>
-      <c r="G75" s="14" t="s">
+      <c r="H75" s="14" t="s">
         <v>659</v>
       </c>
-      <c r="H75" s="14" t="s">
+      <c r="I75" s="10" t="s">
         <v>660</v>
       </c>
-      <c r="I75" s="10" t="s">
+      <c r="J75" s="10" t="s">
+        <v>926</v>
+      </c>
+      <c r="K75" s="10" t="s">
         <v>661</v>
-      </c>
-      <c r="J75" s="10" t="s">
-        <v>927</v>
-      </c>
-      <c r="K75" s="10" t="s">
-        <v>662</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
@@ -8660,26 +8660,26 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
+        <v>662</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>663</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="F76" s="10" t="s">
         <v>664</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="G76" s="14" t="s">
         <v>665</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>666</v>
       </c>
       <c r="H76" s="14"/>
       <c r="I76" s="10" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L76" s="15" t="s">
         <v>43</v>
@@ -8699,28 +8699,28 @@
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>668</v>
       </c>
-      <c r="E77" s="11" t="s">
+      <c r="F77" s="11" t="s">
         <v>669</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="G77" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="H77" s="43" t="s">
+        <v>670</v>
+      </c>
+      <c r="I77" s="11" t="s">
         <v>671</v>
       </c>
-      <c r="H77" s="43" t="s">
-        <v>671</v>
-      </c>
-      <c r="I77" s="11" t="s">
+      <c r="J77" s="11" t="s">
         <v>672</v>
       </c>
-      <c r="J77" s="11" t="s">
-        <v>673</v>
-      </c>
       <c r="K77" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L77" s="15" t="s">
         <v>43</v>
@@ -8740,23 +8740,23 @@
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="F78" s="11" t="s">
         <v>675</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>676</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
+        <v>676</v>
+      </c>
+      <c r="I78" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="J78" s="11" t="s">
         <v>678</v>
-      </c>
-      <c r="J78" s="11" t="s">
-        <v>679</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>73</v>
@@ -8770,7 +8770,7 @@
     </row>
     <row r="79" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8779,25 +8779,25 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="F79" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="H79" s="43" t="s">
+        <v>683</v>
+      </c>
+      <c r="I79" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="H79" s="43" t="s">
-        <v>684</v>
-      </c>
-      <c r="I79" s="11" t="s">
+      <c r="J79" s="11" t="s">
         <v>685</v>
-      </c>
-      <c r="J79" s="11" t="s">
-        <v>686</v>
       </c>
       <c r="K79" s="11">
         <v>16</v>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="80" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8820,19 +8820,19 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>687</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="F80" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="F80" s="11" t="s">
+      <c r="G80" s="43" t="s">
         <v>689</v>
       </c>
-      <c r="G80" s="43" t="s">
-        <v>690</v>
-      </c>
       <c r="H80" s="43" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>172</v>
@@ -8841,7 +8841,7 @@
         <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
@@ -8852,7 +8852,7 @@
     </row>
     <row r="81" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8861,25 +8861,25 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="F81" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="G81" s="43" t="s">
         <v>694</v>
       </c>
-      <c r="G81" s="43" t="s">
+      <c r="H81" s="43" t="s">
         <v>695</v>
       </c>
-      <c r="H81" s="43" t="s">
+      <c r="I81" s="11" t="s">
         <v>696</v>
       </c>
-      <c r="I81" s="11" t="s">
+      <c r="J81" s="11" t="s">
         <v>697</v>
-      </c>
-      <c r="J81" s="11" t="s">
-        <v>698</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>182</v>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="82" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8902,28 +8902,28 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
+        <v>698</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="F82" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="G82" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="H82" s="14" t="s">
         <v>702</v>
       </c>
-      <c r="H82" s="14" t="s">
+      <c r="I82" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="J82" s="10" t="s">
-        <v>705</v>
-      </c>
       <c r="K82" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>43</v>
@@ -8934,7 +8934,7 @@
     </row>
     <row r="83" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B83" s="10">
         <v>20</v>
@@ -8943,23 +8943,23 @@
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="E83" s="11" t="s">
         <v>706</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="F83" s="10" t="s">
         <v>707</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="G83" s="10" t="s">
         <v>708</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>709</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>697</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>698</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>182</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="84" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B84" s="10">
         <v>20</v>
@@ -8982,26 +8982,26 @@
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>710</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="F84" s="10" t="s">
         <v>711</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="G84" s="10" t="s">
         <v>712</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>713</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>43</v>
@@ -9021,25 +9021,25 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="E85" s="46" t="s">
         <v>715</v>
       </c>
-      <c r="E85" s="46" t="s">
+      <c r="F85" s="11" t="s">
         <v>716</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="G85" s="43" t="s">
         <v>717</v>
       </c>
-      <c r="G85" s="43" t="s">
+      <c r="H85" s="43" t="s">
+        <v>717</v>
+      </c>
+      <c r="I85" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="H85" s="43" t="s">
-        <v>718</v>
-      </c>
-      <c r="I85" s="4" t="s">
+      <c r="J85" s="4" t="s">
         <v>719</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>720</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>49</v>
@@ -9062,29 +9062,29 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="E86" s="46" t="s">
         <v>721</v>
       </c>
-      <c r="E86" s="46" t="s">
+      <c r="F86" s="46" t="s">
         <v>722</v>
       </c>
-      <c r="F86" s="46" t="s">
+      <c r="G86" s="10" t="s">
         <v>723</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>724</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>725</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>726</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M86" s="15">
         <v>50</v>
@@ -9101,31 +9101,31 @@
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="F87" s="46" t="s">
         <v>728</v>
       </c>
-      <c r="F87" s="46" t="s">
+      <c r="G87" s="29" t="s">
         <v>729</v>
       </c>
-      <c r="G87" s="29" t="s">
+      <c r="H87" s="12" t="s">
         <v>730</v>
       </c>
-      <c r="H87" s="12" t="s">
-        <v>731</v>
-      </c>
       <c r="I87" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>725</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>726</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M87" s="15">
         <v>50</v>
@@ -9142,28 +9142,28 @@
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="E88" s="46" t="s">
         <v>732</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="F88" s="46" t="s">
         <v>733</v>
       </c>
-      <c r="F88" s="46" t="s">
+      <c r="G88" s="43" t="s">
         <v>734</v>
       </c>
-      <c r="G88" s="43" t="s">
+      <c r="H88" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="I88" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="H88" s="43" t="s">
-        <v>735</v>
-      </c>
-      <c r="I88" s="4" t="s">
+      <c r="J88" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="J88" s="4" t="s">
+      <c r="K88" s="4" t="s">
         <v>737</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>738</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
@@ -9183,25 +9183,25 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="E89" s="46" t="s">
         <v>739</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="F89" s="11" t="s">
         <v>740</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="G89" s="29" t="s">
         <v>741</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="H89" s="12" t="s">
         <v>742</v>
       </c>
-      <c r="H89" s="12" t="s">
+      <c r="I89" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="J89" s="4" t="s">
         <v>744</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>745</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>210</v>
@@ -9224,26 +9224,26 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>746</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>747</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="G90" s="16" t="s">
         <v>748</v>
-      </c>
-      <c r="G90" s="16" t="s">
-        <v>749</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>751</v>
-      </c>
-      <c r="K90" s="4" t="s">
-        <v>752</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
@@ -9263,26 +9263,26 @@
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="E91" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="F91" s="11" t="s">
         <v>754</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="G91" s="29" t="s">
         <v>755</v>
-      </c>
-      <c r="G91" s="29" t="s">
-        <v>756</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="K91" s="4" t="s">
         <v>751</v>
-      </c>
-      <c r="K91" s="4" t="s">
-        <v>752</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
@@ -9302,25 +9302,25 @@
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
+        <v>756</v>
+      </c>
+      <c r="E92" s="11" t="s">
         <v>757</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="F92" s="10" t="s">
         <v>758</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="G92" s="10" t="s">
         <v>759</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="I92" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>762</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>763</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>43</v>
@@ -9340,26 +9340,26 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>764</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="F93" s="10" t="s">
         <v>765</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="G93" s="14" t="s">
         <v>766</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>767</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="J93" s="4" t="s">
+      <c r="K93" s="4" t="s">
         <v>769</v>
-      </c>
-      <c r="K93" s="4" t="s">
-        <v>770</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
@@ -9379,28 +9379,28 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="E94" s="10" t="s">
         <v>771</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="10" t="s">
         <v>772</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="G94" s="12" t="s">
         <v>773</v>
       </c>
-      <c r="G94" s="12" t="s">
+      <c r="H94" s="14" t="s">
         <v>774</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="I94" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="J94" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="J94" s="4" t="s">
+      <c r="K94" s="48" t="s">
         <v>777</v>
-      </c>
-      <c r="K94" s="48" t="s">
-        <v>778</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>54</v>
@@ -9420,23 +9420,23 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>779</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="F95" s="11" t="s">
         <v>780</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="G95" s="29" t="s">
         <v>781</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>782</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>783</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>784</v>
       </c>
       <c r="K95" s="4">
         <v>3</v>
@@ -9459,26 +9459,26 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="F96" s="10" t="s">
         <v>786</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="G96" s="10" t="s">
         <v>787</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>788</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>789</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="K96" s="4" t="s">
         <v>790</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>791</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>43</v>
@@ -9498,31 +9498,31 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="E97" s="10" t="s">
         <v>792</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="F97" s="10" t="s">
         <v>793</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="G97" s="10" t="s">
         <v>794</v>
       </c>
-      <c r="G97" s="10" t="s">
+      <c r="H97" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="H97" s="10" t="s">
+      <c r="I97" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="J97" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="K97" s="4" t="s">
         <v>798</v>
       </c>
-      <c r="K97" s="4" t="s">
-        <v>799</v>
-      </c>
       <c r="L97" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M97" s="15">
         <v>50</v>
@@ -9539,31 +9539,31 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>800</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="F98" s="11" t="s">
         <v>801</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="G98" s="29" t="s">
         <v>802</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="H98" s="12" t="s">
         <v>803</v>
       </c>
-      <c r="H98" s="12" t="s">
+      <c r="I98" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="J98" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="K98" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="K98" s="4" t="s">
-        <v>807</v>
-      </c>
       <c r="L98" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M98" s="15">
         <v>50</v>
@@ -9580,25 +9580,25 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>808</v>
       </c>
-      <c r="E99" s="11" t="s">
+      <c r="F99" s="11" t="s">
         <v>809</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="G99" s="43" t="s">
         <v>810</v>
       </c>
-      <c r="G99" s="43" t="s">
+      <c r="H99" s="43" t="s">
+        <v>810</v>
+      </c>
+      <c r="I99" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="H99" s="43" t="s">
-        <v>811</v>
-      </c>
-      <c r="I99" s="4" t="s">
+      <c r="J99" s="4" t="s">
         <v>812</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>813</v>
       </c>
       <c r="K99" s="4">
         <v>3</v>
@@ -9621,19 +9621,19 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="E100" s="10" t="s">
         <v>814</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="F100" s="10" t="s">
         <v>815</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="I100" s="48" t="s">
         <v>816</v>
       </c>
-      <c r="I100" s="48" t="s">
+      <c r="J100" s="48" t="s">
         <v>817</v>
-      </c>
-      <c r="J100" s="48" t="s">
-        <v>818</v>
       </c>
       <c r="K100" s="48" t="s">
         <v>100</v>
@@ -9656,31 +9656,31 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>819</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="F101" s="11" t="s">
         <v>820</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="10" t="s">
         <v>821</v>
       </c>
-      <c r="G101" s="10" t="s">
+      <c r="H101" s="10" t="s">
         <v>822</v>
       </c>
-      <c r="H101" s="10" t="s">
+      <c r="I101" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="I101" s="11" t="s">
+      <c r="J101" s="11" t="s">
+        <v>928</v>
+      </c>
+      <c r="K101" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="J101" s="11" t="s">
-        <v>929</v>
-      </c>
-      <c r="K101" s="11" t="s">
-        <v>825</v>
-      </c>
       <c r="L101" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M101" s="15">
         <v>50</v>
@@ -9697,31 +9697,31 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="E102" s="11" t="s">
         <v>826</v>
       </c>
-      <c r="E102" s="11" t="s">
+      <c r="F102" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="G102" s="10" t="s">
         <v>828</v>
       </c>
-      <c r="G102" s="10" t="s">
+      <c r="H102" s="11" t="s">
         <v>829</v>
       </c>
-      <c r="H102" s="11" t="s">
+      <c r="I102" s="11" t="s">
         <v>830</v>
       </c>
-      <c r="I102" s="11" t="s">
+      <c r="J102" s="11" t="s">
         <v>831</v>
       </c>
-      <c r="J102" s="11" t="s">
+      <c r="K102" s="11" t="s">
         <v>832</v>
       </c>
-      <c r="K102" s="11" t="s">
-        <v>833</v>
-      </c>
       <c r="L102" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M102" s="15">
         <v>50</v>
@@ -9738,28 +9738,28 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>834</v>
       </c>
-      <c r="E103" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="G103" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="I103" s="11" t="s">
         <v>838</v>
       </c>
-      <c r="I103" s="11" t="s">
+      <c r="J103" s="11" t="s">
         <v>839</v>
       </c>
-      <c r="J103" s="11" t="s">
-        <v>840</v>
-      </c>
       <c r="K103" s="11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L103" s="15" t="s">
         <v>43</v>
@@ -9779,25 +9779,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="E104" s="11" t="s">
         <v>841</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="F104" s="11" t="s">
         <v>842</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="G104" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="G104" s="11" t="s">
+      <c r="H104" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="H104" s="11" t="s">
+      <c r="I104" s="11" t="s">
         <v>845</v>
       </c>
-      <c r="I104" s="11" t="s">
+      <c r="J104" s="11" t="s">
         <v>846</v>
-      </c>
-      <c r="J104" s="11" t="s">
-        <v>847</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>182</v>
@@ -9820,25 +9820,25 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="E105" s="11" t="s">
         <v>848</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="F105" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="G105" s="10" t="s">
         <v>850</v>
       </c>
-      <c r="G105" s="10" t="s">
+      <c r="H105" s="14" t="s">
         <v>851</v>
       </c>
-      <c r="H105" s="14" t="s">
+      <c r="I105" s="11" t="s">
         <v>852</v>
       </c>
-      <c r="I105" s="11" t="s">
+      <c r="J105" s="11" t="s">
         <v>853</v>
-      </c>
-      <c r="J105" s="11" t="s">
-        <v>854</v>
       </c>
       <c r="K105" s="11" t="s">
         <v>210</v>
@@ -9861,25 +9861,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>855</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="F106" s="11" t="s">
         <v>856</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="G106" s="10" t="s">
         <v>857</v>
       </c>
-      <c r="G106" s="10" t="s">
+      <c r="H106" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="H106" s="11" t="s">
+      <c r="I106" s="11" t="s">
         <v>859</v>
       </c>
-      <c r="I106" s="11" t="s">
+      <c r="J106" s="11" t="s">
         <v>860</v>
-      </c>
-      <c r="J106" s="11" t="s">
-        <v>861</v>
       </c>
       <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
@@ -9900,25 +9900,25 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="F107" s="11" t="s">
         <v>863</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="G107" s="10" t="s">
         <v>864</v>
       </c>
-      <c r="G107" s="10" t="s">
+      <c r="H107" s="10" t="s">
         <v>865</v>
       </c>
-      <c r="H107" s="10" t="s">
+      <c r="I107" s="11" t="s">
         <v>866</v>
       </c>
-      <c r="I107" s="11" t="s">
+      <c r="J107" s="11" t="s">
         <v>867</v>
-      </c>
-      <c r="J107" s="11" t="s">
-        <v>868</v>
       </c>
       <c r="K107" s="11" t="s">
         <v>167</v>
@@ -9941,25 +9941,25 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="F108" s="11" t="s">
         <v>870</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="G108" s="10" t="s">
         <v>871</v>
       </c>
-      <c r="G108" s="10" t="s">
+      <c r="H108" s="14" t="s">
         <v>872</v>
       </c>
-      <c r="H108" s="14" t="s">
+      <c r="I108" s="11" t="s">
         <v>873</v>
       </c>
-      <c r="I108" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>874</v>
-      </c>
-      <c r="J108" s="11" t="s">
-        <v>875</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>182</v>
@@ -9982,22 +9982,22 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="E109" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="F109" s="11" t="s">
         <v>877</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="G109" s="10" t="s">
         <v>878</v>
       </c>
-      <c r="G109" s="10" t="s">
+      <c r="H109" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="H109" s="11" t="s">
+      <c r="I109" s="11" t="s">
         <v>880</v>
-      </c>
-      <c r="I109" s="11" t="s">
-        <v>881</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>209</v>
@@ -10023,28 +10023,28 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="E110" s="11" t="s">
         <v>882</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="F110" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="G110" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="G110" s="10" t="s">
+      <c r="H110" s="10" t="s">
         <v>885</v>
       </c>
-      <c r="H110" s="10" t="s">
+      <c r="I110" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="I110" s="11" t="s">
+      <c r="J110" s="11" t="s">
         <v>887</v>
       </c>
-      <c r="J110" s="11" t="s">
+      <c r="K110" s="11" t="s">
         <v>888</v>
-      </c>
-      <c r="K110" s="11" t="s">
-        <v>889</v>
       </c>
       <c r="L110" s="15" t="s">
         <v>43</v>
@@ -10064,31 +10064,31 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>889</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="F111" s="11" t="s">
         <v>891</v>
       </c>
-      <c r="F111" s="11" t="s">
+      <c r="G111" s="12" t="s">
         <v>892</v>
       </c>
-      <c r="G111" s="12" t="s">
+      <c r="H111" s="14" t="s">
+        <v>851</v>
+      </c>
+      <c r="I111" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="H111" s="14" t="s">
-        <v>852</v>
-      </c>
-      <c r="I111" s="11" t="s">
+      <c r="J111" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="J111" s="11" t="s">
+      <c r="K111" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="K111" s="11" t="s">
-        <v>896</v>
-      </c>
       <c r="L111" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M111" s="15">
         <v>50</v>
@@ -10105,25 +10105,25 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>896</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="F112" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="G112" s="10" t="s">
         <v>899</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="14" t="s">
         <v>900</v>
       </c>
-      <c r="H112" s="14" t="s">
+      <c r="I112" s="11" t="s">
         <v>901</v>
       </c>
-      <c r="I112" s="11" t="s">
+      <c r="J112" s="11" t="s">
         <v>902</v>
-      </c>
-      <c r="J112" s="11" t="s">
-        <v>903</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>217</v>
@@ -10146,22 +10146,22 @@
         <v>112</v>
       </c>
       <c r="D113" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>904</v>
       </c>
-      <c r="E113" s="11" t="s">
+      <c r="F113" s="11" t="s">
         <v>905</v>
       </c>
-      <c r="F113" s="11" t="s">
+      <c r="G113" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="G113" s="13" t="s">
+      <c r="H113" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="H113" s="11" t="s">
+      <c r="I113" s="11" t="s">
         <v>908</v>
-      </c>
-      <c r="I113" s="11" t="s">
-        <v>909</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>209</v>
@@ -10187,31 +10187,31 @@
         <v>113</v>
       </c>
       <c r="D114" s="10" t="s">
+        <v>909</v>
+      </c>
+      <c r="E114" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="F114" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>912</v>
       </c>
-      <c r="G114" s="11" t="s">
+      <c r="H114" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="H114" s="11" t="s">
+      <c r="I114" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="I114" s="11" t="s">
+      <c r="J114" s="11" t="s">
         <v>915</v>
-      </c>
-      <c r="J114" s="11" t="s">
-        <v>916</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>67</v>
       </c>
       <c r="L114" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M114" s="15">
         <v>50</v>
@@ -10327,6 +10327,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C83BDCBE8D48284D85D769B4BB94FC3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25512200c29be4ab0576bf074008b9cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a41d324c-c108-411a-a0c2-0fa88bc9ce3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c4e5cc0cd8b102faac2405d31b1db89" ns2:_="">
     <xsd:import namespace="a41d324c-c108-411a-a0c2-0fa88bc9ce3f"/>
@@ -10458,22 +10473,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FB4DFF8-A81D-4740-94AE-9D4036BDAAAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10489,21 +10506,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Penetration Testing Findings Repository 1.0.xlsx
Added XSS to the Improper Input Handling finding.

It is described in the weppappsec page as included in Improper Input Handling, "While expecting UTF-8 [14] encoded characters, the application fails to sanitize and transform input supplied in the form on UTF-7 [15] leading to a Cross-site scripting attack."
</commit_message>
<xml_diff>
--- a/assets/Penetration Testing Findings Repository 1.0.xlsx
+++ b/assets/Penetration Testing Findings Repository 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/external-version/rva-reporting-engine/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubenwhitney/Documents/GitHub/rva-reporting-engine/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B57523-7E67-C147-A534-8414CBF09FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E9D7CA-4033-CB4F-BEA4-754893563423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16380" yWindow="2140" windowWidth="34820" windowHeight="19640" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
+    <workbookView xWindow="15460" yWindow="2100" windowWidth="34820" windowHeight="19640" activeTab="3" xr2:uid="{9C899BDA-8373-FC47-B9D6-CA7758CA3389}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="1" r:id="rId1"/>
@@ -2167,9 +2167,6 @@
     <t>Improper Input Handling</t>
   </si>
   <si>
-    <t>Improper input handling occurs when functions like validation, sanitization, filtering, encoding, and/or decoding of input data are not implemented correctly. This weakness is common in web applications and can make these applications vulnerable to attacks (e.g., buffer overflows, Structured Query Language [SQL] injections, and denial of service [DoS]).</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ensure the web application is performing server-side validation checks and client-side validation. Implement input sanitation and filtering mechanisms to allow acceptable input types and block unacceptable ones. </t>
   </si>
   <si>
@@ -3242,6 +3239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Windows New Technology LAN Manager (NTLM) authentication, introduced in Windows NT 3.1, validates whether a user is who they claim to be. A successor of LanMan (LM), NTLM authentication continues to use insecure methods through a hashing process of credentials. NTLM authentication also lacks effective support for smart cards and other multifactor authentication (MFA) solutions. If an attacker can obtain a username and a hash, they can conduct attacks such as Pass-the-Hash. On the client side, password hashes are stored in SYSTEM and Security Account Manager (SAM) files, readable by anyone with administrator access. On the server side, password hashes are stored in the NTDS.dit file on the domain controller and are susceptible to DCSync attacks.  </t>
+  </si>
+  <si>
+    <t>Improper input handling occurs when functions like validation, sanitization, filtering, encoding, and/or decoding of input data are not implemented correctly. This weakness is common in web applications and can make these applications vulnerable to attacks (e.g., buffer overflows, Structured Query Language [SQL] injections, denial of service [DoS], and cross-site scripting [XSS]).</t>
   </si>
 </sst>
 </file>
@@ -4294,7 +4294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDF0EF5-6DED-0A40-A55B-9157B9D1CA48}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -4518,7 +4518,7 @@
         <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="187" x14ac:dyDescent="0.2">
@@ -4547,7 +4547,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -4585,7 +4585,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -4623,7 +4623,7 @@
         <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -4662,7 +4662,7 @@
         <v>59</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>60</v>
@@ -4703,7 +4703,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>67</v>
@@ -4781,7 +4781,7 @@
         <v>78</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>79</v>
@@ -4980,7 +4980,7 @@
         <v>112</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>113</v>
@@ -5019,7 +5019,7 @@
         <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>119</v>
@@ -5479,7 +5479,7 @@
         <v>198</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>199</v>
@@ -5613,9 +5613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE6EBA3-B14F-E947-A615-39B9D02994B2}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5673,7 +5673,7 @@
         <v>36</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.2">
@@ -5854,7 +5854,7 @@
         <v>248</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>249</v>
@@ -6109,7 +6109,7 @@
         <v>292</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>293</v>
@@ -6232,7 +6232,7 @@
         <v>315</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>49</v>
@@ -6311,7 +6311,7 @@
         <v>327</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>328</v>
@@ -6903,10 +6903,10 @@
         <v>419</v>
       </c>
       <c r="E32" s="10" t="s">
+        <v>943</v>
+      </c>
+      <c r="F32" s="45" t="s">
         <v>944</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>945</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>420</v>
@@ -6944,10 +6944,10 @@
         <v>425</v>
       </c>
       <c r="E33" s="10" t="s">
+        <v>945</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>946</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>947</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>426</v>
@@ -6983,7 +6983,7 @@
         <v>428</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>429</v>
@@ -7536,26 +7536,26 @@
         <v>47</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>939</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>940</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="F48" s="11" t="s">
-        <v>942</v>
-      </c>
       <c r="G48" s="29" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="J48" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>937</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>938</v>
       </c>
       <c r="L48" s="15" t="s">
         <v>54</v>
@@ -7575,26 +7575,26 @@
         <v>48</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>928</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>931</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>942</v>
+      </c>
+      <c r="G49" s="29" t="s">
         <v>929</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>932</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>943</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>930</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="L49" s="15" t="s">
         <v>625</v>
@@ -7630,7 +7630,7 @@
         <v>520</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>480</v>
@@ -7737,7 +7737,7 @@
         <v>535</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="G53" s="43" t="s">
         <v>536</v>
@@ -7778,7 +7778,7 @@
         <v>541</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G54" s="43" t="s">
         <v>536</v>
@@ -7938,7 +7938,7 @@
         <v>557</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>558</v>
@@ -7979,7 +7979,7 @@
         <v>564</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G59" s="11" t="s">
         <v>565</v>
@@ -8020,7 +8020,7 @@
         <v>570</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>571</v>
@@ -8061,7 +8061,7 @@
         <v>577</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>578</v>
@@ -8102,7 +8102,7 @@
         <v>584</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G62" s="14" t="s">
         <v>585</v>
@@ -8143,7 +8143,7 @@
         <v>591</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G63" s="14" t="s">
         <v>592</v>
@@ -8184,7 +8184,7 @@
         <v>598</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G64" s="14" t="s">
         <v>599</v>
@@ -8223,7 +8223,7 @@
         <v>603</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G65" s="14" t="s">
         <v>604</v>
@@ -8264,7 +8264,7 @@
         <v>610</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>611</v>
@@ -8305,7 +8305,7 @@
         <v>615</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G67" s="14" t="s">
         <v>616</v>
@@ -8346,7 +8346,7 @@
         <v>620</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>621</v>
@@ -8501,22 +8501,22 @@
         <v>639</v>
       </c>
       <c r="E72" s="11" t="s">
+        <v>963</v>
+      </c>
+      <c r="F72" s="11" t="s">
         <v>640</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>641</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="H72" s="43" t="s">
+        <v>641</v>
+      </c>
+      <c r="I72" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="H72" s="43" t="s">
-        <v>642</v>
-      </c>
-      <c r="I72" s="11" t="s">
+      <c r="J72" s="11" t="s">
         <v>643</v>
-      </c>
-      <c r="J72" s="11" t="s">
-        <v>644</v>
       </c>
       <c r="K72" s="11">
         <v>16</v>
@@ -8539,25 +8539,25 @@
         <v>72</v>
       </c>
       <c r="D73" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>645</v>
       </c>
-      <c r="E73" s="11" t="s">
+      <c r="F73" s="11" t="s">
         <v>646</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>647</v>
       </c>
-      <c r="G73" s="11" t="s">
-        <v>648</v>
-      </c>
       <c r="H73" s="43" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I73" s="11" t="s">
+        <v>642</v>
+      </c>
+      <c r="J73" s="11" t="s">
         <v>643</v>
-      </c>
-      <c r="J73" s="11" t="s">
-        <v>644</v>
       </c>
       <c r="K73" s="11">
         <v>16</v>
@@ -8580,23 +8580,23 @@
         <v>73</v>
       </c>
       <c r="D74" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="E74" s="11" t="s">
         <v>649</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="F74" s="11" t="s">
         <v>650</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="G74" s="11" t="s">
         <v>651</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>652</v>
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>653</v>
-      </c>
-      <c r="J74" s="11" t="s">
-        <v>654</v>
       </c>
       <c r="K74" s="11" t="s">
         <v>266</v>
@@ -8619,28 +8619,28 @@
         <v>74</v>
       </c>
       <c r="D75" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>655</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="F75" s="10" t="s">
         <v>656</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="G75" s="14" t="s">
         <v>657</v>
       </c>
-      <c r="G75" s="14" t="s">
+      <c r="H75" s="14" t="s">
         <v>658</v>
       </c>
-      <c r="H75" s="14" t="s">
+      <c r="I75" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="I75" s="10" t="s">
+      <c r="J75" s="10" t="s">
+        <v>925</v>
+      </c>
+      <c r="K75" s="10" t="s">
         <v>660</v>
-      </c>
-      <c r="J75" s="10" t="s">
-        <v>926</v>
-      </c>
-      <c r="K75" s="10" t="s">
-        <v>661</v>
       </c>
       <c r="L75" s="15" t="s">
         <v>43</v>
@@ -8660,23 +8660,23 @@
         <v>75</v>
       </c>
       <c r="D76" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>662</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="F76" s="10" t="s">
         <v>663</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="G76" s="14" t="s">
         <v>664</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>665</v>
       </c>
       <c r="H76" s="14"/>
       <c r="I76" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="K76" s="10" t="s">
         <v>328</v>
@@ -8699,25 +8699,25 @@
         <v>76</v>
       </c>
       <c r="D77" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>667</v>
       </c>
-      <c r="E77" s="11" t="s">
+      <c r="F77" s="11" t="s">
         <v>668</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="G77" s="11" t="s">
         <v>669</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="H77" s="43" t="s">
+        <v>669</v>
+      </c>
+      <c r="I77" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="H77" s="43" t="s">
-        <v>670</v>
-      </c>
-      <c r="I77" s="11" t="s">
+      <c r="J77" s="11" t="s">
         <v>671</v>
-      </c>
-      <c r="J77" s="11" t="s">
-        <v>672</v>
       </c>
       <c r="K77" s="11" t="s">
         <v>362</v>
@@ -8740,23 +8740,23 @@
         <v>77</v>
       </c>
       <c r="D78" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>673</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="F78" s="11" t="s">
         <v>674</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>675</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="43" t="s">
+        <v>675</v>
+      </c>
+      <c r="I78" s="11" t="s">
         <v>676</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="J78" s="11" t="s">
         <v>677</v>
-      </c>
-      <c r="J78" s="11" t="s">
-        <v>678</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>73</v>
@@ -8770,7 +8770,7 @@
     </row>
     <row r="79" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B79" s="10">
         <v>20</v>
@@ -8779,25 +8779,25 @@
         <v>78</v>
       </c>
       <c r="D79" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>680</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="F79" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="H79" s="43" t="s">
+        <v>682</v>
+      </c>
+      <c r="I79" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="H79" s="43" t="s">
-        <v>683</v>
-      </c>
-      <c r="I79" s="11" t="s">
+      <c r="J79" s="11" t="s">
         <v>684</v>
-      </c>
-      <c r="J79" s="11" t="s">
-        <v>685</v>
       </c>
       <c r="K79" s="11">
         <v>16</v>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="80" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B80" s="10">
         <v>20</v>
@@ -8820,19 +8820,19 @@
         <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>686</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="F80" s="11" t="s">
         <v>687</v>
       </c>
-      <c r="F80" s="11" t="s">
+      <c r="G80" s="43" t="s">
         <v>688</v>
       </c>
-      <c r="G80" s="43" t="s">
-        <v>689</v>
-      </c>
       <c r="H80" s="43" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>172</v>
@@ -8841,7 +8841,7 @@
         <v>173</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L80" s="15" t="s">
         <v>43</v>
@@ -8852,7 +8852,7 @@
     </row>
     <row r="81" spans="1:13" ht="306" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B81" s="10">
         <v>20</v>
@@ -8861,25 +8861,25 @@
         <v>80</v>
       </c>
       <c r="D81" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="F81" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="G81" s="43" t="s">
         <v>693</v>
       </c>
-      <c r="G81" s="43" t="s">
+      <c r="H81" s="43" t="s">
         <v>694</v>
       </c>
-      <c r="H81" s="43" t="s">
+      <c r="I81" s="11" t="s">
         <v>695</v>
       </c>
-      <c r="I81" s="11" t="s">
+      <c r="J81" s="11" t="s">
         <v>696</v>
-      </c>
-      <c r="J81" s="11" t="s">
-        <v>697</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>182</v>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="82" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B82" s="10">
         <v>20</v>
@@ -8902,25 +8902,25 @@
         <v>81</v>
       </c>
       <c r="D82" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="F82" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="G82" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="H82" s="14" t="s">
         <v>701</v>
       </c>
-      <c r="H82" s="14" t="s">
+      <c r="I82" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="10" t="s">
         <v>703</v>
-      </c>
-      <c r="J82" s="10" t="s">
-        <v>704</v>
       </c>
       <c r="K82" s="15" t="s">
         <v>508</v>
@@ -8934,7 +8934,7 @@
     </row>
     <row r="83" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B83" s="10">
         <v>20</v>
@@ -8943,23 +8943,23 @@
         <v>82</v>
       </c>
       <c r="D83" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="E83" s="11" t="s">
         <v>705</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="F83" s="10" t="s">
         <v>706</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="G83" s="10" t="s">
         <v>707</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>708</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>696</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>697</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>182</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="84" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B84" s="10">
         <v>20</v>
@@ -8982,20 +8982,20 @@
         <v>83</v>
       </c>
       <c r="D84" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>709</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="F84" s="10" t="s">
         <v>710</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="G84" s="10" t="s">
         <v>711</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>712</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>515</v>
@@ -9021,25 +9021,25 @@
         <v>84</v>
       </c>
       <c r="D85" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="E85" s="46" t="s">
         <v>714</v>
       </c>
-      <c r="E85" s="46" t="s">
+      <c r="F85" s="11" t="s">
         <v>715</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="G85" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="G85" s="43" t="s">
+      <c r="H85" s="43" t="s">
+        <v>716</v>
+      </c>
+      <c r="I85" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="H85" s="43" t="s">
-        <v>717</v>
-      </c>
-      <c r="I85" s="4" t="s">
+      <c r="J85" s="4" t="s">
         <v>718</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>719</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>49</v>
@@ -9062,23 +9062,23 @@
         <v>85</v>
       </c>
       <c r="D86" s="10" t="s">
+        <v>719</v>
+      </c>
+      <c r="E86" s="46" t="s">
         <v>720</v>
       </c>
-      <c r="E86" s="46" t="s">
+      <c r="F86" s="46" t="s">
         <v>721</v>
       </c>
-      <c r="F86" s="46" t="s">
+      <c r="G86" s="10" t="s">
         <v>722</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>723</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>724</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>725</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>73</v>
@@ -9101,25 +9101,25 @@
         <v>86</v>
       </c>
       <c r="D87" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>726</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="F87" s="46" t="s">
         <v>727</v>
       </c>
-      <c r="F87" s="46" t="s">
+      <c r="G87" s="29" t="s">
         <v>728</v>
       </c>
-      <c r="G87" s="29" t="s">
+      <c r="H87" s="12" t="s">
         <v>729</v>
       </c>
-      <c r="H87" s="12" t="s">
-        <v>730</v>
-      </c>
       <c r="I87" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>724</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>725</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>73</v>
@@ -9142,28 +9142,28 @@
         <v>87</v>
       </c>
       <c r="D88" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="E88" s="46" t="s">
         <v>731</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="F88" s="46" t="s">
         <v>732</v>
       </c>
-      <c r="F88" s="46" t="s">
+      <c r="G88" s="43" t="s">
         <v>733</v>
       </c>
-      <c r="G88" s="43" t="s">
+      <c r="H88" s="43" t="s">
+        <v>733</v>
+      </c>
+      <c r="I88" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="H88" s="43" t="s">
-        <v>734</v>
-      </c>
-      <c r="I88" s="4" t="s">
+      <c r="J88" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="J88" s="4" t="s">
+      <c r="K88" s="4" t="s">
         <v>736</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>737</v>
       </c>
       <c r="L88" s="15" t="s">
         <v>43</v>
@@ -9183,25 +9183,25 @@
         <v>88</v>
       </c>
       <c r="D89" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="E89" s="46" t="s">
         <v>738</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="F89" s="11" t="s">
         <v>739</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="G89" s="29" t="s">
         <v>740</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="H89" s="12" t="s">
         <v>741</v>
       </c>
-      <c r="H89" s="12" t="s">
+      <c r="I89" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="J89" s="4" t="s">
         <v>743</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>744</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>210</v>
@@ -9224,26 +9224,26 @@
         <v>89</v>
       </c>
       <c r="D90" s="10" t="s">
+        <v>744</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>745</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>746</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="G90" s="16" t="s">
         <v>747</v>
-      </c>
-      <c r="G90" s="16" t="s">
-        <v>748</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>750</v>
-      </c>
-      <c r="K90" s="4" t="s">
-        <v>751</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>43</v>
@@ -9263,26 +9263,26 @@
         <v>90</v>
       </c>
       <c r="D91" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="E91" s="11" t="s">
         <v>752</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="F91" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="G91" s="29" t="s">
         <v>754</v>
-      </c>
-      <c r="G91" s="29" t="s">
-        <v>755</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="K91" s="4" t="s">
         <v>750</v>
-      </c>
-      <c r="K91" s="4" t="s">
-        <v>751</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>43</v>
@@ -9302,25 +9302,25 @@
         <v>91</v>
       </c>
       <c r="D92" s="10" t="s">
+        <v>755</v>
+      </c>
+      <c r="E92" s="11" t="s">
         <v>756</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="F92" s="10" t="s">
         <v>757</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="G92" s="10" t="s">
         <v>758</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="I92" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>761</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>762</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>43</v>
@@ -9340,26 +9340,26 @@
         <v>92</v>
       </c>
       <c r="D93" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="F93" s="10" t="s">
         <v>764</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="G93" s="14" t="s">
         <v>765</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>766</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>767</v>
       </c>
-      <c r="J93" s="4" t="s">
+      <c r="K93" s="4" t="s">
         <v>768</v>
-      </c>
-      <c r="K93" s="4" t="s">
-        <v>769</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>43</v>
@@ -9379,28 +9379,28 @@
         <v>93</v>
       </c>
       <c r="D94" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="E94" s="10" t="s">
         <v>770</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="10" t="s">
         <v>771</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="G94" s="12" t="s">
         <v>772</v>
       </c>
-      <c r="G94" s="12" t="s">
+      <c r="H94" s="14" t="s">
         <v>773</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="I94" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="J94" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="J94" s="4" t="s">
+      <c r="K94" s="48" t="s">
         <v>776</v>
-      </c>
-      <c r="K94" s="48" t="s">
-        <v>777</v>
       </c>
       <c r="L94" s="15" t="s">
         <v>54</v>
@@ -9420,23 +9420,23 @@
         <v>94</v>
       </c>
       <c r="D95" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>778</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="F95" s="11" t="s">
         <v>779</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="G95" s="29" t="s">
         <v>780</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>781</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>782</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>783</v>
       </c>
       <c r="K95" s="4">
         <v>3</v>
@@ -9459,26 +9459,26 @@
         <v>95</v>
       </c>
       <c r="D96" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>784</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="F96" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="G96" s="10" t="s">
         <v>786</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>787</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>788</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="K96" s="4" t="s">
         <v>789</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>790</v>
       </c>
       <c r="L96" s="15" t="s">
         <v>43</v>
@@ -9498,28 +9498,28 @@
         <v>96</v>
       </c>
       <c r="D97" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="E97" s="10" t="s">
         <v>791</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="F97" s="10" t="s">
         <v>792</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="G97" s="10" t="s">
         <v>793</v>
       </c>
-      <c r="G97" s="10" t="s">
+      <c r="H97" s="10" t="s">
         <v>794</v>
       </c>
-      <c r="H97" s="10" t="s">
+      <c r="I97" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="J97" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="K97" s="4" t="s">
         <v>797</v>
-      </c>
-      <c r="K97" s="4" t="s">
-        <v>798</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>384</v>
@@ -9539,28 +9539,28 @@
         <v>97</v>
       </c>
       <c r="D98" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>799</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="F98" s="11" t="s">
         <v>800</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="G98" s="29" t="s">
         <v>801</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="H98" s="12" t="s">
         <v>802</v>
       </c>
-      <c r="H98" s="12" t="s">
+      <c r="I98" s="4" t="s">
         <v>803</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="J98" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="K98" s="4" t="s">
         <v>805</v>
-      </c>
-      <c r="K98" s="4" t="s">
-        <v>806</v>
       </c>
       <c r="L98" s="15" t="s">
         <v>384</v>
@@ -9580,25 +9580,25 @@
         <v>98</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>806</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>807</v>
       </c>
-      <c r="E99" s="11" t="s">
+      <c r="F99" s="11" t="s">
         <v>808</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="G99" s="43" t="s">
         <v>809</v>
       </c>
-      <c r="G99" s="43" t="s">
+      <c r="H99" s="43" t="s">
+        <v>809</v>
+      </c>
+      <c r="I99" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="H99" s="43" t="s">
-        <v>810</v>
-      </c>
-      <c r="I99" s="4" t="s">
+      <c r="J99" s="4" t="s">
         <v>811</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>812</v>
       </c>
       <c r="K99" s="4">
         <v>3</v>
@@ -9621,19 +9621,19 @@
         <v>99</v>
       </c>
       <c r="D100" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="E100" s="10" t="s">
         <v>813</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="F100" s="10" t="s">
         <v>814</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="I100" s="48" t="s">
         <v>815</v>
       </c>
-      <c r="I100" s="48" t="s">
+      <c r="J100" s="48" t="s">
         <v>816</v>
-      </c>
-      <c r="J100" s="48" t="s">
-        <v>817</v>
       </c>
       <c r="K100" s="48" t="s">
         <v>100</v>
@@ -9656,28 +9656,28 @@
         <v>100</v>
       </c>
       <c r="D101" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>818</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="F101" s="11" t="s">
         <v>819</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="10" t="s">
         <v>820</v>
       </c>
-      <c r="G101" s="10" t="s">
+      <c r="H101" s="10" t="s">
         <v>821</v>
       </c>
-      <c r="H101" s="10" t="s">
+      <c r="I101" s="11" t="s">
         <v>822</v>
       </c>
-      <c r="I101" s="11" t="s">
+      <c r="J101" s="11" t="s">
+        <v>927</v>
+      </c>
+      <c r="K101" s="11" t="s">
         <v>823</v>
-      </c>
-      <c r="J101" s="11" t="s">
-        <v>928</v>
-      </c>
-      <c r="K101" s="11" t="s">
-        <v>824</v>
       </c>
       <c r="L101" s="15" t="s">
         <v>384</v>
@@ -9697,28 +9697,28 @@
         <v>101</v>
       </c>
       <c r="D102" s="10" t="s">
+        <v>824</v>
+      </c>
+      <c r="E102" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="E102" s="11" t="s">
+      <c r="F102" s="11" t="s">
         <v>826</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="G102" s="10" t="s">
         <v>827</v>
       </c>
-      <c r="G102" s="10" t="s">
+      <c r="H102" s="11" t="s">
         <v>828</v>
       </c>
-      <c r="H102" s="11" t="s">
+      <c r="I102" s="11" t="s">
         <v>829</v>
       </c>
-      <c r="I102" s="11" t="s">
+      <c r="J102" s="11" t="s">
         <v>830</v>
       </c>
-      <c r="J102" s="11" t="s">
+      <c r="K102" s="11" t="s">
         <v>831</v>
-      </c>
-      <c r="K102" s="11" t="s">
-        <v>832</v>
       </c>
       <c r="L102" s="15" t="s">
         <v>384</v>
@@ -9738,25 +9738,25 @@
         <v>102</v>
       </c>
       <c r="D103" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>833</v>
       </c>
-      <c r="E103" s="11" t="s">
+      <c r="F103" s="11" t="s">
         <v>834</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="G103" s="10" t="s">
         <v>835</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="I103" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="I103" s="11" t="s">
+      <c r="J103" s="11" t="s">
         <v>838</v>
-      </c>
-      <c r="J103" s="11" t="s">
-        <v>839</v>
       </c>
       <c r="K103" s="11" t="s">
         <v>508</v>
@@ -9779,25 +9779,25 @@
         <v>103</v>
       </c>
       <c r="D104" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="E104" s="11" t="s">
         <v>840</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="F104" s="11" t="s">
         <v>841</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="G104" s="11" t="s">
         <v>842</v>
       </c>
-      <c r="G104" s="11" t="s">
+      <c r="H104" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="H104" s="11" t="s">
+      <c r="I104" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="I104" s="11" t="s">
+      <c r="J104" s="11" t="s">
         <v>845</v>
-      </c>
-      <c r="J104" s="11" t="s">
-        <v>846</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>182</v>
@@ -9820,25 +9820,25 @@
         <v>104</v>
       </c>
       <c r="D105" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="E105" s="11" t="s">
         <v>847</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="F105" s="11" t="s">
         <v>848</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="G105" s="10" t="s">
         <v>849</v>
       </c>
-      <c r="G105" s="10" t="s">
+      <c r="H105" s="14" t="s">
         <v>850</v>
       </c>
-      <c r="H105" s="14" t="s">
+      <c r="I105" s="11" t="s">
         <v>851</v>
       </c>
-      <c r="I105" s="11" t="s">
+      <c r="J105" s="11" t="s">
         <v>852</v>
-      </c>
-      <c r="J105" s="11" t="s">
-        <v>853</v>
       </c>
       <c r="K105" s="11" t="s">
         <v>210</v>
@@ -9861,25 +9861,25 @@
         <v>105</v>
       </c>
       <c r="D106" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="F106" s="11" t="s">
         <v>855</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="G106" s="10" t="s">
         <v>856</v>
       </c>
-      <c r="G106" s="10" t="s">
+      <c r="H106" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="H106" s="11" t="s">
+      <c r="I106" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="I106" s="11" t="s">
+      <c r="J106" s="11" t="s">
         <v>859</v>
-      </c>
-      <c r="J106" s="11" t="s">
-        <v>860</v>
       </c>
       <c r="K106" s="11"/>
       <c r="L106" s="15" t="s">
@@ -9900,25 +9900,25 @@
         <v>106</v>
       </c>
       <c r="D107" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>861</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="F107" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="G107" s="10" t="s">
         <v>863</v>
       </c>
-      <c r="G107" s="10" t="s">
+      <c r="H107" s="10" t="s">
         <v>864</v>
       </c>
-      <c r="H107" s="10" t="s">
+      <c r="I107" s="11" t="s">
         <v>865</v>
       </c>
-      <c r="I107" s="11" t="s">
+      <c r="J107" s="11" t="s">
         <v>866</v>
-      </c>
-      <c r="J107" s="11" t="s">
-        <v>867</v>
       </c>
       <c r="K107" s="11" t="s">
         <v>167</v>
@@ -9941,25 +9941,25 @@
         <v>107</v>
       </c>
       <c r="D108" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>868</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="F108" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="G108" s="10" t="s">
         <v>870</v>
       </c>
-      <c r="G108" s="10" t="s">
+      <c r="H108" s="14" t="s">
         <v>871</v>
       </c>
-      <c r="H108" s="14" t="s">
+      <c r="I108" s="11" t="s">
         <v>872</v>
       </c>
-      <c r="I108" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>873</v>
-      </c>
-      <c r="J108" s="11" t="s">
-        <v>874</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>182</v>
@@ -9982,22 +9982,22 @@
         <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="E109" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="F109" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="G109" s="10" t="s">
         <v>877</v>
       </c>
-      <c r="G109" s="10" t="s">
+      <c r="H109" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="H109" s="11" t="s">
+      <c r="I109" s="11" t="s">
         <v>879</v>
-      </c>
-      <c r="I109" s="11" t="s">
-        <v>880</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>209</v>
@@ -10023,28 +10023,28 @@
         <v>109</v>
       </c>
       <c r="D110" s="10" t="s">
+        <v>880</v>
+      </c>
+      <c r="E110" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="F110" s="11" t="s">
         <v>882</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="G110" s="10" t="s">
         <v>883</v>
       </c>
-      <c r="G110" s="10" t="s">
+      <c r="H110" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="H110" s="10" t="s">
+      <c r="I110" s="11" t="s">
         <v>885</v>
       </c>
-      <c r="I110" s="11" t="s">
+      <c r="J110" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="J110" s="11" t="s">
+      <c r="K110" s="11" t="s">
         <v>887</v>
-      </c>
-      <c r="K110" s="11" t="s">
-        <v>888</v>
       </c>
       <c r="L110" s="15" t="s">
         <v>43</v>
@@ -10064,28 +10064,28 @@
         <v>110</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>888</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>889</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="F111" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="F111" s="11" t="s">
+      <c r="G111" s="12" t="s">
         <v>891</v>
       </c>
-      <c r="G111" s="12" t="s">
+      <c r="H111" s="14" t="s">
+        <v>850</v>
+      </c>
+      <c r="I111" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="H111" s="14" t="s">
-        <v>851</v>
-      </c>
-      <c r="I111" s="11" t="s">
+      <c r="J111" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="J111" s="11" t="s">
+      <c r="K111" s="11" t="s">
         <v>894</v>
-      </c>
-      <c r="K111" s="11" t="s">
-        <v>895</v>
       </c>
       <c r="L111" s="15" t="s">
         <v>384</v>
@@ -10105,25 +10105,25 @@
         <v>111</v>
       </c>
       <c r="D112" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>896</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="F112" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="G112" s="10" t="s">
         <v>898</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="14" t="s">
         <v>899</v>
       </c>
-      <c r="H112" s="14" t="s">
+      <c r="I112" s="11" t="s">
         <v>900</v>
       </c>
-      <c r="I112" s="11" t="s">
+      <c r="J112" s="11" t="s">
         <v>901</v>
-      </c>
-      <c r="J112" s="11" t="s">
-        <v>902</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>217</v>
@@ -10146,22 +10146,22 @@
         <v>112</v>
       </c>
       <c r="D113" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="E113" s="11" t="s">
+      <c r="F113" s="11" t="s">
         <v>904</v>
       </c>
-      <c r="F113" s="11" t="s">
+      <c r="G113" s="13" t="s">
         <v>905</v>
       </c>
-      <c r="G113" s="13" t="s">
+      <c r="H113" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="H113" s="11" t="s">
+      <c r="I113" s="11" t="s">
         <v>907</v>
-      </c>
-      <c r="I113" s="11" t="s">
-        <v>908</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>209</v>
@@ -10187,25 +10187,25 @@
         <v>113</v>
       </c>
       <c r="D114" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E114" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="F114" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="G114" s="11" t="s">
+      <c r="H114" s="11" t="s">
         <v>912</v>
       </c>
-      <c r="H114" s="11" t="s">
+      <c r="I114" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="I114" s="11" t="s">
+      <c r="J114" s="11" t="s">
         <v>914</v>
-      </c>
-      <c r="J114" s="11" t="s">
-        <v>915</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>67</v>
@@ -10327,18 +10327,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10474,18 +10474,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B525D9CE-2987-4221-8A14-0DB305486239}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED0DD4F-EF38-4B94-9E1F-316F1E175FBF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>